<commit_message>
final commit mv ga4 merch
</commit_message>
<xml_diff>
--- a/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
+++ b/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
@@ -1007,7 +1007,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1110,7 +1110,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/5k run</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1118,7 +1118,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1126,7 +1126,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/apparelgoogle beekeepers onesie pink</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1238,7 +1238,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt ls</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1246,7 +1246,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/google land and sea mug ls</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1254,7 +1254,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1262,7 +1262,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1270,7 +1270,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1278,7 +1278,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/notebooks journals</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1286,7 +1286,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1294,7 +1294,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1302,7 +1302,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/small goods</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1310,7 +1310,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/small goods</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1318,7 +1318,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1326,7 +1326,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>google redesign/wearables</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1334,7 +1334,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/wearables</t>
+          <t>google rmg redesign/lifestyle</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1342,7 +1342,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle</t>
+          <t>google yellowesign/apparel</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1350,7 +1350,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1358,7 +1358,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1366,7 +1366,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1374,7 +1374,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1382,7 +1382,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1390,7 +1390,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>store-policies/privacy-policy</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1398,7 +1398,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
+          <t>store-policies/return-policy</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1406,7 +1406,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
+          <t>store-policies/shipping-information</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1414,7 +1414,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
+          <t>store-policies/terms-of-use</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1422,7 +1422,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1430,7 +1430,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1438,7 +1438,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>the google merchandise store - register</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1446,18 +1446,10 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>your wishlist</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>your wishlist</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1470,7 +1462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B384"/>
+  <dimension ref="A1:B376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1573,7 +1565,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/5k run/google 5k run 2020 unisex tee</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1581,7 +1573,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google redesign/accessories/android iconic pin</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1589,7 +1581,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android iconic pin</t>
+          <t>google redesign/accessories/android large removable sticker sheet</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1597,7 +1589,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android large removable sticker sheet</t>
+          <t>google redesign/accessories/android lumberjack pin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1725,7 +1717,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork key ring</t>
+          <t>google redesign/accessories/google cork passport holder</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1733,7 +1725,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork passport holder</t>
+          <t>google redesign/accessories/google cork tablet case</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1741,7 +1733,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork tablet case</t>
+          <t>google redesign/accessories/google emoji magnet set</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1749,7 +1741,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji magnet set</t>
+          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1757,7 +1749,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
+          <t>google redesign/accessories/google felt luggage tag</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1765,7 +1757,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt luggage tag</t>
+          <t>google redesign/accessories/google inverted umbrella</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1773,7 +1765,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt strap keyring</t>
+          <t>google redesign/accessories/google keychain 19</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1781,7 +1773,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google inverted umbrella</t>
+          <t>google redesign/accessories/google lapel pin</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1789,7 +1781,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google keychain 19</t>
+          <t>google redesign/accessories/google laptop sleeve charcoal</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1797,7 +1789,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lapel pin</t>
+          <t>google redesign/accessories/google large pet collar blue green</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1805,7 +1797,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google laptop sleeve charcoal</t>
+          <t>google redesign/accessories/google lovehandle black</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1813,7 +1805,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lovehandle black</t>
+          <t>google redesign/accessories/google magnet</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1821,7 +1813,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google magnet</t>
+          <t>google redesign/accessories/google maps pin</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1829,7 +1821,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google maps pin</t>
+          <t>google redesign/accessories/google medium pet collar blue green</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1837,7 +1829,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google medium pet collar blue green</t>
+          <t>google redesign/accessories/google mouse pad navy</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1845,7 +1837,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google medium pet leash blue green</t>
+          <t>google redesign/accessories/google mural sticker sheet</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1853,7 +1845,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mouse pad navy</t>
+          <t>google redesign/accessories/google pride sticker</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1861,7 +1853,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mural sticker sheet</t>
+          <t>google redesign/accessories/google see no hear no set</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1869,7 +1861,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google nyc campus lapel pin</t>
+          <t>google redesign/accessories/google small cable organizer blue</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1877,7 +1869,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google nyc campus sticker</t>
+          <t>google redesign/accessories/google tech taco</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1885,7 +1877,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google pride sticker</t>
+          <t>google redesign/accessories/google utensil set</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1893,7 +1885,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google see no hear no set</t>
+          <t>google redesign/accessories/iamremarkable lapel pin</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1901,7 +1893,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google small cable organizer blue</t>
+          <t>google redesign/accessories/noogler android figure 2019</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1909,7 +1901,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google tech taco</t>
+          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1917,7 +1909,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google utensil set</t>
+          <t>google redesign/accessories/youtube iconic play pin</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1925,7 +1917,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google yellow yoyo</t>
+          <t>google redesign/accessories/youtube small sticker sheet</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1933,7 +1925,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>google redesign/accessories/iamremarkable lapel pin</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1941,7 +1933,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>google redesign/accessories/noogler android figure 2019</t>
+          <t>google redesign/apparel/android garden tee orange</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1949,7 +1941,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
+          <t>google redesign/apparel/android iconic beanie</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1957,7 +1949,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube iconic play pin</t>
+          <t>google redesign/apparel/android iconic crew</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1965,7 +1957,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube small sticker sheet</t>
+          <t>google redesign/apparel/android iconic hat green</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1973,7 +1965,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/apparel/android iconic hat v2 black</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1981,7 +1973,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android garden tee orange</t>
+          <t>google redesign/apparel/android iconic hat white</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1989,7 +1981,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic beanie</t>
+          <t>google redesign/apparel/android iconic sock</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1997,7 +1989,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic crew</t>
+          <t>google redesign/apparel/android pocket onesie navy</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -2005,7 +1997,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat green</t>
+          <t>google redesign/apparel/android pocket onesie white</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -2013,7 +2005,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat v2 black</t>
+          <t>google redesign/apparel/android pocket tee green</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -2021,7 +2013,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat white</t>
+          <t>google redesign/apparel/android pocket tee navy</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -2029,7 +2021,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic sock</t>
+          <t>google redesign/apparel/android pocket toddler tee navy</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -2037,7 +2029,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie navy</t>
+          <t>google redesign/apparel/android pocket toddler tee white</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2045,7 +2037,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie white</t>
+          <t>google redesign/apparel/android pocket youth tee green</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2053,7 +2045,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee green</t>
+          <t>google redesign/apparel/android pocket youth tee navy</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -2061,7 +2053,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee navy</t>
+          <t>google redesign/apparel/flamingo and friends tee blue</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -2069,7 +2061,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee navy</t>
+          <t>google redesign/apparel/google austin campus unisex tee</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -2077,7 +2069,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee white</t>
+          <t>google redesign/apparel/google austin campus zip hoodie</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2085,7 +2077,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee green</t>
+          <t>google redesign/apparel/google badge heavyweight pullover black</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2093,7 +2085,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee navy</t>
+          <t>google redesign/apparel/google black cloud zip hoodie</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -2101,7 +2093,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>google redesign/apparel/flamingo and friends tee blue</t>
+          <t>google redesign/apparel/google black tee</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -2109,7 +2101,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus unisex tee</t>
+          <t>google redesign/apparel/google cambridge campus unisex tee</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -2117,7 +2109,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus zip hoodie</t>
+          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -2125,7 +2117,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google badge heavyweight pullover black</t>
+          <t>google redesign/apparel/google campus bike eco tee navy</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -2133,7 +2125,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black cloud zip hoodie</t>
+          <t>google redesign/apparel/google chicago campus unisex tee</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -2141,7 +2133,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black tee</t>
+          <t>google redesign/apparel/google chicago campus zip hoodie</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -2149,7 +2141,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google boulder campus unisex tee</t>
+          <t>google redesign/apparel/google cotopaxi shell</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -2157,7 +2149,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus unisex tee</t>
+          <t>google redesign/apparel/google crew grey</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2165,7 +2157,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
+          <t>google redesign/apparel/google crew socks</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2173,7 +2165,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google campus bike eco tee navy</t>
+          <t>google redesign/apparel/google crewneck sweatshirt green</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -2181,7 +2173,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus zip hoodie</t>
+          <t>google redesign/apparel/google dino game tee</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -2189,7 +2181,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cotopaxi shell</t>
+          <t>google redesign/apparel/google fc longsleeve ash</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2197,7 +2189,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew grey</t>
+          <t>google redesign/apparel/google fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2205,7 +2197,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew socks</t>
+          <t>google redesign/apparel/google google blue kids sunglasses</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2213,7 +2205,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crewneck sweatshirt green</t>
+          <t>google redesign/apparel/google google crew combed cotton sock</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -2221,7 +2213,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google dino game tee</t>
+          <t>google redesign/apparel/google google crew striped athletic sock</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -2229,7 +2221,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve ash</t>
+          <t>google redesign/apparel/google google kids playful tee</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -2237,7 +2229,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google google premium sunglasses</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2245,7 +2237,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google blue kids sunglasses</t>
+          <t>google redesign/apparel/google google summer19 crew grey</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2253,7 +2245,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew combed cotton sock</t>
+          <t>google redesign/apparel/google grey tee</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -2261,7 +2253,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew striped athletic sock</t>
+          <t>google redesign/apparel/google heather green speckled tee</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -2269,7 +2261,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google kids playful tee</t>
+          <t>google redesign/apparel/google heathered pom beanie</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -2277,7 +2269,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google premium sunglasses</t>
+          <t>google redesign/apparel/google infant charcoal onesie</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -2285,7 +2277,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google summer19 crew grey</t>
+          <t>google redesign/apparel/google infant hero onesie grey</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2293,7 +2285,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google grey tee</t>
+          <t>google redesign/apparel/google infant hero tee olive</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -2301,7 +2293,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heather green speckled tee</t>
+          <t>google redesign/apparel/google kirkland campus unisex tee</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -2309,7 +2301,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heathered pom beanie</t>
+          <t>google redesign/apparel/google la campus unisex tee</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -2317,7 +2309,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant charcoal onesie</t>
+          <t>google redesign/apparel/google la campus zip hoodie</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2325,7 +2317,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero onesie grey</t>
+          <t>google redesign/apparel/google land and sea cotton cap ls</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2333,7 +2325,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero tee olive</t>
+          <t>google redesign/apparel/google land and sea unisex tee</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -2341,7 +2333,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google kirkland campus unisex tee</t>
+          <t>google redesign/apparel/google land and sea womens eco tee</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -2349,7 +2341,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus unisex tee</t>
+          <t>google redesign/apparel/google leather strap hat black</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -2357,7 +2349,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus zip hoodie</t>
+          <t>google redesign/apparel/google leather strap hat blue</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -2365,7 +2357,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea cotton cap ls</t>
+          <t>google redesign/apparel/google mens discovery lt rain shell</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -2373,7 +2365,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea unisex tee</t>
+          <t>google redesign/apparel/google mens microfleece jacket black</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -2381,7 +2373,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea womens eco tee</t>
+          <t>google redesign/apparel/google mens puff jacket black</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -2389,7 +2381,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat black</t>
+          <t>google redesign/apparel/google mens softshell moss</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -2397,7 +2389,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat blue</t>
+          <t>google redesign/apparel/google mens tech fleece grey</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -2405,7 +2397,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens discovery lt rain shell</t>
+          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -2413,7 +2405,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens microfleece jacket black</t>
+          <t>google redesign/apparel/google mountain view tee blue</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -2421,7 +2413,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens puff jacket black</t>
+          <t>google redesign/apparel/google mural socks</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -2429,7 +2421,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens softshell moss</t>
+          <t>google redesign/apparel/google navy speckled tee</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -2437,7 +2429,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece grey</t>
+          <t>google redesign/apparel/google nyc campus unisex tee</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -2445,7 +2437,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google nyc campus zip hoodie</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -2453,7 +2445,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee blue</t>
+          <t>google redesign/apparel/google pnw campus unisex tee</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -2461,7 +2453,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee red</t>
+          <t>google redesign/apparel/google pnw campus zip hoodie</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -2469,7 +2461,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mural socks</t>
+          <t>google redesign/apparel/google raincoat navy</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -2477,7 +2469,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google navy speckled tee</t>
+          <t>google redesign/apparel/google red speckled tee</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -2485,7 +2477,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus ladies tee</t>
+          <t>google redesign/apparel/google seattle campus unisex tee</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -2493,7 +2485,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus unisex tee</t>
+          <t>google redesign/apparel/google sf campus ladies tee</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -2501,7 +2493,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus zip hoodie</t>
+          <t>google redesign/apparel/google sf campus unisex tee</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -2509,7 +2501,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus unisex tee</t>
+          <t>google redesign/apparel/google sf campus zip hoodie</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -2517,7 +2509,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus zip hoodie</t>
+          <t>google redesign/apparel/google sherpa vest black</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -2525,7 +2517,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google raincoat navy</t>
+          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -2533,7 +2525,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google red speckled tee</t>
+          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
@@ -2541,7 +2533,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google seattle campus unisex tee</t>
+          <t>google redesign/apparel/google speckled beanie grey</t>
         </is>
       </c>
       <c r="B133" t="inlineStr"/>
@@ -2549,7 +2541,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus ladies tee</t>
+          <t>google redesign/apparel/google speckled beanie navy</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -2557,7 +2549,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus unisex tee</t>
+          <t>google redesign/apparel/google split seam tee olive</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
@@ -2565,7 +2557,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus zip hoodie</t>
+          <t>google redesign/apparel/google tee blue</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -2573,7 +2565,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa vest black</t>
+          <t>google redesign/apparel/google tee dark blue</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -2581,7 +2573,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
+          <t>google redesign/apparel/google tee fc black</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -2589,7 +2581,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
+          <t>google redesign/apparel/google tee mint green</t>
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
@@ -2597,7 +2589,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie grey</t>
+          <t>google redesign/apparel/google tee red</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -2605,7 +2597,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie navy</t>
+          <t>google redesign/apparel/google toddler fc tee charcoal</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -2613,7 +2605,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google split seam tee olive</t>
+          <t>google redesign/apparel/google toddler fc zip hoodie</t>
         </is>
       </c>
       <c r="B142" t="inlineStr"/>
@@ -2621,7 +2613,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee blue</t>
+          <t>google redesign/apparel/google toddler hero tee black</t>
         </is>
       </c>
       <c r="B143" t="inlineStr"/>
@@ -2629,7 +2621,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee dark blue</t>
+          <t>google redesign/apparel/google toddler hero tee olive</t>
         </is>
       </c>
       <c r="B144" t="inlineStr"/>
@@ -2637,7 +2629,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee fc black</t>
+          <t>google redesign/apparel/google toddler tee white</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -2645,7 +2637,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee mint green</t>
+          <t>google redesign/apparel/google tonal tee coral</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -2653,7 +2645,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee red</t>
+          <t>google redesign/apparel/google tonal tee spearmint</t>
         </is>
       </c>
       <c r="B147" t="inlineStr"/>
@@ -2661,7 +2653,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc tee charcoal</t>
+          <t>google redesign/apparel/google tracking hat</t>
         </is>
       </c>
       <c r="B148" t="inlineStr"/>
@@ -2669,7 +2661,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc zip hoodie</t>
+          <t>google redesign/apparel/google tudes recycled tee</t>
         </is>
       </c>
       <c r="B149" t="inlineStr"/>
@@ -2677,7 +2669,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee black</t>
+          <t>google redesign/apparel/google twill cap charcoal</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
@@ -2685,7 +2677,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee olive</t>
+          <t>google redesign/apparel/google unisex eco tee black</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -2693,7 +2685,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler tee white</t>
+          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
         </is>
       </c>
       <c r="B152" t="inlineStr"/>
@@ -2701,7 +2693,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee coral</t>
+          <t>google redesign/apparel/google unisex google pocket tee grey</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
@@ -2709,7 +2701,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee spearmint</t>
+          <t>google redesign/apparel/google unisex pride eco-tee black</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -2717,7 +2709,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tracking hat</t>
+          <t>google redesign/apparel/google womens black tee</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
@@ -2725,7 +2717,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tudes recycled tee</t>
+          <t>google redesign/apparel/google womens discovery</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -2733,7 +2725,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google twill cap charcoal</t>
+          <t>google redesign/apparel/google womens eco tee black</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
@@ -2741,7 +2733,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex eco tee black</t>
+          <t>google redesign/apparel/google womens google striped ls</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
@@ -2749,7 +2741,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
+          <t>google redesign/apparel/google womens grid zip up</t>
         </is>
       </c>
       <c r="B159" t="inlineStr"/>
@@ -2757,7 +2749,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google pocket tee grey</t>
+          <t>google redesign/apparel/google womens kirkland pullover</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
@@ -2765,7 +2757,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex pride eco-tee black</t>
+          <t>google redesign/apparel/google womens microfleece jacket black</t>
         </is>
       </c>
       <c r="B161" t="inlineStr"/>
@@ -2773,7 +2765,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens black tee</t>
+          <t>google redesign/apparel/google womens pride eco-tee black</t>
         </is>
       </c>
       <c r="B162" t="inlineStr"/>
@@ -2781,7 +2773,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens discovery</t>
+          <t>google redesign/apparel/google womens puff jacket black</t>
         </is>
       </c>
       <c r="B163" t="inlineStr"/>
@@ -2789,7 +2781,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens eco tee black</t>
+          <t>google redesign/apparel/google womens softshell moss</t>
         </is>
       </c>
       <c r="B164" t="inlineStr"/>
@@ -2797,7 +2789,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens google striped ls</t>
+          <t>google redesign/apparel/google womens tech fleece grey</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -2805,7 +2797,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens grid zip up</t>
+          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
@@ -2813,7 +2805,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens kirkland pullover</t>
+          <t>google redesign/apparel/google youth badge tee navy</t>
         </is>
       </c>
       <c r="B167" t="inlineStr"/>
@@ -2821,7 +2813,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens microfleece jacket black</t>
+          <t>google redesign/apparel/google youth badge tee olive</t>
         </is>
       </c>
       <c r="B168" t="inlineStr"/>
@@ -2829,7 +2821,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens pride eco-tee black</t>
+          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B169" t="inlineStr"/>
@@ -2837,7 +2829,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens puff jacket black</t>
+          <t>google redesign/apparel/google youth fc pullover hoodie</t>
         </is>
       </c>
       <c r="B170" t="inlineStr"/>
@@ -2845,7 +2837,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens softshell moss</t>
+          <t>google redesign/apparel/google youth fc tee charcoal</t>
         </is>
       </c>
       <c r="B171" t="inlineStr"/>
@@ -2853,7 +2845,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece grey</t>
+          <t>google redesign/apparel/google youth fc zip hoodie</t>
         </is>
       </c>
       <c r="B172" t="inlineStr"/>
@@ -2861,7 +2853,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google youth hero tee grey</t>
         </is>
       </c>
       <c r="B173" t="inlineStr"/>
@@ -2869,7 +2861,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee navy</t>
+          <t>google redesign/apparel/google youth hero tee maroon</t>
         </is>
       </c>
       <c r="B174" t="inlineStr"/>
@@ -2877,7 +2869,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee olive</t>
+          <t>google redesign/apparel/google youth jumbo print tee white</t>
         </is>
       </c>
       <c r="B175" t="inlineStr"/>
@@ -2885,7 +2877,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google zip hoodie fc</t>
         </is>
       </c>
       <c r="B176" t="inlineStr"/>
@@ -2893,7 +2885,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc pullover hoodie</t>
+          <t>google redesign/apparel/hats</t>
         </is>
       </c>
       <c r="B177" t="inlineStr"/>
@@ -2901,7 +2893,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc tee charcoal</t>
+          <t>google redesign/apparel/iamremarkable hoodie</t>
         </is>
       </c>
       <c r="B178" t="inlineStr"/>
@@ -2909,7 +2901,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc zip hoodie</t>
+          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
         </is>
       </c>
       <c r="B179" t="inlineStr"/>
@@ -2917,7 +2909,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee grey</t>
+          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
         </is>
       </c>
       <c r="B180" t="inlineStr"/>
@@ -2925,7 +2917,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee maroon</t>
+          <t>google redesign/apparel/kids</t>
         </is>
       </c>
       <c r="B181" t="inlineStr"/>
@@ -2933,7 +2925,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth jumbo print tee white</t>
+          <t>google redesign/apparel/mens</t>
         </is>
       </c>
       <c r="B182" t="inlineStr"/>
@@ -2941,7 +2933,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google zip hoodie fc</t>
+          <t>google redesign/apparel/socks</t>
         </is>
       </c>
       <c r="B183" t="inlineStr"/>
@@ -2949,7 +2941,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>google redesign/apparel/hats</t>
+          <t>google redesign/apparel/stan and friends tee green</t>
         </is>
       </c>
       <c r="B184" t="inlineStr"/>
@@ -2957,7 +2949,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable hoodie</t>
+          <t>google redesign/apparel/stan and friends toddler tee green</t>
         </is>
       </c>
       <c r="B185" t="inlineStr"/>
@@ -2965,7 +2957,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
+          <t>google redesign/apparel/womens</t>
         </is>
       </c>
       <c r="B186" t="inlineStr"/>
@@ -2973,7 +2965,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
+          <t>google redesign/apparel/youtube crew socks</t>
         </is>
       </c>
       <c r="B187" t="inlineStr"/>
@@ -2981,7 +2973,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>google redesign/apparel/kids</t>
+          <t>google redesign/apparel/youtube favorite tee white</t>
         </is>
       </c>
       <c r="B188" t="inlineStr"/>
@@ -2989,7 +2981,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>google redesign/apparel/mens</t>
+          <t>google redesign/apparel/youtube icon hoodie black</t>
         </is>
       </c>
       <c r="B189" t="inlineStr"/>
@@ -2997,7 +2989,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>google redesign/apparel/socks</t>
+          <t>google redesign/apparel/youtube icon tee charcoal</t>
         </is>
       </c>
       <c r="B190" t="inlineStr"/>
@@ -3005,7 +2997,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends tee green</t>
+          <t>google redesign/apparel/youtube icon tee grey</t>
         </is>
       </c>
       <c r="B191" t="inlineStr"/>
@@ -3013,7 +3005,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends youth tee green</t>
+          <t>google redesign/apparel/youtube leather strap hat black</t>
         </is>
       </c>
       <c r="B192" t="inlineStr"/>
@@ -3021,7 +3013,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>google redesign/apparel/womens</t>
+          <t>google redesign/apparel/youtube standards zip hoodie black</t>
         </is>
       </c>
       <c r="B193" t="inlineStr"/>
@@ -3029,7 +3021,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube crew socks</t>
+          <t>google redesign/apparel/youtube transmission journal red</t>
         </is>
       </c>
       <c r="B194" t="inlineStr"/>
@@ -3037,7 +3029,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube favorite tee white</t>
+          <t>google redesign/apparel/youtube twill cap sandwich black</t>
         </is>
       </c>
       <c r="B195" t="inlineStr"/>
@@ -3045,7 +3037,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon hoodie black</t>
+          <t>google redesign/apparelgoogle beekeepers onesie pink</t>
         </is>
       </c>
       <c r="B196" t="inlineStr"/>
@@ -3053,7 +3045,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee charcoal</t>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
         </is>
       </c>
       <c r="B197" t="inlineStr"/>
@@ -3061,7 +3053,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee grey</t>
+          <t>google redesign/bags/android iconic backpack</t>
         </is>
       </c>
       <c r="B198" t="inlineStr"/>
@@ -3069,7 +3061,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube leather strap hat black</t>
+          <t>google redesign/bags/backpacks</t>
         </is>
       </c>
       <c r="B199" t="inlineStr"/>
@@ -3077,7 +3069,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube standards zip hoodie black</t>
+          <t>google redesign/bags/essential canvas tote</t>
         </is>
       </c>
       <c r="B200" t="inlineStr"/>
@@ -3085,7 +3077,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube transmission journal red</t>
+          <t>google redesign/bags/google bike mini backpack</t>
         </is>
       </c>
       <c r="B201" t="inlineStr"/>
@@ -3093,7 +3085,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube twill cap sandwich black</t>
+          <t>google redesign/bags/google flat front bag grey</t>
         </is>
       </c>
       <c r="B202" t="inlineStr"/>
@@ -3101,7 +3093,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+          <t>google redesign/bags/google google campus bike tote navy</t>
         </is>
       </c>
       <c r="B203" t="inlineStr"/>
@@ -3109,7 +3101,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>google redesign/bags/android iconic backpack</t>
+          <t>google redesign/bags/google google confetti accessory pouch</t>
         </is>
       </c>
       <c r="B204" t="inlineStr"/>
@@ -3117,7 +3109,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>google redesign/bags/backpacks</t>
+          <t>google redesign/bags/google google striped penny pouch</t>
         </is>
       </c>
       <c r="B205" t="inlineStr"/>
@@ -3125,7 +3117,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>google redesign/bags/essential canvas tote</t>
+          <t>google redesign/bags/google hemp tote</t>
         </is>
       </c>
       <c r="B206" t="inlineStr"/>
@@ -3133,7 +3125,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>google redesign/bags/google bike mini backpack</t>
+          <t>google redesign/bags/google incognito dopp kit v2</t>
         </is>
       </c>
       <c r="B207" t="inlineStr"/>
@@ -3141,7 +3133,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>google redesign/bags/google flat front bag grey</t>
+          <t>google redesign/bags/google incognito flap pack</t>
         </is>
       </c>
       <c r="B208" t="inlineStr"/>
@@ -3149,7 +3141,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google campus bike tote navy</t>
+          <t>google redesign/bags/google incognito laptop organizer v2</t>
         </is>
       </c>
       <c r="B209" t="inlineStr"/>
@@ -3157,7 +3149,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google confetti accessory pouch</t>
+          <t>google redesign/bags/google incognito messenger bag</t>
         </is>
       </c>
       <c r="B210" t="inlineStr"/>
@@ -3165,7 +3157,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google striped penny pouch</t>
+          <t>google redesign/bags/google incognito techpack v2</t>
         </is>
       </c>
       <c r="B211" t="inlineStr"/>
@@ -3173,7 +3165,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>google redesign/bags/google hemp tote</t>
+          <t>google redesign/bags/google incognito zippack v2</t>
         </is>
       </c>
       <c r="B212" t="inlineStr"/>
@@ -3181,7 +3173,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito dopp kit v2</t>
+          <t>google redesign/bags/google large tote white</t>
         </is>
       </c>
       <c r="B213" t="inlineStr"/>
@@ -3189,7 +3181,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito flap pack</t>
+          <t>google redesign/bags/google mesh bag blue</t>
         </is>
       </c>
       <c r="B214" t="inlineStr"/>
@@ -3197,7 +3189,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito laptop organizer v2</t>
+          <t>google redesign/bags/google mural tote</t>
         </is>
       </c>
       <c r="B215" t="inlineStr"/>
@@ -3205,7 +3197,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito messenger bag</t>
+          <t>google redesign/bags/google packable bag black</t>
         </is>
       </c>
       <c r="B216" t="inlineStr"/>
@@ -3213,7 +3205,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito techpack v2</t>
+          <t>google redesign/bags/google seaport tote</t>
         </is>
       </c>
       <c r="B217" t="inlineStr"/>
@@ -3221,7 +3213,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito zippack v2</t>
+          <t>google redesign/bags/google totepak</t>
         </is>
       </c>
       <c r="B218" t="inlineStr"/>
@@ -3229,7 +3221,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>google redesign/bags/google large tote white</t>
+          <t>google redesign/bags/google utility backpack</t>
         </is>
       </c>
       <c r="B219" t="inlineStr"/>
@@ -3237,7 +3229,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>google redesign/bags/google large white gift bag 5pk</t>
+          <t>google redesign/bags/google utility bag grey</t>
         </is>
       </c>
       <c r="B220" t="inlineStr"/>
@@ -3245,7 +3237,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mesh bag blue</t>
+          <t>google redesign/bags/iamremarkable tote</t>
         </is>
       </c>
       <c r="B221" t="inlineStr"/>
@@ -3253,7 +3245,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mural tote</t>
+          <t>google redesign/bags/more bags</t>
         </is>
       </c>
       <c r="B222" t="inlineStr"/>
@@ -3261,7 +3253,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>google redesign/bags/google packable bag black</t>
+          <t>google redesign/bags/shopping and totes</t>
         </is>
       </c>
       <c r="B223" t="inlineStr"/>
@@ -3269,7 +3261,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>google redesign/bags/google seaport tote</t>
+          <t>google redesign/bags/supernatural paper backpack</t>
         </is>
       </c>
       <c r="B224" t="inlineStr"/>
@@ -3277,7 +3269,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>google redesign/bags/google sf campus tote</t>
+          <t>google redesign/bags/supernatural paper lunch sack</t>
         </is>
       </c>
       <c r="B225" t="inlineStr"/>
@@ -3285,7 +3277,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>google redesign/bags/google totepak</t>
+          <t>google redesign/bags/supernatural paper tote</t>
         </is>
       </c>
       <c r="B226" t="inlineStr"/>
@@ -3293,7 +3285,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility backpack</t>
+          <t>google redesign/blm unisex pullover hoodie</t>
         </is>
       </c>
       <c r="B227" t="inlineStr"/>
@@ -3301,7 +3293,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility bag grey</t>
+          <t>google redesign/campus collection</t>
         </is>
       </c>
       <c r="B228" t="inlineStr"/>
@@ -3309,7 +3301,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>google redesign/bags/more bags</t>
+          <t>google redesign/campus collection/google mountain view campus mug</t>
         </is>
       </c>
       <c r="B229" t="inlineStr"/>
@@ -3317,7 +3309,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>google redesign/bags/shopping and totes</t>
+          <t>google redesign/campus collection/google mountain view campus sticker</t>
         </is>
       </c>
       <c r="B230" t="inlineStr"/>
@@ -3325,7 +3317,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper backpack</t>
+          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
         </is>
       </c>
       <c r="B231" t="inlineStr"/>
@@ -3333,7 +3325,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper lunch sack</t>
+          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
         </is>
       </c>
       <c r="B232" t="inlineStr"/>
@@ -3341,7 +3333,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper tote</t>
+          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
         </is>
       </c>
       <c r="B233" t="inlineStr"/>
@@ -3349,7 +3341,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
+          <t>google redesign/campus collection/google sunnyvale campus ladies tee</t>
         </is>
       </c>
       <c r="B234" t="inlineStr"/>
@@ -3357,7 +3349,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
+          <t>google redesign/campus collection/google sunnyvale campus mug</t>
         </is>
       </c>
       <c r="B235" t="inlineStr"/>
@@ -3365,7 +3357,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus mug</t>
+          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
         </is>
       </c>
       <c r="B236" t="inlineStr"/>
@@ -3373,7 +3365,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus sticker</t>
+          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
         </is>
       </c>
       <c r="B237" t="inlineStr"/>
@@ -3381,7 +3373,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
+          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
         </is>
       </c>
       <c r="B238" t="inlineStr"/>
@@ -3389,7 +3381,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
+          <t>google redesign/clearance</t>
         </is>
       </c>
       <c r="B239" t="inlineStr"/>
@@ -3397,7 +3389,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
+          <t>google redesign/drinkware/android buoy bottle</t>
         </is>
       </c>
       <c r="B240" t="inlineStr"/>
@@ -3405,7 +3397,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus ladies tee</t>
+          <t>google redesign/drinkware/android iconic mug gray</t>
         </is>
       </c>
       <c r="B241" t="inlineStr"/>
@@ -3413,7 +3405,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus mug</t>
+          <t>google redesign/drinkware/campus corkbase mug blue</t>
         </is>
       </c>
       <c r="B242" t="inlineStr"/>
@@ -3421,7 +3413,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
+          <t>google redesign/drinkware/google 16oz tumbler blue</t>
         </is>
       </c>
       <c r="B243" t="inlineStr"/>
@@ -3429,7 +3421,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
+          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
         </is>
       </c>
       <c r="B244" t="inlineStr"/>
@@ -3437,7 +3429,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
+          <t>google redesign/drinkware/google 24oz ring bottle red</t>
         </is>
       </c>
       <c r="B245" t="inlineStr"/>
@@ -3445,7 +3437,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android buoy bottle</t>
+          <t>google redesign/drinkware/google bike bottle</t>
         </is>
       </c>
       <c r="B246" t="inlineStr"/>
@@ -3453,7 +3445,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic glass bottle green</t>
+          <t>google redesign/drinkware/google cambridge campus bottle</t>
         </is>
       </c>
       <c r="B247" t="inlineStr"/>
@@ -3461,7 +3453,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic mug gray</t>
+          <t>google redesign/drinkware/google cambridge campus mug</t>
         </is>
       </c>
       <c r="B248" t="inlineStr"/>
@@ -3469,7 +3461,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/campus corkbase mug blue</t>
+          <t>google redesign/drinkware/google camp mug ivory</t>
         </is>
       </c>
       <c r="B249" t="inlineStr"/>
@@ -3477,7 +3469,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 16oz tumbler blue</t>
+          <t>google redesign/drinkware/google canteen bottle black</t>
         </is>
       </c>
       <c r="B250" t="inlineStr"/>
@@ -3485,7 +3477,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
+          <t>google redesign/drinkware/google chicago campus mug</t>
         </is>
       </c>
       <c r="B251" t="inlineStr"/>
@@ -3493,7 +3485,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle red</t>
+          <t>google redesign/drinkware/google cork base tumbler</t>
         </is>
       </c>
       <c r="B252" t="inlineStr"/>
@@ -3501,7 +3493,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google austin campus mug</t>
+          <t>google redesign/drinkware/google cup cap tumbler grey</t>
         </is>
       </c>
       <c r="B253" t="inlineStr"/>
@@ -3509,7 +3501,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google bike bottle</t>
+          <t>google redesign/drinkware/google glass bottle</t>
         </is>
       </c>
       <c r="B254" t="inlineStr"/>
@@ -3517,7 +3509,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus bottle</t>
+          <t>google redesign/drinkware/google keepcup</t>
         </is>
       </c>
       <c r="B255" t="inlineStr"/>
@@ -3525,7 +3517,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus mug</t>
+          <t>google redesign/drinkware/google kirkland campus mug</t>
         </is>
       </c>
       <c r="B256" t="inlineStr"/>
@@ -3533,7 +3525,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google camp mug ivory</t>
+          <t>google redesign/drinkware/google la campus mug</t>
         </is>
       </c>
       <c r="B257" t="inlineStr"/>
@@ -3541,7 +3533,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google canteen bottle black</t>
+          <t>google redesign/drinkware/google mural bottle</t>
         </is>
       </c>
       <c r="B258" t="inlineStr"/>
@@ -3549,7 +3541,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google chicago campus mug</t>
+          <t>google redesign/drinkware/google mural mug</t>
         </is>
       </c>
       <c r="B259" t="inlineStr"/>
@@ -3557,7 +3549,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cork base tumbler</t>
+          <t>google redesign/drinkware/google nyc campus bottle</t>
         </is>
       </c>
       <c r="B260" t="inlineStr"/>
@@ -3565,7 +3557,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cup cap tumbler grey</t>
+          <t>google redesign/drinkware/google nyc campus mug</t>
         </is>
       </c>
       <c r="B261" t="inlineStr"/>
@@ -3573,7 +3565,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google glass bottle</t>
+          <t>google redesign/drinkware/google perk thermal cup</t>
         </is>
       </c>
       <c r="B262" t="inlineStr"/>
@@ -3581,7 +3573,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google keepcup</t>
+          <t>google redesign/drinkware/google pnw campus mug</t>
         </is>
       </c>
       <c r="B263" t="inlineStr"/>
@@ -3589,7 +3581,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google la campus mug</t>
+          <t>google redesign/drinkware/google seattle campus mug</t>
         </is>
       </c>
       <c r="B264" t="inlineStr"/>
@@ -3597,7 +3589,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural bottle</t>
+          <t>google redesign/drinkware/google sf campus bottle</t>
         </is>
       </c>
       <c r="B265" t="inlineStr"/>
@@ -3605,7 +3597,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural mug</t>
+          <t>google redesign/drinkware/google sf campus mug</t>
         </is>
       </c>
       <c r="B266" t="inlineStr"/>
@@ -3613,7 +3605,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus bottle</t>
+          <t>google redesign/drinkware/google super g tumbler blue lid</t>
         </is>
       </c>
       <c r="B267" t="inlineStr"/>
@@ -3621,7 +3613,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus mug</t>
+          <t>google redesign/drinkware/google super g tumbler red lid</t>
         </is>
       </c>
       <c r="B268" t="inlineStr"/>
@@ -3629,7 +3621,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google perk thermal cup</t>
+          <t>google redesign/drinkware/google thermal tumbler navy</t>
         </is>
       </c>
       <c r="B269" t="inlineStr"/>
@@ -3637,7 +3629,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google seattle campus mug</t>
+          <t>google redesign/drinkware/google woodtop bottle black</t>
         </is>
       </c>
       <c r="B270" t="inlineStr"/>
@@ -3645,7 +3637,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus bottle</t>
+          <t>google redesign/drinkware/iamremarkable water bottle</t>
         </is>
       </c>
       <c r="B271" t="inlineStr"/>
@@ -3653,7 +3645,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus mug</t>
+          <t>google redesign/drinkware/mugs tumblers</t>
         </is>
       </c>
       <c r="B272" t="inlineStr"/>
@@ -3661,7 +3653,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler blue lid</t>
+          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
         </is>
       </c>
       <c r="B273" t="inlineStr"/>
@@ -3669,7 +3661,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler red lid</t>
+          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
         </is>
       </c>
       <c r="B274" t="inlineStr"/>
@@ -3677,7 +3669,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google thermal tumbler navy</t>
+          <t>google redesign/drinkware/water bottles</t>
         </is>
       </c>
       <c r="B275" t="inlineStr"/>
@@ -3685,7 +3677,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google woodtop bottle black</t>
+          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
         </is>
       </c>
       <c r="B276" t="inlineStr"/>
@@ -3693,7 +3685,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/iamremarkable water bottle</t>
+          <t>google redesign/drinkware/youtube play mug</t>
         </is>
       </c>
       <c r="B277" t="inlineStr"/>
@@ -3701,7 +3693,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/mugs tumblers</t>
+          <t>google redesign/eco friendly</t>
         </is>
       </c>
       <c r="B278" t="inlineStr"/>
@@ -3709,7 +3701,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
+          <t>google redesign/electronics</t>
         </is>
       </c>
       <c r="B279" t="inlineStr"/>
@@ -3717,7 +3709,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
+          <t>google redesign/electronics/accessories</t>
         </is>
       </c>
       <c r="B280" t="inlineStr"/>
@@ -3725,7 +3717,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/water bottles</t>
+          <t>google redesign/electronics/audio</t>
         </is>
       </c>
       <c r="B281" t="inlineStr"/>
@@ -3733,7 +3725,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
+          <t>google redesign/gift cards</t>
         </is>
       </c>
       <c r="B282" t="inlineStr"/>
@@ -3741,7 +3733,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube play mug</t>
+          <t>google redesign/google blue stojo cup</t>
         </is>
       </c>
       <c r="B283" t="inlineStr"/>
@@ -3749,7 +3741,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
+          <t>google redesign/google chrome dino light up water bottle</t>
         </is>
       </c>
       <c r="B284" t="inlineStr"/>
@@ -3757,7 +3749,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
+          <t>google redesign/google crew sweater navy</t>
         </is>
       </c>
       <c r="B285" t="inlineStr"/>
@@ -3765,7 +3757,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>google redesign/electronics/accessories</t>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
         </is>
       </c>
       <c r="B286" t="inlineStr"/>
@@ -3773,7 +3765,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>google redesign/electronics/audio</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B287" t="inlineStr"/>
@@ -3781,7 +3773,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
+          <t>google redesign/google land and sea mug ls</t>
         </is>
       </c>
       <c r="B288" t="inlineStr"/>
@@ -3789,7 +3781,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B289" t="inlineStr"/>
@@ -3797,7 +3789,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B290" t="inlineStr"/>
@@ -3805,7 +3797,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
+          <t>google redesign/lifestyle/bags</t>
         </is>
       </c>
       <c r="B291" t="inlineStr"/>
@@ -3813,7 +3805,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
+          <t>google redesign/lifestyle/drinkware</t>
         </is>
       </c>
       <c r="B292" t="inlineStr"/>
@@ -3821,7 +3813,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt ls</t>
+          <t>google redesign/lifestyle/fun</t>
         </is>
       </c>
       <c r="B293" t="inlineStr"/>
@@ -3829,7 +3821,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/lifestyle/google aluminum bottle red</t>
         </is>
       </c>
       <c r="B294" t="inlineStr"/>
@@ -3837,7 +3829,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/lifestyle/google bear baby blanket beige</t>
         </is>
       </c>
       <c r="B295" t="inlineStr"/>
@@ -3845,7 +3837,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/lifestyle/google camp mug gray</t>
         </is>
       </c>
       <c r="B296" t="inlineStr"/>
@@ -3853,7 +3845,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/lifestyle/google knit blanket</t>
         </is>
       </c>
       <c r="B297" t="inlineStr"/>
@@ -3861,7 +3853,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/bags</t>
+          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
         </is>
       </c>
       <c r="B298" t="inlineStr"/>
@@ -3869,7 +3861,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/drinkware</t>
+          <t>google redesign/lifestyle/google land and sea tote bag</t>
         </is>
       </c>
       <c r="B299" t="inlineStr"/>
@@ -3877,7 +3869,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/fun</t>
+          <t>google redesign/lifestyle/google-frisbee</t>
         </is>
       </c>
       <c r="B300" t="inlineStr"/>
@@ -3885,7 +3877,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google aluminum bottle red</t>
+          <t>google redesign/lifestyle/small goods</t>
         </is>
       </c>
       <c r="B301" t="inlineStr"/>
@@ -3893,7 +3885,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google bear baby blanket beige</t>
+          <t>google redesign/lifestyle/white google shoreline bottle</t>
         </is>
       </c>
       <c r="B302" t="inlineStr"/>
@@ -3901,7 +3893,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google camp mug gray</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B303" t="inlineStr"/>
@@ -3909,7 +3901,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google knit blanket</t>
+          <t>google redesign/notebooks journals/google large standard journal grey</t>
         </is>
       </c>
       <c r="B304" t="inlineStr"/>
@@ -3917,7 +3909,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B305" t="inlineStr"/>
@@ -3925,7 +3917,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea tote bag</t>
+          <t>google redesign/office/android iconic notebook</t>
         </is>
       </c>
       <c r="B306" t="inlineStr"/>
@@ -3933,7 +3925,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google-frisbee</t>
+          <t>google redesign/office/android large trace journal black</t>
         </is>
       </c>
       <c r="B307" t="inlineStr"/>
@@ -3941,7 +3933,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/small goods</t>
+          <t>google redesign/office/android small trace journal bl</t>
         </is>
       </c>
       <c r="B308" t="inlineStr"/>
@@ -3949,7 +3941,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/white google shoreline bottle</t>
+          <t>google redesign/office/google appeel journal red</t>
         </is>
       </c>
       <c r="B309" t="inlineStr"/>
@@ -3957,7 +3949,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/office/google black cork journal</t>
         </is>
       </c>
       <c r="B310" t="inlineStr"/>
@@ -3965,7 +3957,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals/google large standard journal grey</t>
+          <t>google redesign/office/google clear pen 4pack</t>
         </is>
       </c>
       <c r="B311" t="inlineStr"/>
@@ -3973,7 +3965,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/office/google cork journal</t>
         </is>
       </c>
       <c r="B312" t="inlineStr"/>
@@ -3981,7 +3973,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>google redesign/office/android iconic notebook</t>
+          <t>google redesign/office/google cork pencil pouch</t>
         </is>
       </c>
       <c r="B313" t="inlineStr"/>
@@ -3989,7 +3981,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>google redesign/office/android large trace journal black</t>
+          <t>google redesign/office/google felt refillable journal</t>
         </is>
       </c>
       <c r="B314" t="inlineStr"/>
@@ -3997,7 +3989,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>google redesign/office/android small trace journal bl</t>
+          <t>google redesign/office/google google campus bike grid task pad</t>
         </is>
       </c>
       <c r="B315" t="inlineStr"/>
@@ -4005,7 +3997,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>google redesign/office/google appeel journal red</t>
+          <t>google redesign/office/google google color block notebook</t>
         </is>
       </c>
       <c r="B316" t="inlineStr"/>
@@ -4013,7 +4005,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>google redesign/office/google black cork journal</t>
+          <t>google redesign/office/google google confetti pen white</t>
         </is>
       </c>
       <c r="B317" t="inlineStr"/>
@@ -4021,7 +4013,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>google redesign/office/google clear pen 4pack</t>
+          <t>google redesign/office/google google confetti slim task pad</t>
         </is>
       </c>
       <c r="B318" t="inlineStr"/>
@@ -4029,7 +4021,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork journal</t>
+          <t>google redesign/office/google google confetti task pad</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
@@ -4037,7 +4029,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork pencil pouch</t>
+          <t>google redesign/office/google light up pen blue</t>
         </is>
       </c>
       <c r="B320" t="inlineStr"/>
@@ -4045,7 +4037,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>google redesign/office/google felt refillable journal</t>
+          <t>google redesign/office/google light up pen green</t>
         </is>
       </c>
       <c r="B321" t="inlineStr"/>
@@ -4053,7 +4045,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>google redesign/office/google google campus bike grid task pad</t>
+          <t>google redesign/office/google light up pen red</t>
         </is>
       </c>
       <c r="B322" t="inlineStr"/>
@@ -4061,7 +4053,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>google redesign/office/google google color block notebook</t>
+          <t>google redesign/office/google mural notebook</t>
         </is>
       </c>
       <c r="B323" t="inlineStr"/>
@@ -4069,7 +4061,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti pen white</t>
+          <t>google redesign/office/google mural sticky note pad</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
@@ -4077,7 +4069,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti slim task pad</t>
+          <t>google redesign/office/google pen citron</t>
         </is>
       </c>
       <c r="B325" t="inlineStr"/>
@@ -4085,7 +4077,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti task pad</t>
+          <t>google redesign/office/google pen grey</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
@@ -4093,7 +4085,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen blue</t>
+          <t>google redesign/office/google pen red</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
@@ -4101,7 +4093,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen green</t>
+          <t>google redesign/office/google pen white</t>
         </is>
       </c>
       <c r="B328" t="inlineStr"/>
@@ -4109,7 +4101,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen red</t>
+          <t>google redesign/office/google phone stand bamboo</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
@@ -4117,7 +4109,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural notebook</t>
+          <t>google redesign/office/google recycled notebook set natural</t>
         </is>
       </c>
       <c r="B330" t="inlineStr"/>
@@ -4125,7 +4117,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural sticky note pad</t>
+          <t>google redesign/office/google recycled pen black</t>
         </is>
       </c>
       <c r="B331" t="inlineStr"/>
@@ -4133,7 +4125,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grass green</t>
+          <t>google redesign/office/google recycled pen green</t>
         </is>
       </c>
       <c r="B332" t="inlineStr"/>
@@ -4141,7 +4133,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grey</t>
+          <t>google redesign/office/google recycled writing set</t>
         </is>
       </c>
       <c r="B333" t="inlineStr"/>
@@ -4149,7 +4141,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen neon coral</t>
+          <t>google redesign/office/google small standard journal navy</t>
         </is>
       </c>
       <c r="B334" t="inlineStr"/>
@@ -4157,7 +4149,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen red</t>
+          <t>google redesign/office/google soft modal scarf</t>
         </is>
       </c>
       <c r="B335" t="inlineStr"/>
@@ -4165,7 +4157,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen white</t>
+          <t>google redesign/office/google sustainable pencil pouch</t>
         </is>
       </c>
       <c r="B336" t="inlineStr"/>
@@ -4173,7 +4165,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>google redesign/office/google phone stand bamboo</t>
+          <t>google redesign/office/iamremarkable journal</t>
         </is>
       </c>
       <c r="B337" t="inlineStr"/>
@@ -4181,7 +4173,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled notebook set natural</t>
+          <t>google redesign/office/iamremarkable pen</t>
         </is>
       </c>
       <c r="B338" t="inlineStr"/>
@@ -4189,7 +4181,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen black</t>
+          <t>google redesign/office/notebooks journals</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
@@ -4197,7 +4189,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen green</t>
+          <t>google redesign/office/stickers</t>
         </is>
       </c>
       <c r="B340" t="inlineStr"/>
@@ -4205,7 +4197,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled writing set</t>
+          <t>google redesign/office/writing</t>
         </is>
       </c>
       <c r="B341" t="inlineStr"/>
@@ -4213,7 +4205,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>google redesign/office/google small standard journal navy</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B342" t="inlineStr"/>
@@ -4221,7 +4213,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>google redesign/office/google soft modal scarf</t>
+          <t>google redesign/shop by brand/android</t>
         </is>
       </c>
       <c r="B343" t="inlineStr"/>
@@ -4229,7 +4221,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>google redesign/office/google sustainable pencil pouch</t>
+          <t>google redesign/shop by brand/google</t>
         </is>
       </c>
       <c r="B344" t="inlineStr"/>
@@ -4237,7 +4229,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable journal</t>
+          <t>google redesign/shop by brand/google cloud</t>
         </is>
       </c>
       <c r="B345" t="inlineStr"/>
@@ -4245,7 +4237,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable pen</t>
+          <t>google redesign/shop by brand/i am remarkable</t>
         </is>
       </c>
       <c r="B346" t="inlineStr"/>
@@ -4253,7 +4245,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>google redesign/office/notebooks journals</t>
+          <t>google redesign/shop by brand/youtube</t>
         </is>
       </c>
       <c r="B347" t="inlineStr"/>
@@ -4261,7 +4253,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>google redesign/office/stickers</t>
+          <t>google redesign/small goods/daddy works at google book</t>
         </is>
       </c>
       <c r="B348" t="inlineStr"/>
@@ -4269,7 +4261,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>google redesign/office/writing</t>
+          <t>google redesign/small goods/mommy works at google book</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
@@ -4277,7 +4269,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B350" t="inlineStr"/>
@@ -4285,7 +4277,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/android</t>
+          <t>google redesign/stationery/android jotter task pad</t>
         </is>
       </c>
       <c r="B351" t="inlineStr"/>
@@ -4293,7 +4285,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google</t>
+          <t>google redesign/stationery/google 4in decal</t>
         </is>
       </c>
       <c r="B352" t="inlineStr"/>
@@ -4301,7 +4293,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google cloud</t>
+          <t>google redesign/stationery/google cloud pen</t>
         </is>
       </c>
       <c r="B353" t="inlineStr"/>
@@ -4309,7 +4301,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/i am remarkable</t>
+          <t>google redesign/stationery/google jotter task pad</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
@@ -4317,7 +4309,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/youtube</t>
+          <t>google redesign/stationery/google land and sea journal set</t>
         </is>
       </c>
       <c r="B355" t="inlineStr"/>
@@ -4325,7 +4317,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>google redesign/small goods/daddy works at google book</t>
+          <t>google redesign/stationery/notebooks</t>
         </is>
       </c>
       <c r="B356" t="inlineStr"/>
@@ -4333,7 +4325,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>google redesign/small goods/mommy works at google book</t>
+          <t>google redesign/stationery/stickers</t>
         </is>
       </c>
       <c r="B357" t="inlineStr"/>
@@ -4341,7 +4333,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/stationery/writing</t>
         </is>
       </c>
       <c r="B358" t="inlineStr"/>
@@ -4349,7 +4341,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>google redesign/stationery/android jotter task pad</t>
+          <t>google redesign/stationery/youtube jotter task pad</t>
         </is>
       </c>
       <c r="B359" t="inlineStr"/>
@@ -4357,7 +4349,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google 4in decal</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B360" t="inlineStr"/>
@@ -4365,7 +4357,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google cloud pen</t>
+          <t>google redesign/wearables/men s t-shirts</t>
         </is>
       </c>
       <c r="B361" t="inlineStr"/>
@@ -4373,7 +4365,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google jotter task pad</t>
+          <t>google rmg redesign/lifestyle/mural food container</t>
         </is>
       </c>
       <c r="B362" t="inlineStr"/>
@@ -4381,7 +4373,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google land and sea journal set</t>
+          <t>google yellowesign/apparel/google tee yellow</t>
         </is>
       </c>
       <c r="B363" t="inlineStr"/>
@@ -4389,7 +4381,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>google redesign/stationery/notebooks</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B364" t="inlineStr"/>
@@ -4397,7 +4389,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>google redesign/stationery/stickers</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B365" t="inlineStr"/>
@@ -4405,7 +4397,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>google redesign/stationery/writing</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B366" t="inlineStr"/>
@@ -4413,7 +4405,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>google redesign/stationery/youtube jotter task pad</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B367" t="inlineStr"/>
@@ -4421,7 +4413,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B368" t="inlineStr"/>
@@ -4429,7 +4421,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>google redesign/wearables/men s t-shirts</t>
+          <t>store-policies/privacy-policy</t>
         </is>
       </c>
       <c r="B369" t="inlineStr"/>
@@ -4437,7 +4429,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle/mural food container</t>
+          <t>store-policies/return-policy</t>
         </is>
       </c>
       <c r="B370" t="inlineStr"/>
@@ -4445,7 +4437,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel/google tee yellow</t>
+          <t>store-policies/shipping-information</t>
         </is>
       </c>
       <c r="B371" t="inlineStr"/>
@@ -4453,7 +4445,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>store-policies/terms-of-use</t>
         </is>
       </c>
       <c r="B372" t="inlineStr"/>
@@ -4461,7 +4453,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B373" t="inlineStr"/>
@@ -4469,7 +4461,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B374" t="inlineStr"/>
@@ -4477,7 +4469,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>the google merchandise store - register</t>
         </is>
       </c>
       <c r="B375" t="inlineStr"/>
@@ -4485,74 +4477,10 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>your wishlist</t>
         </is>
       </c>
       <c r="B376" t="inlineStr"/>
-    </row>
-    <row r="377">
-      <c r="A377" t="inlineStr">
-        <is>
-          <t>store-policies/privacy-policy</t>
-        </is>
-      </c>
-      <c r="B377" t="inlineStr"/>
-    </row>
-    <row r="378">
-      <c r="A378" t="inlineStr">
-        <is>
-          <t>store-policies/return-policy</t>
-        </is>
-      </c>
-      <c r="B378" t="inlineStr"/>
-    </row>
-    <row r="379">
-      <c r="A379" t="inlineStr">
-        <is>
-          <t>store-policies/shipping-information</t>
-        </is>
-      </c>
-      <c r="B379" t="inlineStr"/>
-    </row>
-    <row r="380">
-      <c r="A380" t="inlineStr">
-        <is>
-          <t>store-policies/terms-of-use</t>
-        </is>
-      </c>
-      <c r="B380" t="inlineStr"/>
-    </row>
-    <row r="381">
-      <c r="A381" t="inlineStr">
-        <is>
-          <t>the google merchandise store - log in</t>
-        </is>
-      </c>
-      <c r="B381" t="inlineStr"/>
-    </row>
-    <row r="382">
-      <c r="A382" t="inlineStr">
-        <is>
-          <t>the google merchandise store - my account</t>
-        </is>
-      </c>
-      <c r="B382" t="inlineStr"/>
-    </row>
-    <row r="383">
-      <c r="A383" t="inlineStr">
-        <is>
-          <t>the google merchandise store - register</t>
-        </is>
-      </c>
-      <c r="B383" t="inlineStr"/>
-    </row>
-    <row r="384">
-      <c r="A384" t="inlineStr">
-        <is>
-          <t>your wishlist</t>
-        </is>
-      </c>
-      <c r="B384" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
ga4 merch with mv, outliers, scaling, balancing start
</commit_message>
<xml_diff>
--- a/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
+++ b/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
@@ -808,7 +808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -871,7 +871,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>google greenesign</t>
+          <t>clearance</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -879,7 +879,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
+          <t>google greenesign</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -887,7 +887,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
+          <t>google merchandise store - forgot password</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -895,7 +895,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google online store</t>
+          <t>google merchandise store - reset password</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -903,7 +903,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google redesign</t>
+          <t>google online store</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -911,7 +911,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google rmg redesign</t>
+          <t>google redesign</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -919,7 +919,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google yellowesign</t>
+          <t>google rmg redesign</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -927,7 +927,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>google yellowesign</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -935,7 +935,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -943,7 +943,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -951,7 +951,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -959,7 +959,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>store-policies</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -967,7 +967,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>store-policies</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -975,7 +975,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -983,7 +983,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -991,10 +991,18 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>the google merchandise store - register</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>your wishlist</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1007,7 +1015,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1078,7 +1086,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google greenesign/apparel</t>
+          <t>clearance/clearance-accessories</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -1086,7 +1094,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
+          <t>google greenesign/apparel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -1094,7 +1102,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
+          <t>google merchandise store - forgot password</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -1102,7 +1110,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google online store</t>
+          <t>google merchandise store - reset password</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1110,7 +1118,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google online store</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1118,7 +1126,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1126,7 +1134,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers onesie pink</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1238,7 +1246,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/google land and sea french terry sweatshirt ls</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1246,7 +1254,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1254,7 +1262,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/google land and sea mug ls</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1262,7 +1270,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1270,7 +1278,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1278,7 +1286,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1286,7 +1294,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/notebooks journals</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1294,7 +1302,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1302,7 +1310,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/small goods</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1310,7 +1318,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/small goods</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1318,7 +1326,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1326,7 +1334,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/wearables</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1334,7 +1342,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle</t>
+          <t>google redesign/wearables</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1342,7 +1350,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel</t>
+          <t>google rmg redesign/lifestyle</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1350,7 +1358,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>google yellowesign/apparel</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1358,7 +1366,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1366,7 +1374,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1374,7 +1382,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1382,7 +1390,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1390,7 +1398,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1398,7 +1406,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
+          <t>store-policies/privacy-policy</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1406,7 +1414,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
+          <t>store-policies/return-policy</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1414,7 +1422,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
+          <t>store-policies/shipping-information</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1422,7 +1430,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>store-policies/terms-of-use</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1430,7 +1438,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1438,7 +1446,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1446,10 +1454,18 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>the google merchandise store - register</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
           <t>your wishlist</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr"/>
+      <c r="B55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1462,7 +1478,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B376"/>
+  <dimension ref="A1:B407"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1533,7 +1549,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google greenesign/apparel/google tee green</t>
+          <t>clearance/clearance-accessories</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -1541,7 +1557,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
+          <t>google greenesign/apparel/google tee green</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -1549,7 +1565,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
+          <t>google merchandise store - forgot password</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -1557,7 +1573,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google online store</t>
+          <t>google merchandise store - reset password</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1565,7 +1581,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google online store</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1573,7 +1589,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android iconic pin</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1581,7 +1597,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android large removable sticker sheet</t>
+          <t>google redesign/accessories/android iconic 4in decal</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1589,7 +1605,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android lumberjack pin</t>
+          <t>google redesign/accessories/android iconic pin</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1597,7 +1613,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android puzzlebot v2</t>
+          <t>google redesign/accessories/android large removable sticker sheet</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1605,7 +1621,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android sm sticker sheet</t>
+          <t>google redesign/accessories/android lumberjack pin</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1613,7 +1629,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android super hero 3d framed art</t>
+          <t>google redesign/accessories/android puzzlebot v2</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1621,7 +1637,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android techie 3d framed art</t>
+          <t>google redesign/accessories/android sm sticker sheet</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1629,7 +1645,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>google redesign/accessories/fun</t>
+          <t>google redesign/accessories/android super hero 3d framed art</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1637,7 +1653,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google blue yoyo</t>
+          <t>google redesign/accessories/android techie 3d framed art</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -1645,7 +1661,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google bot</t>
+          <t>google redesign/accessories/fun</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1653,7 +1669,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google bot multicolored</t>
+          <t>google redesign/accessories/google blue yoyo</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1661,7 +1677,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google campus bike</t>
+          <t>google redesign/accessories/google bot</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1669,7 +1685,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google chrome dinosaur collectible</t>
+          <t>google redesign/accessories/google bot multicolored</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1677,7 +1693,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed blue shades</t>
+          <t>google redesign/accessories/google campus bike</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1685,7 +1701,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed gray shades</t>
+          <t>google redesign/accessories/google chrome dinosaur collectible</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1693,7 +1709,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed yellow shades</t>
+          <t>google redesign/accessories/google clear framed blue shades</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1701,7 +1717,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cloth pouch black</t>
+          <t>google redesign/accessories/google clear framed gray shades</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1709,7 +1725,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork card holder</t>
+          <t>google redesign/accessories/google clear framed yellow shades</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1717,7 +1733,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork passport holder</t>
+          <t>google redesign/accessories/google cloth pouch black</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1725,7 +1741,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork tablet case</t>
+          <t>google redesign/accessories/google cork card holder</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1733,7 +1749,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji magnet set</t>
+          <t>google redesign/accessories/google cork passport holder</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1741,7 +1757,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
+          <t>google redesign/accessories/google cork tablet case</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1749,7 +1765,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt luggage tag</t>
+          <t>google redesign/accessories/google emoji magnet set</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1757,7 +1773,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google inverted umbrella</t>
+          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1765,7 +1781,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google keychain 19</t>
+          <t>google redesign/accessories/google felt luggage tag</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1773,7 +1789,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lapel pin</t>
+          <t>google redesign/accessories/google felt strap keyring</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1781,7 +1797,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google laptop sleeve charcoal</t>
+          <t>google redesign/accessories/google inverted umbrella</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1789,7 +1805,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google large pet collar blue green</t>
+          <t>google redesign/accessories/google keychain 19</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1797,7 +1813,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lovehandle black</t>
+          <t>google redesign/accessories/google lapel pin</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1805,7 +1821,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google magnet</t>
+          <t>google redesign/accessories/google laptop sleeve charcoal</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1813,7 +1829,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google maps pin</t>
+          <t>google redesign/accessories/google large pet collar blue green</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1821,7 +1837,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google medium pet collar blue green</t>
+          <t>google redesign/accessories/google large pet leash red yellow</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1829,7 +1845,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mouse pad navy</t>
+          <t>google redesign/accessories/google lovehandle black</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1837,7 +1853,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mural sticker sheet</t>
+          <t>google redesign/accessories/google magnet</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1845,7 +1861,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google pride sticker</t>
+          <t>google redesign/accessories/google maps pin</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1853,7 +1869,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google see no hear no set</t>
+          <t>google redesign/accessories/google medium pet collar blue green</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1861,7 +1877,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google small cable organizer blue</t>
+          <t>google redesign/accessories/google mouse pad navy</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1869,7 +1885,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google tech taco</t>
+          <t>google redesign/accessories/google mural sticker sheet</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1877,7 +1893,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google utensil set</t>
+          <t>google redesign/accessories/google nyc campus lapel pin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1885,7 +1901,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>google redesign/accessories/iamremarkable lapel pin</t>
+          <t>google redesign/accessories/google nyc campus sticker</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1893,7 +1909,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>google redesign/accessories/noogler android figure 2019</t>
+          <t>google redesign/accessories/google pride sticker</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1901,7 +1917,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
+          <t>google redesign/accessories/google see no hear no set</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1909,7 +1925,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube iconic play pin</t>
+          <t>google redesign/accessories/google sf campus lapel pin</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1917,7 +1933,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube small sticker sheet</t>
+          <t>google redesign/accessories/google small cable organizer blue</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1925,7 +1941,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/accessories/google tech taco</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1933,7 +1949,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android garden tee orange</t>
+          <t>google redesign/accessories/google utensil set</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1941,7 +1957,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic beanie</t>
+          <t>google redesign/accessories/google yellow yoyo</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1949,7 +1965,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic crew</t>
+          <t>google redesign/accessories/iamremarkable lapel pin</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1957,7 +1973,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat green</t>
+          <t>google redesign/accessories/noogler android figure 2019</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1965,7 +1981,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat v2 black</t>
+          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1973,7 +1989,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat white</t>
+          <t>google redesign/accessories/youtube iconic play pin</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1981,7 +1997,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic sock</t>
+          <t>google redesign/accessories/youtube small sticker sheet</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -1989,7 +2005,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie navy</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -1997,7 +2013,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie white</t>
+          <t>google redesign/apparel/android garden tee orange</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -2005,7 +2021,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee green</t>
+          <t>google redesign/apparel/android iconic beanie</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -2013,7 +2029,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee navy</t>
+          <t>google redesign/apparel/android iconic crew</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -2021,7 +2037,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee navy</t>
+          <t>google redesign/apparel/android iconic hat green</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -2029,7 +2045,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee white</t>
+          <t>google redesign/apparel/android iconic hat v2 black</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2037,7 +2053,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee green</t>
+          <t>google redesign/apparel/android iconic hat white</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2045,7 +2061,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee navy</t>
+          <t>google redesign/apparel/android iconic sock</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -2053,7 +2069,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>google redesign/apparel/flamingo and friends tee blue</t>
+          <t>google redesign/apparel/android pocket onesie navy</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -2061,7 +2077,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus unisex tee</t>
+          <t>google redesign/apparel/android pocket onesie white</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -2069,7 +2085,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus zip hoodie</t>
+          <t>google redesign/apparel/android pocket tee green</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2077,7 +2093,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google badge heavyweight pullover black</t>
+          <t>google redesign/apparel/android pocket tee navy</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2085,7 +2101,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black cloud zip hoodie</t>
+          <t>google redesign/apparel/android pocket toddler tee navy</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -2093,7 +2109,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black tee</t>
+          <t>google redesign/apparel/android pocket toddler tee white</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -2101,7 +2117,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus unisex tee</t>
+          <t>google redesign/apparel/android pocket youth tee green</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -2109,7 +2125,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
+          <t>google redesign/apparel/android pocket youth tee navy</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -2117,7 +2133,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google campus bike eco tee navy</t>
+          <t>google redesign/apparel/flamingo and friends tee blue</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -2125,7 +2141,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus unisex tee</t>
+          <t>google redesign/apparel/google austin campus unisex tee</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -2133,7 +2149,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus zip hoodie</t>
+          <t>google redesign/apparel/google austin campus zip hoodie</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -2141,7 +2157,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cotopaxi shell</t>
+          <t>google redesign/apparel/google badge heavyweight pullover black</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -2149,7 +2165,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew grey</t>
+          <t>google redesign/apparel/google black cloud zip hoodie</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2157,7 +2173,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew socks</t>
+          <t>google redesign/apparel/google black tee</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2165,7 +2181,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crewneck sweatshirt green</t>
+          <t>google redesign/apparel/google boulder campus unisex tee</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -2173,7 +2189,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google dino game tee</t>
+          <t>google redesign/apparel/google boulder campus zip hoodie</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -2181,7 +2197,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve ash</t>
+          <t>google redesign/apparel/google cambridge campus ladies tee</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2189,7 +2205,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google cambridge campus unisex tee</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2197,7 +2213,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google blue kids sunglasses</t>
+          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2205,7 +2221,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew combed cotton sock</t>
+          <t>google redesign/apparel/google campus bike eco tee navy</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -2213,7 +2229,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew striped athletic sock</t>
+          <t>google redesign/apparel/google chicago campus unisex tee</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -2221,7 +2237,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google kids playful tee</t>
+          <t>google redesign/apparel/google chicago campus zip hoodie</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -2229,7 +2245,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google premium sunglasses</t>
+          <t>google redesign/apparel/google cotopaxi shell</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2237,7 +2253,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google summer19 crew grey</t>
+          <t>google redesign/apparel/google crew grey</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2245,7 +2261,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google grey tee</t>
+          <t>google redesign/apparel/google crew socks</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -2253,7 +2269,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heather green speckled tee</t>
+          <t>google redesign/apparel/google crewneck sweatshirt green</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -2261,7 +2277,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heathered pom beanie</t>
+          <t>google redesign/apparel/google dino game tee</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -2269,7 +2285,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant charcoal onesie</t>
+          <t>google redesign/apparel/google fc longsleeve ash</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -2277,7 +2293,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero onesie grey</t>
+          <t>google redesign/apparel/google fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2285,7 +2301,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero tee olive</t>
+          <t>google redesign/apparel/google google blue kids sunglasses</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -2293,7 +2309,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google kirkland campus unisex tee</t>
+          <t>google redesign/apparel/google google crew combed cotton sock</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -2301,7 +2317,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus unisex tee</t>
+          <t>google redesign/apparel/google google crew striped athletic sock</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -2309,7 +2325,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus zip hoodie</t>
+          <t>google redesign/apparel/google google kids playful tee</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2317,7 +2333,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea cotton cap ls</t>
+          <t>google redesign/apparel/google google premium sunglasses</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2325,7 +2341,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea unisex tee</t>
+          <t>google redesign/apparel/google google red kids sunglasses</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -2333,7 +2349,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea womens eco tee</t>
+          <t>google redesign/apparel/google google summer19 crew grey</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -2341,7 +2357,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat black</t>
+          <t>google redesign/apparel/google grey tee</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -2349,7 +2365,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat blue</t>
+          <t>google redesign/apparel/google heather green speckled tee</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -2357,7 +2373,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens discovery lt rain shell</t>
+          <t>google redesign/apparel/google heathered pom beanie</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -2365,7 +2381,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens microfleece jacket black</t>
+          <t>google redesign/apparel/google infant charcoal onesie</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -2373,7 +2389,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens puff jacket black</t>
+          <t>google redesign/apparel/google infant hero onesie grey</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -2381,7 +2397,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens softshell moss</t>
+          <t>google redesign/apparel/google infant hero tee olive</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -2389,7 +2405,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece grey</t>
+          <t>google redesign/apparel/google kirkland campus unisex tee</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -2397,7 +2413,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google la campus unisex tee</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -2405,7 +2421,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee blue</t>
+          <t>google redesign/apparel/google la campus zip hoodie</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -2413,7 +2429,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mural socks</t>
+          <t>google redesign/apparel/google land and sea cotton cap ls</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -2421,7 +2437,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google navy speckled tee</t>
+          <t>google redesign/apparel/google land and sea unisex tee</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -2429,7 +2445,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus unisex tee</t>
+          <t>google redesign/apparel/google land and sea womens eco tee</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -2437,7 +2453,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus zip hoodie</t>
+          <t>google redesign/apparel/google leather strap hat black</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -2445,7 +2461,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus unisex tee</t>
+          <t>google redesign/apparel/google leather strap hat blue</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -2453,7 +2469,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus zip hoodie</t>
+          <t>google redesign/apparel/google mens discovery lt rain shell</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -2461,7 +2477,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google raincoat navy</t>
+          <t>google redesign/apparel/google mens microfleece jacket black</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -2469,7 +2485,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google red speckled tee</t>
+          <t>google redesign/apparel/google mens puff jacket black</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -2477,7 +2493,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google seattle campus unisex tee</t>
+          <t>google redesign/apparel/google mens softshell moss</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -2485,7 +2501,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus ladies tee</t>
+          <t>google redesign/apparel/google mens tech fleece grey</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -2493,7 +2509,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus unisex tee</t>
+          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -2501,7 +2517,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus zip hoodie</t>
+          <t>google redesign/apparel/google mountain view tee blue</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -2509,7 +2525,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa vest black</t>
+          <t>google redesign/apparel/google mountain view tee red</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -2517,7 +2533,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
+          <t>google redesign/apparel/google mural socks</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -2525,7 +2541,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
+          <t>google redesign/apparel/google navy speckled tee</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
@@ -2533,7 +2549,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie grey</t>
+          <t>google redesign/apparel/google nyc campus ladies tee</t>
         </is>
       </c>
       <c r="B133" t="inlineStr"/>
@@ -2541,7 +2557,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie navy</t>
+          <t>google redesign/apparel/google nyc campus unisex tee</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -2549,7 +2565,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google split seam tee olive</t>
+          <t>google redesign/apparel/google nyc campus zip hoodie</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
@@ -2557,7 +2573,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee blue</t>
+          <t>google redesign/apparel/google pnw campus unisex tee</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -2565,7 +2581,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee dark blue</t>
+          <t>google redesign/apparel/google pnw campus zip hoodie</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -2573,7 +2589,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee fc black</t>
+          <t>google redesign/apparel/google raincoat navy</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -2581,7 +2597,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee mint green</t>
+          <t>google redesign/apparel/google red speckled tee</t>
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
@@ -2589,7 +2605,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee red</t>
+          <t>google redesign/apparel/google seattle campus unisex tee</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -2597,7 +2613,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc tee charcoal</t>
+          <t>google redesign/apparel/google sf campus ladies tee</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -2605,7 +2621,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc zip hoodie</t>
+          <t>google redesign/apparel/google sf campus unisex tee</t>
         </is>
       </c>
       <c r="B142" t="inlineStr"/>
@@ -2613,7 +2629,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee black</t>
+          <t>google redesign/apparel/google sf campus zip hoodie</t>
         </is>
       </c>
       <c r="B143" t="inlineStr"/>
@@ -2621,7 +2637,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee olive</t>
+          <t>google redesign/apparel/google sherpa vest black</t>
         </is>
       </c>
       <c r="B144" t="inlineStr"/>
@@ -2629,7 +2645,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler tee white</t>
+          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -2637,7 +2653,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee coral</t>
+          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -2645,7 +2661,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee spearmint</t>
+          <t>google redesign/apparel/google speckled beanie grey</t>
         </is>
       </c>
       <c r="B147" t="inlineStr"/>
@@ -2653,7 +2669,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tracking hat</t>
+          <t>google redesign/apparel/google speckled beanie navy</t>
         </is>
       </c>
       <c r="B148" t="inlineStr"/>
@@ -2661,7 +2677,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tudes recycled tee</t>
+          <t>google redesign/apparel/google split seam tee olive</t>
         </is>
       </c>
       <c r="B149" t="inlineStr"/>
@@ -2669,7 +2685,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google twill cap charcoal</t>
+          <t>google redesign/apparel/google tee blue</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
@@ -2677,7 +2693,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex eco tee black</t>
+          <t>google redesign/apparel/google tee dark blue</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -2685,7 +2701,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
+          <t>google redesign/apparel/google tee fc black</t>
         </is>
       </c>
       <c r="B152" t="inlineStr"/>
@@ -2693,7 +2709,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google pocket tee grey</t>
+          <t>google redesign/apparel/google tee mint green</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
@@ -2701,7 +2717,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex pride eco-tee black</t>
+          <t>google redesign/apparel/google tee red</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -2709,7 +2725,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens black tee</t>
+          <t>google redesign/apparel/google toddler fc tee charcoal</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
@@ -2717,7 +2733,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens discovery</t>
+          <t>google redesign/apparel/google toddler fc zip hoodie</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -2725,7 +2741,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens eco tee black</t>
+          <t>google redesign/apparel/google toddler hero tee black</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
@@ -2733,7 +2749,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens google striped ls</t>
+          <t>google redesign/apparel/google toddler hero tee olive</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
@@ -2741,7 +2757,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens grid zip up</t>
+          <t>google redesign/apparel/google toddler tee white</t>
         </is>
       </c>
       <c r="B159" t="inlineStr"/>
@@ -2749,7 +2765,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens kirkland pullover</t>
+          <t>google redesign/apparel/google tonal tee coral</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
@@ -2757,7 +2773,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens microfleece jacket black</t>
+          <t>google redesign/apparel/google tonal tee spearmint</t>
         </is>
       </c>
       <c r="B161" t="inlineStr"/>
@@ -2765,7 +2781,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens pride eco-tee black</t>
+          <t>google redesign/apparel/google tracking hat</t>
         </is>
       </c>
       <c r="B162" t="inlineStr"/>
@@ -2773,7 +2789,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens puff jacket black</t>
+          <t>google redesign/apparel/google tudes recycled tee</t>
         </is>
       </c>
       <c r="B163" t="inlineStr"/>
@@ -2781,7 +2797,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens softshell moss</t>
+          <t>google redesign/apparel/google twill cap charcoal</t>
         </is>
       </c>
       <c r="B164" t="inlineStr"/>
@@ -2789,7 +2805,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece grey</t>
+          <t>google redesign/apparel/google unisex eco tee black</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -2797,7 +2813,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
@@ -2805,7 +2821,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee navy</t>
+          <t>google redesign/apparel/google unisex google pocket tee grey</t>
         </is>
       </c>
       <c r="B167" t="inlineStr"/>
@@ -2813,7 +2829,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee olive</t>
+          <t>google redesign/apparel/google unisex pride eco-tee black</t>
         </is>
       </c>
       <c r="B168" t="inlineStr"/>
@@ -2821,7 +2837,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google womens black tee</t>
         </is>
       </c>
       <c r="B169" t="inlineStr"/>
@@ -2829,7 +2845,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc pullover hoodie</t>
+          <t>google redesign/apparel/google womens discovery</t>
         </is>
       </c>
       <c r="B170" t="inlineStr"/>
@@ -2837,7 +2853,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc tee charcoal</t>
+          <t>google redesign/apparel/google womens eco tee black</t>
         </is>
       </c>
       <c r="B171" t="inlineStr"/>
@@ -2845,7 +2861,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc zip hoodie</t>
+          <t>google redesign/apparel/google womens google striped ls</t>
         </is>
       </c>
       <c r="B172" t="inlineStr"/>
@@ -2853,7 +2869,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee grey</t>
+          <t>google redesign/apparel/google womens grid zip up</t>
         </is>
       </c>
       <c r="B173" t="inlineStr"/>
@@ -2861,7 +2877,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee maroon</t>
+          <t>google redesign/apparel/google womens kirkland pullover</t>
         </is>
       </c>
       <c r="B174" t="inlineStr"/>
@@ -2869,7 +2885,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth jumbo print tee white</t>
+          <t>google redesign/apparel/google womens microfleece jacket black</t>
         </is>
       </c>
       <c r="B175" t="inlineStr"/>
@@ -2877,7 +2893,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google zip hoodie fc</t>
+          <t>google redesign/apparel/google womens pride eco-tee black</t>
         </is>
       </c>
       <c r="B176" t="inlineStr"/>
@@ -2885,7 +2901,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>google redesign/apparel/hats</t>
+          <t>google redesign/apparel/google womens puff jacket black</t>
         </is>
       </c>
       <c r="B177" t="inlineStr"/>
@@ -2893,7 +2909,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable hoodie</t>
+          <t>google redesign/apparel/google womens softshell moss</t>
         </is>
       </c>
       <c r="B178" t="inlineStr"/>
@@ -2901,7 +2917,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
+          <t>google redesign/apparel/google womens tech fleece grey</t>
         </is>
       </c>
       <c r="B179" t="inlineStr"/>
@@ -2909,7 +2925,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
+          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B180" t="inlineStr"/>
@@ -2917,7 +2933,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>google redesign/apparel/kids</t>
+          <t>google redesign/apparel/google youth badge tee navy</t>
         </is>
       </c>
       <c r="B181" t="inlineStr"/>
@@ -2925,7 +2941,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>google redesign/apparel/mens</t>
+          <t>google redesign/apparel/google youth badge tee olive</t>
         </is>
       </c>
       <c r="B182" t="inlineStr"/>
@@ -2933,7 +2949,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>google redesign/apparel/socks</t>
+          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B183" t="inlineStr"/>
@@ -2941,7 +2957,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends tee green</t>
+          <t>google redesign/apparel/google youth fc pullover hoodie</t>
         </is>
       </c>
       <c r="B184" t="inlineStr"/>
@@ -2949,7 +2965,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends toddler tee green</t>
+          <t>google redesign/apparel/google youth fc tee charcoal</t>
         </is>
       </c>
       <c r="B185" t="inlineStr"/>
@@ -2957,7 +2973,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>google redesign/apparel/womens</t>
+          <t>google redesign/apparel/google youth fc zip hoodie</t>
         </is>
       </c>
       <c r="B186" t="inlineStr"/>
@@ -2965,7 +2981,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube crew socks</t>
+          <t>google redesign/apparel/google youth hero tee grey</t>
         </is>
       </c>
       <c r="B187" t="inlineStr"/>
@@ -2973,7 +2989,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube favorite tee white</t>
+          <t>google redesign/apparel/google youth hero tee maroon</t>
         </is>
       </c>
       <c r="B188" t="inlineStr"/>
@@ -2981,7 +2997,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon hoodie black</t>
+          <t>google redesign/apparel/google youth jumbo print tee white</t>
         </is>
       </c>
       <c r="B189" t="inlineStr"/>
@@ -2989,7 +3005,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee charcoal</t>
+          <t>google redesign/apparel/google zip hoodie fc</t>
         </is>
       </c>
       <c r="B190" t="inlineStr"/>
@@ -2997,7 +3013,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee grey</t>
+          <t>google redesign/apparel/hats</t>
         </is>
       </c>
       <c r="B191" t="inlineStr"/>
@@ -3005,7 +3021,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube leather strap hat black</t>
+          <t>google redesign/apparel/iamremarkable hoodie</t>
         </is>
       </c>
       <c r="B192" t="inlineStr"/>
@@ -3013,7 +3029,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube standards zip hoodie black</t>
+          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
         </is>
       </c>
       <c r="B193" t="inlineStr"/>
@@ -3021,7 +3037,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube transmission journal red</t>
+          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
         </is>
       </c>
       <c r="B194" t="inlineStr"/>
@@ -3029,7 +3045,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube twill cap sandwich black</t>
+          <t>google redesign/apparel/kids</t>
         </is>
       </c>
       <c r="B195" t="inlineStr"/>
@@ -3037,7 +3053,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers onesie pink</t>
+          <t>google redesign/apparel/mens</t>
         </is>
       </c>
       <c r="B196" t="inlineStr"/>
@@ -3045,7 +3061,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+          <t>google redesign/apparel/socks</t>
         </is>
       </c>
       <c r="B197" t="inlineStr"/>
@@ -3053,7 +3069,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>google redesign/bags/android iconic backpack</t>
+          <t>google redesign/apparel/stan and friends onesie green</t>
         </is>
       </c>
       <c r="B198" t="inlineStr"/>
@@ -3061,7 +3077,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>google redesign/bags/backpacks</t>
+          <t>google redesign/apparel/stan and friends tee green</t>
         </is>
       </c>
       <c r="B199" t="inlineStr"/>
@@ -3069,7 +3085,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>google redesign/bags/essential canvas tote</t>
+          <t>google redesign/apparel/stan and friends toddler tee green</t>
         </is>
       </c>
       <c r="B200" t="inlineStr"/>
@@ -3077,7 +3093,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>google redesign/bags/google bike mini backpack</t>
+          <t>google redesign/apparel/stan and friends youth tee green</t>
         </is>
       </c>
       <c r="B201" t="inlineStr"/>
@@ -3085,7 +3101,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>google redesign/bags/google flat front bag grey</t>
+          <t>google redesign/apparel/womens</t>
         </is>
       </c>
       <c r="B202" t="inlineStr"/>
@@ -3093,7 +3109,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google campus bike tote navy</t>
+          <t>google redesign/apparel/youtube crew socks</t>
         </is>
       </c>
       <c r="B203" t="inlineStr"/>
@@ -3101,7 +3117,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google confetti accessory pouch</t>
+          <t>google redesign/apparel/youtube favorite tee white</t>
         </is>
       </c>
       <c r="B204" t="inlineStr"/>
@@ -3109,7 +3125,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google striped penny pouch</t>
+          <t>google redesign/apparel/youtube icon hoodie black</t>
         </is>
       </c>
       <c r="B205" t="inlineStr"/>
@@ -3117,7 +3133,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>google redesign/bags/google hemp tote</t>
+          <t>google redesign/apparel/youtube icon tee charcoal</t>
         </is>
       </c>
       <c r="B206" t="inlineStr"/>
@@ -3125,7 +3141,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito dopp kit v2</t>
+          <t>google redesign/apparel/youtube icon tee grey</t>
         </is>
       </c>
       <c r="B207" t="inlineStr"/>
@@ -3133,7 +3149,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito flap pack</t>
+          <t>google redesign/apparel/youtube leather strap hat black</t>
         </is>
       </c>
       <c r="B208" t="inlineStr"/>
@@ -3141,7 +3157,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito laptop organizer v2</t>
+          <t>google redesign/apparel/youtube standards zip hoodie black</t>
         </is>
       </c>
       <c r="B209" t="inlineStr"/>
@@ -3149,7 +3165,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito messenger bag</t>
+          <t>google redesign/apparel/youtube transmission journal red</t>
         </is>
       </c>
       <c r="B210" t="inlineStr"/>
@@ -3157,7 +3173,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito techpack v2</t>
+          <t>google redesign/apparel/youtube twill cap sandwich black</t>
         </is>
       </c>
       <c r="B211" t="inlineStr"/>
@@ -3165,7 +3181,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito zippack v2</t>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
         </is>
       </c>
       <c r="B212" t="inlineStr"/>
@@ -3173,7 +3189,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>google redesign/bags/google large tote white</t>
+          <t>google redesign/bags/android iconic backpack</t>
         </is>
       </c>
       <c r="B213" t="inlineStr"/>
@@ -3181,7 +3197,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mesh bag blue</t>
+          <t>google redesign/bags/backpacks</t>
         </is>
       </c>
       <c r="B214" t="inlineStr"/>
@@ -3189,7 +3205,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mural tote</t>
+          <t>google redesign/bags/essential canvas tote</t>
         </is>
       </c>
       <c r="B215" t="inlineStr"/>
@@ -3197,7 +3213,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>google redesign/bags/google packable bag black</t>
+          <t>google redesign/bags/google bike mini backpack</t>
         </is>
       </c>
       <c r="B216" t="inlineStr"/>
@@ -3205,7 +3221,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>google redesign/bags/google seaport tote</t>
+          <t>google redesign/bags/google cambridge campus tote</t>
         </is>
       </c>
       <c r="B217" t="inlineStr"/>
@@ -3213,7 +3229,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>google redesign/bags/google totepak</t>
+          <t>google redesign/bags/google flat front bag grey</t>
         </is>
       </c>
       <c r="B218" t="inlineStr"/>
@@ -3221,7 +3237,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility backpack</t>
+          <t>google redesign/bags/google google campus bike carry pouch</t>
         </is>
       </c>
       <c r="B219" t="inlineStr"/>
@@ -3229,7 +3245,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility bag grey</t>
+          <t>google redesign/bags/google google campus bike tote navy</t>
         </is>
       </c>
       <c r="B220" t="inlineStr"/>
@@ -3237,7 +3253,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>google redesign/bags/iamremarkable tote</t>
+          <t>google redesign/bags/google google confetti accessory pouch</t>
         </is>
       </c>
       <c r="B221" t="inlineStr"/>
@@ -3245,7 +3261,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>google redesign/bags/more bags</t>
+          <t>google redesign/bags/google google striped penny pouch</t>
         </is>
       </c>
       <c r="B222" t="inlineStr"/>
@@ -3253,7 +3269,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>google redesign/bags/shopping and totes</t>
+          <t>google redesign/bags/google hemp tote</t>
         </is>
       </c>
       <c r="B223" t="inlineStr"/>
@@ -3261,7 +3277,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper backpack</t>
+          <t>google redesign/bags/google incognito dopp kit v2</t>
         </is>
       </c>
       <c r="B224" t="inlineStr"/>
@@ -3269,7 +3285,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper lunch sack</t>
+          <t>google redesign/bags/google incognito flap pack</t>
         </is>
       </c>
       <c r="B225" t="inlineStr"/>
@@ -3277,7 +3293,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper tote</t>
+          <t>google redesign/bags/google incognito laptop organizer v2</t>
         </is>
       </c>
       <c r="B226" t="inlineStr"/>
@@ -3285,7 +3301,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
+          <t>google redesign/bags/google incognito messenger bag</t>
         </is>
       </c>
       <c r="B227" t="inlineStr"/>
@@ -3293,7 +3309,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
+          <t>google redesign/bags/google incognito techpack v2</t>
         </is>
       </c>
       <c r="B228" t="inlineStr"/>
@@ -3301,7 +3317,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus mug</t>
+          <t>google redesign/bags/google incognito zippack v2</t>
         </is>
       </c>
       <c r="B229" t="inlineStr"/>
@@ -3309,7 +3325,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus sticker</t>
+          <t>google redesign/bags/google large tote white</t>
         </is>
       </c>
       <c r="B230" t="inlineStr"/>
@@ -3317,7 +3333,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
+          <t>google redesign/bags/google mesh bag blue</t>
         </is>
       </c>
       <c r="B231" t="inlineStr"/>
@@ -3325,7 +3341,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
+          <t>google redesign/bags/google mesh bag red</t>
         </is>
       </c>
       <c r="B232" t="inlineStr"/>
@@ -3333,7 +3349,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
+          <t>google redesign/bags/google mural tote</t>
         </is>
       </c>
       <c r="B233" t="inlineStr"/>
@@ -3341,7 +3357,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus ladies tee</t>
+          <t>google redesign/bags/google packable bag black</t>
         </is>
       </c>
       <c r="B234" t="inlineStr"/>
@@ -3349,7 +3365,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus mug</t>
+          <t>google redesign/bags/google seaport tote</t>
         </is>
       </c>
       <c r="B235" t="inlineStr"/>
@@ -3357,7 +3373,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
+          <t>google redesign/bags/google sf campus tote</t>
         </is>
       </c>
       <c r="B236" t="inlineStr"/>
@@ -3365,7 +3381,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
+          <t>google redesign/bags/google totepak</t>
         </is>
       </c>
       <c r="B237" t="inlineStr"/>
@@ -3373,7 +3389,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
+          <t>google redesign/bags/google utility backpack</t>
         </is>
       </c>
       <c r="B238" t="inlineStr"/>
@@ -3381,7 +3397,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
+          <t>google redesign/bags/google utility bag grey</t>
         </is>
       </c>
       <c r="B239" t="inlineStr"/>
@@ -3389,7 +3405,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android buoy bottle</t>
+          <t>google redesign/bags/iamremarkable tote</t>
         </is>
       </c>
       <c r="B240" t="inlineStr"/>
@@ -3397,7 +3413,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic mug gray</t>
+          <t>google redesign/bags/more bags</t>
         </is>
       </c>
       <c r="B241" t="inlineStr"/>
@@ -3405,7 +3421,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/campus corkbase mug blue</t>
+          <t>google redesign/bags/shopping and totes</t>
         </is>
       </c>
       <c r="B242" t="inlineStr"/>
@@ -3413,7 +3429,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 16oz tumbler blue</t>
+          <t>google redesign/bags/supernatural paper backpack</t>
         </is>
       </c>
       <c r="B243" t="inlineStr"/>
@@ -3421,7 +3437,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
+          <t>google redesign/bags/supernatural paper lunch sack</t>
         </is>
       </c>
       <c r="B244" t="inlineStr"/>
@@ -3429,7 +3445,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle red</t>
+          <t>google redesign/bags/supernatural paper tote</t>
         </is>
       </c>
       <c r="B245" t="inlineStr"/>
@@ -3437,7 +3453,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google bike bottle</t>
+          <t>google redesign/blm unisex pullover hoodie</t>
         </is>
       </c>
       <c r="B246" t="inlineStr"/>
@@ -3445,7 +3461,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus bottle</t>
+          <t>google redesign/campus collection</t>
         </is>
       </c>
       <c r="B247" t="inlineStr"/>
@@ -3453,7 +3469,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus mug</t>
+          <t>google redesign/campus collection/google mountain view campus mug</t>
         </is>
       </c>
       <c r="B248" t="inlineStr"/>
@@ -3461,7 +3477,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google camp mug ivory</t>
+          <t>google redesign/campus collection/google mountain view campus sticker</t>
         </is>
       </c>
       <c r="B249" t="inlineStr"/>
@@ -3469,7 +3485,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google canteen bottle black</t>
+          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
         </is>
       </c>
       <c r="B250" t="inlineStr"/>
@@ -3477,7 +3493,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google chicago campus mug</t>
+          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
         </is>
       </c>
       <c r="B251" t="inlineStr"/>
@@ -3485,7 +3501,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cork base tumbler</t>
+          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
         </is>
       </c>
       <c r="B252" t="inlineStr"/>
@@ -3493,7 +3509,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cup cap tumbler grey</t>
+          <t>google redesign/campus collection/google sunnyvale campus ladies tee</t>
         </is>
       </c>
       <c r="B253" t="inlineStr"/>
@@ -3501,7 +3517,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google glass bottle</t>
+          <t>google redesign/campus collection/google sunnyvale campus mug</t>
         </is>
       </c>
       <c r="B254" t="inlineStr"/>
@@ -3509,7 +3525,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google keepcup</t>
+          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
         </is>
       </c>
       <c r="B255" t="inlineStr"/>
@@ -3517,7 +3533,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google kirkland campus mug</t>
+          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
         </is>
       </c>
       <c r="B256" t="inlineStr"/>
@@ -3525,7 +3541,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google la campus mug</t>
+          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
         </is>
       </c>
       <c r="B257" t="inlineStr"/>
@@ -3533,7 +3549,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural bottle</t>
+          <t>google redesign/clearance</t>
         </is>
       </c>
       <c r="B258" t="inlineStr"/>
@@ -3541,7 +3557,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural mug</t>
+          <t>google redesign/drinkware/android buoy bottle</t>
         </is>
       </c>
       <c r="B259" t="inlineStr"/>
@@ -3549,7 +3565,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus bottle</t>
+          <t>google redesign/drinkware/android iconic glass bottle green</t>
         </is>
       </c>
       <c r="B260" t="inlineStr"/>
@@ -3557,7 +3573,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus mug</t>
+          <t>google redesign/drinkware/android iconic mug gray</t>
         </is>
       </c>
       <c r="B261" t="inlineStr"/>
@@ -3565,7 +3581,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google perk thermal cup</t>
+          <t>google redesign/drinkware/campus corkbase mug blue</t>
         </is>
       </c>
       <c r="B262" t="inlineStr"/>
@@ -3573,7 +3589,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google pnw campus mug</t>
+          <t>google redesign/drinkware/google 16oz tumbler blue</t>
         </is>
       </c>
       <c r="B263" t="inlineStr"/>
@@ -3581,7 +3597,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google seattle campus mug</t>
+          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
         </is>
       </c>
       <c r="B264" t="inlineStr"/>
@@ -3589,7 +3605,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus bottle</t>
+          <t>google redesign/drinkware/google 24oz ring bottle red</t>
         </is>
       </c>
       <c r="B265" t="inlineStr"/>
@@ -3597,7 +3613,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus mug</t>
+          <t>google redesign/drinkware/google austin campus bottle</t>
         </is>
       </c>
       <c r="B266" t="inlineStr"/>
@@ -3605,7 +3621,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler blue lid</t>
+          <t>google redesign/drinkware/google austin campus mug</t>
         </is>
       </c>
       <c r="B267" t="inlineStr"/>
@@ -3613,7 +3629,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler red lid</t>
+          <t>google redesign/drinkware/google bike bottle</t>
         </is>
       </c>
       <c r="B268" t="inlineStr"/>
@@ -3621,7 +3637,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google thermal tumbler navy</t>
+          <t>google redesign/drinkware/google boulder campus mug</t>
         </is>
       </c>
       <c r="B269" t="inlineStr"/>
@@ -3629,7 +3645,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google woodtop bottle black</t>
+          <t>google redesign/drinkware/google cambridge campus bottle</t>
         </is>
       </c>
       <c r="B270" t="inlineStr"/>
@@ -3637,7 +3653,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/iamremarkable water bottle</t>
+          <t>google redesign/drinkware/google cambridge campus mug</t>
         </is>
       </c>
       <c r="B271" t="inlineStr"/>
@@ -3645,7 +3661,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/mugs tumblers</t>
+          <t>google redesign/drinkware/google camp mug ivory</t>
         </is>
       </c>
       <c r="B272" t="inlineStr"/>
@@ -3653,7 +3669,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
+          <t>google redesign/drinkware/google canteen bottle black</t>
         </is>
       </c>
       <c r="B273" t="inlineStr"/>
@@ -3661,7 +3677,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
+          <t>google redesign/drinkware/google chicago campus mug</t>
         </is>
       </c>
       <c r="B274" t="inlineStr"/>
@@ -3669,7 +3685,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/water bottles</t>
+          <t>google redesign/drinkware/google cork base tumbler</t>
         </is>
       </c>
       <c r="B275" t="inlineStr"/>
@@ -3677,7 +3693,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
+          <t>google redesign/drinkware/google cup cap tumbler grey</t>
         </is>
       </c>
       <c r="B276" t="inlineStr"/>
@@ -3685,7 +3701,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube play mug</t>
+          <t>google redesign/drinkware/google glass bottle</t>
         </is>
       </c>
       <c r="B277" t="inlineStr"/>
@@ -3693,7 +3709,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
+          <t>google redesign/drinkware/google keepcup</t>
         </is>
       </c>
       <c r="B278" t="inlineStr"/>
@@ -3701,7 +3717,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
+          <t>google redesign/drinkware/google kirkland campus mug</t>
         </is>
       </c>
       <c r="B279" t="inlineStr"/>
@@ -3709,7 +3725,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>google redesign/electronics/accessories</t>
+          <t>google redesign/drinkware/google la campus bottle</t>
         </is>
       </c>
       <c r="B280" t="inlineStr"/>
@@ -3717,7 +3733,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>google redesign/electronics/audio</t>
+          <t>google redesign/drinkware/google la campus mug</t>
         </is>
       </c>
       <c r="B281" t="inlineStr"/>
@@ -3725,7 +3741,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
+          <t>google redesign/drinkware/google mural bottle</t>
         </is>
       </c>
       <c r="B282" t="inlineStr"/>
@@ -3733,7 +3749,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
+          <t>google redesign/drinkware/google mural mug</t>
         </is>
       </c>
       <c r="B283" t="inlineStr"/>
@@ -3741,7 +3757,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
+          <t>google redesign/drinkware/google nyc campus bottle</t>
         </is>
       </c>
       <c r="B284" t="inlineStr"/>
@@ -3749,7 +3765,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
+          <t>google redesign/drinkware/google nyc campus mug</t>
         </is>
       </c>
       <c r="B285" t="inlineStr"/>
@@ -3757,7 +3773,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
+          <t>google redesign/drinkware/google perk thermal cup</t>
         </is>
       </c>
       <c r="B286" t="inlineStr"/>
@@ -3765,7 +3781,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/drinkware/google pnw campus bottle</t>
         </is>
       </c>
       <c r="B287" t="inlineStr"/>
@@ -3773,7 +3789,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/drinkware/google pnw campus mug</t>
         </is>
       </c>
       <c r="B288" t="inlineStr"/>
@@ -3781,7 +3797,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/drinkware/google seattle campus mug</t>
         </is>
       </c>
       <c r="B289" t="inlineStr"/>
@@ -3789,7 +3805,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/drinkware/google sf campus bottle</t>
         </is>
       </c>
       <c r="B290" t="inlineStr"/>
@@ -3797,7 +3813,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/bags</t>
+          <t>google redesign/drinkware/google sf campus mug</t>
         </is>
       </c>
       <c r="B291" t="inlineStr"/>
@@ -3805,7 +3821,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/drinkware</t>
+          <t>google redesign/drinkware/google super g tumbler blue lid</t>
         </is>
       </c>
       <c r="B292" t="inlineStr"/>
@@ -3813,7 +3829,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/fun</t>
+          <t>google redesign/drinkware/google super g tumbler red lid</t>
         </is>
       </c>
       <c r="B293" t="inlineStr"/>
@@ -3821,7 +3837,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google aluminum bottle red</t>
+          <t>google redesign/drinkware/google thermal tumbler navy</t>
         </is>
       </c>
       <c r="B294" t="inlineStr"/>
@@ -3829,7 +3845,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google bear baby blanket beige</t>
+          <t>google redesign/drinkware/google woodtop bottle black</t>
         </is>
       </c>
       <c r="B295" t="inlineStr"/>
@@ -3837,7 +3853,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google camp mug gray</t>
+          <t>google redesign/drinkware/iamremarkable water bottle</t>
         </is>
       </c>
       <c r="B296" t="inlineStr"/>
@@ -3845,7 +3861,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google knit blanket</t>
+          <t>google redesign/drinkware/mugs tumblers</t>
         </is>
       </c>
       <c r="B297" t="inlineStr"/>
@@ -3853,7 +3869,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
+          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
         </is>
       </c>
       <c r="B298" t="inlineStr"/>
@@ -3861,7 +3877,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea tote bag</t>
+          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
         </is>
       </c>
       <c r="B299" t="inlineStr"/>
@@ -3869,7 +3885,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google-frisbee</t>
+          <t>google redesign/drinkware/water bottles</t>
         </is>
       </c>
       <c r="B300" t="inlineStr"/>
@@ -3877,7 +3893,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/small goods</t>
+          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
         </is>
       </c>
       <c r="B301" t="inlineStr"/>
@@ -3885,7 +3901,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/white google shoreline bottle</t>
+          <t>google redesign/drinkware/youtube play mug</t>
         </is>
       </c>
       <c r="B302" t="inlineStr"/>
@@ -3893,7 +3909,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/eco friendly</t>
         </is>
       </c>
       <c r="B303" t="inlineStr"/>
@@ -3901,7 +3917,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals/google large standard journal grey</t>
+          <t>google redesign/electronics</t>
         </is>
       </c>
       <c r="B304" t="inlineStr"/>
@@ -3909,7 +3925,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/electronics/accessories</t>
         </is>
       </c>
       <c r="B305" t="inlineStr"/>
@@ -3917,7 +3933,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>google redesign/office/android iconic notebook</t>
+          <t>google redesign/electronics/audio</t>
         </is>
       </c>
       <c r="B306" t="inlineStr"/>
@@ -3925,7 +3941,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>google redesign/office/android large trace journal black</t>
+          <t>google redesign/gift cards</t>
         </is>
       </c>
       <c r="B307" t="inlineStr"/>
@@ -3933,7 +3949,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>google redesign/office/android small trace journal bl</t>
+          <t>google redesign/google blue stojo cup</t>
         </is>
       </c>
       <c r="B308" t="inlineStr"/>
@@ -3941,7 +3957,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>google redesign/office/google appeel journal red</t>
+          <t>google redesign/google chrome dino light up water bottle</t>
         </is>
       </c>
       <c r="B309" t="inlineStr"/>
@@ -3949,7 +3965,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>google redesign/office/google black cork journal</t>
+          <t>google redesign/google crew sweater navy</t>
         </is>
       </c>
       <c r="B310" t="inlineStr"/>
@@ -3957,7 +3973,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>google redesign/office/google clear pen 4pack</t>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
         </is>
       </c>
       <c r="B311" t="inlineStr"/>
@@ -3965,7 +3981,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork journal</t>
+          <t>google redesign/google land and sea french terry sweatshirt ls</t>
         </is>
       </c>
       <c r="B312" t="inlineStr"/>
@@ -3973,7 +3989,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork pencil pouch</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B313" t="inlineStr"/>
@@ -3981,7 +3997,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>google redesign/office/google felt refillable journal</t>
+          <t>google redesign/google land and sea mug ls</t>
         </is>
       </c>
       <c r="B314" t="inlineStr"/>
@@ -3989,7 +4005,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>google redesign/office/google google campus bike grid task pad</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B315" t="inlineStr"/>
@@ -3997,7 +4013,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>google redesign/office/google google color block notebook</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B316" t="inlineStr"/>
@@ -4005,7 +4021,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti pen white</t>
+          <t>google redesign/lifestyle/bags</t>
         </is>
       </c>
       <c r="B317" t="inlineStr"/>
@@ -4013,7 +4029,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti slim task pad</t>
+          <t>google redesign/lifestyle/drinkware</t>
         </is>
       </c>
       <c r="B318" t="inlineStr"/>
@@ -4021,7 +4037,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti task pad</t>
+          <t>google redesign/lifestyle/fun</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
@@ -4029,7 +4045,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen blue</t>
+          <t>google redesign/lifestyle/google aluminum bottle red</t>
         </is>
       </c>
       <c r="B320" t="inlineStr"/>
@@ -4037,7 +4053,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen green</t>
+          <t>google redesign/lifestyle/google bear baby blanket beige</t>
         </is>
       </c>
       <c r="B321" t="inlineStr"/>
@@ -4045,7 +4061,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen red</t>
+          <t>google redesign/lifestyle/google camp mug gray</t>
         </is>
       </c>
       <c r="B322" t="inlineStr"/>
@@ -4053,7 +4069,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural notebook</t>
+          <t>google redesign/lifestyle/google knit blanket</t>
         </is>
       </c>
       <c r="B323" t="inlineStr"/>
@@ -4061,7 +4077,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural sticky note pad</t>
+          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
@@ -4069,7 +4085,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen citron</t>
+          <t>google redesign/lifestyle/google land and sea tote bag</t>
         </is>
       </c>
       <c r="B325" t="inlineStr"/>
@@ -4077,7 +4093,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grey</t>
+          <t>google redesign/lifestyle/google-frisbee</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
@@ -4085,7 +4101,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen red</t>
+          <t>google redesign/lifestyle/small goods</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
@@ -4093,7 +4109,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen white</t>
+          <t>google redesign/lifestyle/white google shoreline bottle</t>
         </is>
       </c>
       <c r="B328" t="inlineStr"/>
@@ -4101,7 +4117,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>google redesign/office/google phone stand bamboo</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
@@ -4109,7 +4125,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled notebook set natural</t>
+          <t>google redesign/notebooks journals/google large standard journal grey</t>
         </is>
       </c>
       <c r="B330" t="inlineStr"/>
@@ -4117,7 +4133,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen black</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B331" t="inlineStr"/>
@@ -4125,7 +4141,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen green</t>
+          <t>google redesign/office/android iconic notebook</t>
         </is>
       </c>
       <c r="B332" t="inlineStr"/>
@@ -4133,7 +4149,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled writing set</t>
+          <t>google redesign/office/android iconic pen</t>
         </is>
       </c>
       <c r="B333" t="inlineStr"/>
@@ -4141,7 +4157,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>google redesign/office/google small standard journal navy</t>
+          <t>google redesign/office/android large trace journal black</t>
         </is>
       </c>
       <c r="B334" t="inlineStr"/>
@@ -4149,7 +4165,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>google redesign/office/google soft modal scarf</t>
+          <t>google redesign/office/android small trace journal bl</t>
         </is>
       </c>
       <c r="B335" t="inlineStr"/>
@@ -4157,7 +4173,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>google redesign/office/google sustainable pencil pouch</t>
+          <t>google redesign/office/google appeel journal red</t>
         </is>
       </c>
       <c r="B336" t="inlineStr"/>
@@ -4165,7 +4181,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable journal</t>
+          <t>google redesign/office/google black cork journal</t>
         </is>
       </c>
       <c r="B337" t="inlineStr"/>
@@ -4173,7 +4189,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable pen</t>
+          <t>google redesign/office/google clear pen 4pack</t>
         </is>
       </c>
       <c r="B338" t="inlineStr"/>
@@ -4181,7 +4197,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>google redesign/office/notebooks journals</t>
+          <t>google redesign/office/google cork journal</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
@@ -4189,7 +4205,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>google redesign/office/stickers</t>
+          <t>google redesign/office/google cork pencil pouch</t>
         </is>
       </c>
       <c r="B340" t="inlineStr"/>
@@ -4197,7 +4213,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>google redesign/office/writing</t>
+          <t>google redesign/office/google felt refillable journal</t>
         </is>
       </c>
       <c r="B341" t="inlineStr"/>
@@ -4205,7 +4221,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/office/google google campus bike grid task pad</t>
         </is>
       </c>
       <c r="B342" t="inlineStr"/>
@@ -4213,7 +4229,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/android</t>
+          <t>google redesign/office/google google color block notebook</t>
         </is>
       </c>
       <c r="B343" t="inlineStr"/>
@@ -4221,7 +4237,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google</t>
+          <t>google redesign/office/google google confetti pen white</t>
         </is>
       </c>
       <c r="B344" t="inlineStr"/>
@@ -4229,7 +4245,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google cloud</t>
+          <t>google redesign/office/google google confetti slim task pad</t>
         </is>
       </c>
       <c r="B345" t="inlineStr"/>
@@ -4237,7 +4253,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/i am remarkable</t>
+          <t>google redesign/office/google google confetti task pad</t>
         </is>
       </c>
       <c r="B346" t="inlineStr"/>
@@ -4245,7 +4261,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/youtube</t>
+          <t>google redesign/office/google light up pen blue</t>
         </is>
       </c>
       <c r="B347" t="inlineStr"/>
@@ -4253,7 +4269,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>google redesign/small goods/daddy works at google book</t>
+          <t>google redesign/office/google light up pen green</t>
         </is>
       </c>
       <c r="B348" t="inlineStr"/>
@@ -4261,7 +4277,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>google redesign/small goods/mommy works at google book</t>
+          <t>google redesign/office/google light up pen red</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
@@ -4269,7 +4285,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/office/google mural notebook</t>
         </is>
       </c>
       <c r="B350" t="inlineStr"/>
@@ -4277,7 +4293,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>google redesign/stationery/android jotter task pad</t>
+          <t>google redesign/office/google mural sticky note pad</t>
         </is>
       </c>
       <c r="B351" t="inlineStr"/>
@@ -4285,7 +4301,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google 4in decal</t>
+          <t>google redesign/office/google pen bright blue</t>
         </is>
       </c>
       <c r="B352" t="inlineStr"/>
@@ -4293,7 +4309,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google cloud pen</t>
+          <t>google redesign/office/google pen citron</t>
         </is>
       </c>
       <c r="B353" t="inlineStr"/>
@@ -4301,7 +4317,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google jotter task pad</t>
+          <t>google redesign/office/google pen grass green</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
@@ -4309,7 +4325,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google land and sea journal set</t>
+          <t>google redesign/office/google pen grey</t>
         </is>
       </c>
       <c r="B355" t="inlineStr"/>
@@ -4317,7 +4333,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>google redesign/stationery/notebooks</t>
+          <t>google redesign/office/google pen lilac</t>
         </is>
       </c>
       <c r="B356" t="inlineStr"/>
@@ -4325,7 +4341,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>google redesign/stationery/stickers</t>
+          <t>google redesign/office/google pen neon coral</t>
         </is>
       </c>
       <c r="B357" t="inlineStr"/>
@@ -4333,7 +4349,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>google redesign/stationery/writing</t>
+          <t>google redesign/office/google pen red</t>
         </is>
       </c>
       <c r="B358" t="inlineStr"/>
@@ -4341,7 +4357,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>google redesign/stationery/youtube jotter task pad</t>
+          <t>google redesign/office/google pen white</t>
         </is>
       </c>
       <c r="B359" t="inlineStr"/>
@@ -4349,7 +4365,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>google redesign/office/google phone stand bamboo</t>
         </is>
       </c>
       <c r="B360" t="inlineStr"/>
@@ -4357,7 +4373,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>google redesign/wearables/men s t-shirts</t>
+          <t>google redesign/office/google recycled notebook set natural</t>
         </is>
       </c>
       <c r="B361" t="inlineStr"/>
@@ -4365,7 +4381,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle/mural food container</t>
+          <t>google redesign/office/google recycled pen black</t>
         </is>
       </c>
       <c r="B362" t="inlineStr"/>
@@ -4373,7 +4389,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel/google tee yellow</t>
+          <t>google redesign/office/google recycled pen green</t>
         </is>
       </c>
       <c r="B363" t="inlineStr"/>
@@ -4381,7 +4397,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>google redesign/office/google recycled writing set</t>
         </is>
       </c>
       <c r="B364" t="inlineStr"/>
@@ -4389,7 +4405,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>google redesign/office/google small standard journal navy</t>
         </is>
       </c>
       <c r="B365" t="inlineStr"/>
@@ -4397,7 +4413,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>google redesign/office/google soft modal scarf</t>
         </is>
       </c>
       <c r="B366" t="inlineStr"/>
@@ -4405,7 +4421,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>google redesign/office/google sustainable pencil pouch</t>
         </is>
       </c>
       <c r="B367" t="inlineStr"/>
@@ -4413,7 +4429,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>google redesign/office/iamremarkable journal</t>
         </is>
       </c>
       <c r="B368" t="inlineStr"/>
@@ -4421,7 +4437,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
+          <t>google redesign/office/iamremarkable pen</t>
         </is>
       </c>
       <c r="B369" t="inlineStr"/>
@@ -4429,7 +4445,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
+          <t>google redesign/office/notebooks journals</t>
         </is>
       </c>
       <c r="B370" t="inlineStr"/>
@@ -4437,7 +4453,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
+          <t>google redesign/office/stickers</t>
         </is>
       </c>
       <c r="B371" t="inlineStr"/>
@@ -4445,7 +4461,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
+          <t>google redesign/office/writing</t>
         </is>
       </c>
       <c r="B372" t="inlineStr"/>
@@ -4453,7 +4469,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B373" t="inlineStr"/>
@@ -4461,7 +4477,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>google redesign/shop by brand/android</t>
         </is>
       </c>
       <c r="B374" t="inlineStr"/>
@@ -4469,7 +4485,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>google redesign/shop by brand/google</t>
         </is>
       </c>
       <c r="B375" t="inlineStr"/>
@@ -4477,10 +4493,258 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
+          <t>google redesign/shop by brand/google cloud</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr"/>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>google redesign/shop by brand/i am remarkable</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr"/>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>google redesign/shop by brand/youtube</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr"/>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>google redesign/small goods/daddy works at google book</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr"/>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>google redesign/small goods/mommy works at google book</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr"/>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>google redesign/stationery</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr"/>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/android jotter task pad</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr"/>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/google 4in decal</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/google cloud pen</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/google jotter task pad</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/google land and sea journal set</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/notebooks</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/stickers</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/writing</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>google redesign/stationery/youtube jotter task pad</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr"/>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>google redesign/super g unisex joggers</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr"/>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>google redesign/wearables/men s t-shirts</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr"/>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>google rmg redesign/lifestyle/mural food container</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr"/>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>google yellowesign/apparel/google tee yellow</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr"/>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr"/>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>payment method</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr"/>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>shopping cart</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr"/>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>store search results</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr"/>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>store-policies/frequently-asked-questions</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr"/>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>store-policies/privacy-policy</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr"/>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>store-policies/return-policy</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr"/>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>store-policies/shipping-information</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr"/>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>store-policies/terms-of-use</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr"/>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>the google merchandise store - log in</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr"/>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>the google merchandise store - my account</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr"/>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>the google merchandise store - register</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr"/>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
           <t>your wishlist</t>
         </is>
       </c>
-      <c r="B376" t="inlineStr"/>
+      <c r="B407" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5734,7 +5998,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5917,10 +6181,18 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Smartphone - Edge</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>Xiaomi - Mi 11</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
+      <c r="B23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added functions for data prep to data functions. trying f2
</commit_message>
<xml_diff>
--- a/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
+++ b/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
@@ -808,7 +808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -839,7 +839,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>black lives matter | google merchandise store</t>
+          <t>checkout confirmation</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -847,7 +847,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
+          <t>checkout review</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -855,7 +855,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout review</t>
+          <t>checkout your information</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -863,7 +863,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout your information</t>
+          <t>clearance</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -871,7 +871,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>clearance</t>
+          <t>google greenesign</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -879,7 +879,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>google greenesign</t>
+          <t>google merchandise store - forgot password</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -887,7 +887,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
+          <t>google merchandise store - reset password</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -895,7 +895,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
+          <t>google online store</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -903,7 +903,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google online store</t>
+          <t>google redesign</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -911,7 +911,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign</t>
+          <t>google rmg redesign</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -919,7 +919,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google rmg redesign</t>
+          <t>google yellowesign</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -927,7 +927,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google yellowesign</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -935,7 +935,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -943,7 +943,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -951,7 +951,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -959,7 +959,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>store-policies</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -967,7 +967,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>store-policies</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -975,7 +975,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -983,7 +983,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>the google merchandise store - register</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -991,18 +991,10 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>your wishlist</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>your wishlist</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1015,7 +1007,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B55"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1054,7 +1046,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>black lives matter | google merchandise store</t>
+          <t>checkout confirmation</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -1062,7 +1054,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
+          <t>checkout review</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -1070,7 +1062,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout review</t>
+          <t>checkout your information</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -1078,7 +1070,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>checkout your information</t>
+          <t>clearance/clearance-accessories</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -1086,7 +1078,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>clearance/clearance-accessories</t>
+          <t>google greenesign/apparel</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -1094,7 +1086,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google greenesign/apparel</t>
+          <t>google merchandise store - forgot password</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -1102,7 +1094,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
+          <t>google merchandise store - reset password</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -1110,7 +1102,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
+          <t>google online store</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1118,7 +1110,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google online store</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1126,7 +1118,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1134,7 +1126,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/apparelgoogle beekeepers onesie pink</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1262,7 +1254,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1270,7 +1262,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1278,7 +1270,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1286,7 +1278,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/notebooks journals</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1294,7 +1286,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1302,7 +1294,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1310,7 +1302,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/small goods</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1318,7 +1310,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/small goods</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1326,7 +1318,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1334,7 +1326,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>google redesign/wearables</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1342,7 +1334,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/wearables</t>
+          <t>google rmg redesign/lifestyle</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1350,7 +1342,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle</t>
+          <t>google yellowesign/apparel</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1358,7 +1350,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1366,7 +1358,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1374,7 +1366,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1382,7 +1374,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1390,7 +1382,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1398,7 +1390,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>store-policies/privacy-policy</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1406,7 +1398,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
+          <t>store-policies/return-policy</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1414,7 +1406,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
+          <t>store-policies/shipping-information</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1422,7 +1414,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
+          <t>store-policies/terms-of-use</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1430,7 +1422,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1438,7 +1430,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1446,7 +1438,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>the google merchandise store - register</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1454,18 +1446,10 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>your wishlist</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>your wishlist</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1478,7 +1462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B407"/>
+  <dimension ref="A1:B385"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1517,7 +1501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>black lives matter | google merchandise store</t>
+          <t>checkout confirmation</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -1525,7 +1509,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
+          <t>checkout review</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -1533,7 +1517,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout review</t>
+          <t>checkout your information</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -1541,7 +1525,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>checkout your information</t>
+          <t>clearance/clearance-accessories</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -1549,7 +1533,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>clearance/clearance-accessories</t>
+          <t>google greenesign/apparel/google tee green</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -1557,7 +1541,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>google greenesign/apparel/google tee green</t>
+          <t>google merchandise store - forgot password</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -1565,7 +1549,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>google merchandise store - forgot password</t>
+          <t>google merchandise store - reset password</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -1573,7 +1557,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>google merchandise store - reset password</t>
+          <t>google online store</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -1581,7 +1565,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google online store</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1589,7 +1573,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google redesign/accessories/android iconic sticker sheet</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1597,7 +1581,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android iconic 4in decal</t>
+          <t>google redesign/accessories/android large removable sticker sheet</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1605,7 +1589,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android iconic pin</t>
+          <t>google redesign/accessories/android puzzlebot v2</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1613,7 +1597,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android large removable sticker sheet</t>
+          <t>google redesign/accessories/android sm sticker sheet</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1621,7 +1605,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android lumberjack pin</t>
+          <t>google redesign/accessories/android super hero 3d framed art</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1629,7 +1613,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android puzzlebot v2</t>
+          <t>google redesign/accessories/android techie 3d framed art</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1637,7 +1621,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android sm sticker sheet</t>
+          <t>google redesign/accessories/fun</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1645,7 +1629,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android super hero 3d framed art</t>
+          <t>google redesign/accessories/google blue yoyo</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1653,7 +1637,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android techie 3d framed art</t>
+          <t>google redesign/accessories/google bot</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -1661,7 +1645,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>google redesign/accessories/fun</t>
+          <t>google redesign/accessories/google bot multicolored</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1669,7 +1653,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google blue yoyo</t>
+          <t>google redesign/accessories/google campus bike</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1677,7 +1661,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google bot</t>
+          <t>google redesign/accessories/google chrome dinosaur collectible</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1685,7 +1669,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google bot multicolored</t>
+          <t>google redesign/accessories/google clear framed blue shades</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1693,7 +1677,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google campus bike</t>
+          <t>google redesign/accessories/google clear framed gray shades</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1701,7 +1685,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google chrome dinosaur collectible</t>
+          <t>google redesign/accessories/google clear framed yellow shades</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1709,7 +1693,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed blue shades</t>
+          <t>google redesign/accessories/google cloth pouch black</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1717,7 +1701,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed gray shades</t>
+          <t>google redesign/accessories/google cork card holder</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1725,7 +1709,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed yellow shades</t>
+          <t>google redesign/accessories/google cork key ring</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1733,7 +1717,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cloth pouch black</t>
+          <t>google redesign/accessories/google cork passport holder</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1741,7 +1725,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork card holder</t>
+          <t>google redesign/accessories/google cork tablet case</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1749,7 +1733,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork passport holder</t>
+          <t>google redesign/accessories/google emoji magnet set</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1757,7 +1741,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork tablet case</t>
+          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1765,7 +1749,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji magnet set</t>
+          <t>google redesign/accessories/google felt luggage tag</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1773,7 +1757,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
+          <t>google redesign/accessories/google felt strap keyring</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1781,7 +1765,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt luggage tag</t>
+          <t>google redesign/accessories/google inverted umbrella</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1789,7 +1773,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt strap keyring</t>
+          <t>google redesign/accessories/google keychain 19</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1797,7 +1781,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google inverted umbrella</t>
+          <t>google redesign/accessories/google lapel pin</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1805,7 +1789,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google keychain 19</t>
+          <t>google redesign/accessories/google laptop sleeve charcoal</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1813,7 +1797,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lapel pin</t>
+          <t>google redesign/accessories/google lovehandle black</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1821,7 +1805,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google laptop sleeve charcoal</t>
+          <t>google redesign/accessories/google magnet</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1829,7 +1813,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google large pet collar blue green</t>
+          <t>google redesign/accessories/google maps pin</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1837,7 +1821,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google large pet leash red yellow</t>
+          <t>google redesign/accessories/google medium pet collar blue green</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1845,7 +1829,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lovehandle black</t>
+          <t>google redesign/accessories/google medium pet leash blue green</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1853,7 +1837,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google magnet</t>
+          <t>google redesign/accessories/google mouse pad navy</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1861,7 +1845,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google maps pin</t>
+          <t>google redesign/accessories/google mural sticker sheet</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1869,7 +1853,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google medium pet collar blue green</t>
+          <t>google redesign/accessories/google nyc campus lapel pin</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1877,7 +1861,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mouse pad navy</t>
+          <t>google redesign/accessories/google pnw campus sticker</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1885,7 +1869,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mural sticker sheet</t>
+          <t>google redesign/accessories/google pride sticker</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1893,7 +1877,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google nyc campus lapel pin</t>
+          <t>google redesign/accessories/google seattle campus lapel pin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1901,7 +1885,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google nyc campus sticker</t>
+          <t>google redesign/accessories/google see no hear no set</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1909,7 +1893,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google pride sticker</t>
+          <t>google redesign/accessories/google small cable organizer blue</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1917,7 +1901,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google see no hear no set</t>
+          <t>google redesign/accessories/google tech taco</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1925,7 +1909,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google sf campus lapel pin</t>
+          <t>google redesign/accessories/google utensil set</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1933,7 +1917,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google small cable organizer blue</t>
+          <t>google redesign/accessories/google yellow yoyo</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1941,7 +1925,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google tech taco</t>
+          <t>google redesign/accessories/iamremarkable lapel pin</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1949,7 +1933,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google utensil set</t>
+          <t>google redesign/accessories/noogler android figure 2019</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1957,7 +1941,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google yellow yoyo</t>
+          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1965,7 +1949,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>google redesign/accessories/iamremarkable lapel pin</t>
+          <t>google redesign/accessories/youtube iconic play pin</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1973,7 +1957,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>google redesign/accessories/noogler android figure 2019</t>
+          <t>google redesign/accessories/youtube small sticker sheet</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1981,7 +1965,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1989,7 +1973,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube iconic play pin</t>
+          <t>google redesign/apparel/android garden tee orange</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1997,7 +1981,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube small sticker sheet</t>
+          <t>google redesign/apparel/android iconic beanie</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -2005,7 +1989,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/apparel/android iconic crew</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -2013,7 +1997,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android garden tee orange</t>
+          <t>google redesign/apparel/android iconic hat green</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -2021,7 +2005,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic beanie</t>
+          <t>google redesign/apparel/android iconic hat v2 black</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -2029,7 +2013,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic crew</t>
+          <t>google redesign/apparel/android iconic hat white</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -2037,7 +2021,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat green</t>
+          <t>google redesign/apparel/android iconic sock</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -2045,7 +2029,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat v2 black</t>
+          <t>google redesign/apparel/android pocket onesie navy</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2053,7 +2037,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat white</t>
+          <t>google redesign/apparel/android pocket onesie white</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2061,7 +2045,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic sock</t>
+          <t>google redesign/apparel/android pocket tee green</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -2069,7 +2053,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie navy</t>
+          <t>google redesign/apparel/android pocket tee navy</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -2077,7 +2061,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie white</t>
+          <t>google redesign/apparel/android pocket toddler tee navy</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -2085,7 +2069,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee green</t>
+          <t>google redesign/apparel/android pocket toddler tee white</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2093,7 +2077,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee navy</t>
+          <t>google redesign/apparel/android pocket youth tee green</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2101,7 +2085,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee navy</t>
+          <t>google redesign/apparel/android pocket youth tee navy</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -2109,7 +2093,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee white</t>
+          <t>google redesign/apparel/flamingo and friends tee blue</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -2117,7 +2101,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee green</t>
+          <t>google redesign/apparel/google austin campus unisex tee</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -2125,7 +2109,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee navy</t>
+          <t>google redesign/apparel/google austin campus zip hoodie</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -2133,7 +2117,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>google redesign/apparel/flamingo and friends tee blue</t>
+          <t>google redesign/apparel/google badge heavyweight pullover black</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -2141,7 +2125,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus unisex tee</t>
+          <t>google redesign/apparel/google black cloud zip hoodie</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -2149,7 +2133,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus zip hoodie</t>
+          <t>google redesign/apparel/google black tee</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -2157,7 +2141,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google badge heavyweight pullover black</t>
+          <t>google redesign/apparel/google boulder campus unisex tee</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -2165,7 +2149,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black cloud zip hoodie</t>
+          <t>google redesign/apparel/google boulder campus zip hoodie</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2173,7 +2157,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black tee</t>
+          <t>google redesign/apparel/google cambridge campus unisex tee</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2181,7 +2165,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google boulder campus unisex tee</t>
+          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -2189,7 +2173,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google boulder campus zip hoodie</t>
+          <t>google redesign/apparel/google campus bike eco tee navy</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -2197,7 +2181,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus ladies tee</t>
+          <t>google redesign/apparel/google chicago campus unisex tee</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2205,7 +2189,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus unisex tee</t>
+          <t>google redesign/apparel/google chicago campus zip hoodie</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2213,7 +2197,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
+          <t>google redesign/apparel/google cotopaxi shell</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2221,7 +2205,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google campus bike eco tee navy</t>
+          <t>google redesign/apparel/google crew grey</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -2229,7 +2213,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus unisex tee</t>
+          <t>google redesign/apparel/google crew socks</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -2237,7 +2221,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus zip hoodie</t>
+          <t>google redesign/apparel/google crewneck sweatshirt green</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -2245,7 +2229,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cotopaxi shell</t>
+          <t>google redesign/apparel/google dino game tee</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2253,7 +2237,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew grey</t>
+          <t>google redesign/apparel/google fc longsleeve ash</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2261,7 +2245,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew socks</t>
+          <t>google redesign/apparel/google fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -2269,7 +2253,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crewneck sweatshirt green</t>
+          <t>google redesign/apparel/google google crew combed cotton sock</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -2277,7 +2261,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google dino game tee</t>
+          <t>google redesign/apparel/google google crew striped athletic sock</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -2285,7 +2269,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve ash</t>
+          <t>google redesign/apparel/google google kids playful tee</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -2293,7 +2277,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google google premium sunglasses</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2301,7 +2285,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google blue kids sunglasses</t>
+          <t>google redesign/apparel/google google red kids sunglasses</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -2309,7 +2293,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew combed cotton sock</t>
+          <t>google redesign/apparel/google google summer19 crew grey</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -2317,7 +2301,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew striped athletic sock</t>
+          <t>google redesign/apparel/google grey tee</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -2325,7 +2309,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google kids playful tee</t>
+          <t>google redesign/apparel/google heather green speckled tee</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2333,7 +2317,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google premium sunglasses</t>
+          <t>google redesign/apparel/google heathered pom beanie</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2341,7 +2325,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google red kids sunglasses</t>
+          <t>google redesign/apparel/google infant charcoal onesie</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -2349,7 +2333,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google summer19 crew grey</t>
+          <t>google redesign/apparel/google infant hero onesie grey</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -2357,7 +2341,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google grey tee</t>
+          <t>google redesign/apparel/google infant hero tee olive</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -2365,7 +2349,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heather green speckled tee</t>
+          <t>google redesign/apparel/google kirkland campus unisex tee</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -2373,7 +2357,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heathered pom beanie</t>
+          <t>google redesign/apparel/google la campus unisex tee</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -2381,7 +2365,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant charcoal onesie</t>
+          <t>google redesign/apparel/google la campus zip hoodie</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -2389,7 +2373,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero onesie grey</t>
+          <t>google redesign/apparel/google land and sea cotton cap ls</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -2397,7 +2381,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero tee olive</t>
+          <t>google redesign/apparel/google land and sea unisex tee</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -2405,7 +2389,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google kirkland campus unisex tee</t>
+          <t>google redesign/apparel/google land and sea womens eco tee</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -2413,7 +2397,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus unisex tee</t>
+          <t>google redesign/apparel/google leather strap hat black</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -2421,7 +2405,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus zip hoodie</t>
+          <t>google redesign/apparel/google leather strap hat blue</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -2429,7 +2413,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea cotton cap ls</t>
+          <t>google redesign/apparel/google mens discovery lt rain shell</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -2437,7 +2421,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea unisex tee</t>
+          <t>google redesign/apparel/google mens microfleece jacket black</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -2445,7 +2429,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea womens eco tee</t>
+          <t>google redesign/apparel/google mens puff jacket black</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -2453,7 +2437,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat black</t>
+          <t>google redesign/apparel/google mens softshell moss</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -2461,7 +2445,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat blue</t>
+          <t>google redesign/apparel/google mens tech fleece grey</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -2469,7 +2453,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens discovery lt rain shell</t>
+          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -2477,7 +2461,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens microfleece jacket black</t>
+          <t>google redesign/apparel/google mountain view tee blue</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -2485,7 +2469,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens puff jacket black</t>
+          <t>google redesign/apparel/google mountain view tee red</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -2493,7 +2477,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens softshell moss</t>
+          <t>google redesign/apparel/google mural socks</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -2501,7 +2485,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece grey</t>
+          <t>google redesign/apparel/google navy speckled tee</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -2509,7 +2493,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google nyc campus ladies tee</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -2517,7 +2501,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee blue</t>
+          <t>google redesign/apparel/google nyc campus unisex tee</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -2525,7 +2509,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee red</t>
+          <t>google redesign/apparel/google nyc campus zip hoodie</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -2533,7 +2517,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mural socks</t>
+          <t>google redesign/apparel/google pnw campus unisex tee</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -2541,7 +2525,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google navy speckled tee</t>
+          <t>google redesign/apparel/google pnw campus zip hoodie</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
@@ -2549,7 +2533,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus ladies tee</t>
+          <t>google redesign/apparel/google raincoat navy</t>
         </is>
       </c>
       <c r="B133" t="inlineStr"/>
@@ -2557,7 +2541,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus unisex tee</t>
+          <t>google redesign/apparel/google red speckled tee</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -2565,7 +2549,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus zip hoodie</t>
+          <t>google redesign/apparel/google sf campus ladies tee</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
@@ -2573,7 +2557,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus unisex tee</t>
+          <t>google redesign/apparel/google sf campus unisex tee</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -2581,7 +2565,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus zip hoodie</t>
+          <t>google redesign/apparel/google sf campus zip hoodie</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -2589,7 +2573,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google raincoat navy</t>
+          <t>google redesign/apparel/google sherpa vest black</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -2597,7 +2581,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google red speckled tee</t>
+          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
@@ -2605,7 +2589,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google seattle campus unisex tee</t>
+          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -2613,7 +2597,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus ladies tee</t>
+          <t>google redesign/apparel/google speckled beanie grey</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -2621,7 +2605,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus unisex tee</t>
+          <t>google redesign/apparel/google speckled beanie navy</t>
         </is>
       </c>
       <c r="B142" t="inlineStr"/>
@@ -2629,7 +2613,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus zip hoodie</t>
+          <t>google redesign/apparel/google split seam tee olive</t>
         </is>
       </c>
       <c r="B143" t="inlineStr"/>
@@ -2637,7 +2621,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa vest black</t>
+          <t>google redesign/apparel/google tee blue</t>
         </is>
       </c>
       <c r="B144" t="inlineStr"/>
@@ -2645,7 +2629,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
+          <t>google redesign/apparel/google tee dark blue</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -2653,7 +2637,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
+          <t>google redesign/apparel/google tee fc black</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -2661,7 +2645,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie grey</t>
+          <t>google redesign/apparel/google tee mint green</t>
         </is>
       </c>
       <c r="B147" t="inlineStr"/>
@@ -2669,7 +2653,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie navy</t>
+          <t>google redesign/apparel/google tee red</t>
         </is>
       </c>
       <c r="B148" t="inlineStr"/>
@@ -2677,7 +2661,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google split seam tee olive</t>
+          <t>google redesign/apparel/google toddler fc tee charcoal</t>
         </is>
       </c>
       <c r="B149" t="inlineStr"/>
@@ -2685,7 +2669,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee blue</t>
+          <t>google redesign/apparel/google toddler fc zip hoodie</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
@@ -2693,7 +2677,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee dark blue</t>
+          <t>google redesign/apparel/google toddler hero tee black</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -2701,7 +2685,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee fc black</t>
+          <t>google redesign/apparel/google toddler hero tee olive</t>
         </is>
       </c>
       <c r="B152" t="inlineStr"/>
@@ -2709,7 +2693,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee mint green</t>
+          <t>google redesign/apparel/google toddler tee white</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
@@ -2717,7 +2701,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee red</t>
+          <t>google redesign/apparel/google tonal tee coral</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -2725,7 +2709,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc tee charcoal</t>
+          <t>google redesign/apparel/google tonal tee spearmint</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
@@ -2733,7 +2717,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc zip hoodie</t>
+          <t>google redesign/apparel/google tracking hat</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -2741,7 +2725,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee black</t>
+          <t>google redesign/apparel/google tudes recycled tee</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
@@ -2749,7 +2733,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee olive</t>
+          <t>google redesign/apparel/google twill cap charcoal</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
@@ -2757,7 +2741,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler tee white</t>
+          <t>google redesign/apparel/google unisex eco tee black</t>
         </is>
       </c>
       <c r="B159" t="inlineStr"/>
@@ -2765,7 +2749,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee coral</t>
+          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
@@ -2773,7 +2757,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee spearmint</t>
+          <t>google redesign/apparel/google unisex google pocket tee grey</t>
         </is>
       </c>
       <c r="B161" t="inlineStr"/>
@@ -2781,7 +2765,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tracking hat</t>
+          <t>google redesign/apparel/google unisex pride eco-tee black</t>
         </is>
       </c>
       <c r="B162" t="inlineStr"/>
@@ -2789,7 +2773,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tudes recycled tee</t>
+          <t>google redesign/apparel/google womens black tee</t>
         </is>
       </c>
       <c r="B163" t="inlineStr"/>
@@ -2797,7 +2781,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google twill cap charcoal</t>
+          <t>google redesign/apparel/google womens discovery</t>
         </is>
       </c>
       <c r="B164" t="inlineStr"/>
@@ -2805,7 +2789,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex eco tee black</t>
+          <t>google redesign/apparel/google womens eco tee black</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -2813,7 +2797,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
+          <t>google redesign/apparel/google womens google striped ls</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
@@ -2821,7 +2805,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google pocket tee grey</t>
+          <t>google redesign/apparel/google womens grid zip up</t>
         </is>
       </c>
       <c r="B167" t="inlineStr"/>
@@ -2829,7 +2813,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex pride eco-tee black</t>
+          <t>google redesign/apparel/google womens kirkland pullover</t>
         </is>
       </c>
       <c r="B168" t="inlineStr"/>
@@ -2837,7 +2821,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens black tee</t>
+          <t>google redesign/apparel/google womens microfleece jacket black</t>
         </is>
       </c>
       <c r="B169" t="inlineStr"/>
@@ -2845,7 +2829,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens discovery</t>
+          <t>google redesign/apparel/google womens pride eco-tee black</t>
         </is>
       </c>
       <c r="B170" t="inlineStr"/>
@@ -2853,7 +2837,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens eco tee black</t>
+          <t>google redesign/apparel/google womens puff jacket black</t>
         </is>
       </c>
       <c r="B171" t="inlineStr"/>
@@ -2861,7 +2845,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens google striped ls</t>
+          <t>google redesign/apparel/google womens softshell moss</t>
         </is>
       </c>
       <c r="B172" t="inlineStr"/>
@@ -2869,7 +2853,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens grid zip up</t>
+          <t>google redesign/apparel/google womens tech fleece grey</t>
         </is>
       </c>
       <c r="B173" t="inlineStr"/>
@@ -2877,7 +2861,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens kirkland pullover</t>
+          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B174" t="inlineStr"/>
@@ -2885,7 +2869,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens microfleece jacket black</t>
+          <t>google redesign/apparel/google youth badge tee navy</t>
         </is>
       </c>
       <c r="B175" t="inlineStr"/>
@@ -2893,7 +2877,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens pride eco-tee black</t>
+          <t>google redesign/apparel/google youth badge tee olive</t>
         </is>
       </c>
       <c r="B176" t="inlineStr"/>
@@ -2901,7 +2885,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens puff jacket black</t>
+          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B177" t="inlineStr"/>
@@ -2909,7 +2893,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens softshell moss</t>
+          <t>google redesign/apparel/google youth fc pullover hoodie</t>
         </is>
       </c>
       <c r="B178" t="inlineStr"/>
@@ -2917,7 +2901,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece grey</t>
+          <t>google redesign/apparel/google youth fc tee charcoal</t>
         </is>
       </c>
       <c r="B179" t="inlineStr"/>
@@ -2925,7 +2909,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google youth fc zip hoodie</t>
         </is>
       </c>
       <c r="B180" t="inlineStr"/>
@@ -2933,7 +2917,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee navy</t>
+          <t>google redesign/apparel/google youth hero tee grey</t>
         </is>
       </c>
       <c r="B181" t="inlineStr"/>
@@ -2941,7 +2925,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee olive</t>
+          <t>google redesign/apparel/google youth hero tee maroon</t>
         </is>
       </c>
       <c r="B182" t="inlineStr"/>
@@ -2949,7 +2933,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google youth jumbo print tee white</t>
         </is>
       </c>
       <c r="B183" t="inlineStr"/>
@@ -2957,7 +2941,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc pullover hoodie</t>
+          <t>google redesign/apparel/google zip hoodie fc</t>
         </is>
       </c>
       <c r="B184" t="inlineStr"/>
@@ -2965,7 +2949,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc tee charcoal</t>
+          <t>google redesign/apparel/hats</t>
         </is>
       </c>
       <c r="B185" t="inlineStr"/>
@@ -2973,7 +2957,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc zip hoodie</t>
+          <t>google redesign/apparel/iamremarkable hoodie</t>
         </is>
       </c>
       <c r="B186" t="inlineStr"/>
@@ -2981,7 +2965,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee grey</t>
+          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
         </is>
       </c>
       <c r="B187" t="inlineStr"/>
@@ -2989,7 +2973,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee maroon</t>
+          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
         </is>
       </c>
       <c r="B188" t="inlineStr"/>
@@ -2997,7 +2981,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth jumbo print tee white</t>
+          <t>google redesign/apparel/kids</t>
         </is>
       </c>
       <c r="B189" t="inlineStr"/>
@@ -3005,7 +2989,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google zip hoodie fc</t>
+          <t>google redesign/apparel/mens</t>
         </is>
       </c>
       <c r="B190" t="inlineStr"/>
@@ -3013,7 +2997,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>google redesign/apparel/hats</t>
+          <t>google redesign/apparel/socks</t>
         </is>
       </c>
       <c r="B191" t="inlineStr"/>
@@ -3021,7 +3005,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable hoodie</t>
+          <t>google redesign/apparel/stan and friends onesie green</t>
         </is>
       </c>
       <c r="B192" t="inlineStr"/>
@@ -3029,7 +3013,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
+          <t>google redesign/apparel/stan and friends tee green</t>
         </is>
       </c>
       <c r="B193" t="inlineStr"/>
@@ -3037,7 +3021,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
+          <t>google redesign/apparel/womens</t>
         </is>
       </c>
       <c r="B194" t="inlineStr"/>
@@ -3045,7 +3029,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>google redesign/apparel/kids</t>
+          <t>google redesign/apparel/youtube crew socks</t>
         </is>
       </c>
       <c r="B195" t="inlineStr"/>
@@ -3053,7 +3037,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>google redesign/apparel/mens</t>
+          <t>google redesign/apparel/youtube favorite tee white</t>
         </is>
       </c>
       <c r="B196" t="inlineStr"/>
@@ -3061,7 +3045,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>google redesign/apparel/socks</t>
+          <t>google redesign/apparel/youtube icon hoodie black</t>
         </is>
       </c>
       <c r="B197" t="inlineStr"/>
@@ -3069,7 +3053,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends onesie green</t>
+          <t>google redesign/apparel/youtube icon tee charcoal</t>
         </is>
       </c>
       <c r="B198" t="inlineStr"/>
@@ -3077,7 +3061,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends tee green</t>
+          <t>google redesign/apparel/youtube icon tee grey</t>
         </is>
       </c>
       <c r="B199" t="inlineStr"/>
@@ -3085,7 +3069,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends toddler tee green</t>
+          <t>google redesign/apparel/youtube leather strap hat black</t>
         </is>
       </c>
       <c r="B200" t="inlineStr"/>
@@ -3093,7 +3077,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends youth tee green</t>
+          <t>google redesign/apparel/youtube standards zip hoodie black</t>
         </is>
       </c>
       <c r="B201" t="inlineStr"/>
@@ -3101,7 +3085,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>google redesign/apparel/womens</t>
+          <t>google redesign/apparel/youtube transmission journal red</t>
         </is>
       </c>
       <c r="B202" t="inlineStr"/>
@@ -3109,7 +3093,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube crew socks</t>
+          <t>google redesign/apparel/youtube twill cap sandwich black</t>
         </is>
       </c>
       <c r="B203" t="inlineStr"/>
@@ -3117,7 +3101,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube favorite tee white</t>
+          <t>google redesign/apparelgoogle beekeepers onesie pink</t>
         </is>
       </c>
       <c r="B204" t="inlineStr"/>
@@ -3125,7 +3109,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon hoodie black</t>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
         </is>
       </c>
       <c r="B205" t="inlineStr"/>
@@ -3133,7 +3117,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee charcoal</t>
+          <t>google redesign/bags/android iconic backpack</t>
         </is>
       </c>
       <c r="B206" t="inlineStr"/>
@@ -3141,7 +3125,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee grey</t>
+          <t>google redesign/bags/backpacks</t>
         </is>
       </c>
       <c r="B207" t="inlineStr"/>
@@ -3149,7 +3133,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube leather strap hat black</t>
+          <t>google redesign/bags/essential canvas tote</t>
         </is>
       </c>
       <c r="B208" t="inlineStr"/>
@@ -3157,7 +3141,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube standards zip hoodie black</t>
+          <t>google redesign/bags/google bike mini backpack</t>
         </is>
       </c>
       <c r="B209" t="inlineStr"/>
@@ -3165,7 +3149,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube transmission journal red</t>
+          <t>google redesign/bags/google flat front bag grey</t>
         </is>
       </c>
       <c r="B210" t="inlineStr"/>
@@ -3173,7 +3157,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube twill cap sandwich black</t>
+          <t>google redesign/bags/google google campus bike carry pouch</t>
         </is>
       </c>
       <c r="B211" t="inlineStr"/>
@@ -3181,7 +3165,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+          <t>google redesign/bags/google google campus bike tote navy</t>
         </is>
       </c>
       <c r="B212" t="inlineStr"/>
@@ -3189,7 +3173,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>google redesign/bags/android iconic backpack</t>
+          <t>google redesign/bags/google google confetti accessory pouch</t>
         </is>
       </c>
       <c r="B213" t="inlineStr"/>
@@ -3197,7 +3181,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>google redesign/bags/backpacks</t>
+          <t>google redesign/bags/google google striped penny pouch</t>
         </is>
       </c>
       <c r="B214" t="inlineStr"/>
@@ -3205,7 +3189,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>google redesign/bags/essential canvas tote</t>
+          <t>google redesign/bags/google hemp tote</t>
         </is>
       </c>
       <c r="B215" t="inlineStr"/>
@@ -3213,7 +3197,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>google redesign/bags/google bike mini backpack</t>
+          <t>google redesign/bags/google incognito dopp kit v2</t>
         </is>
       </c>
       <c r="B216" t="inlineStr"/>
@@ -3221,7 +3205,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>google redesign/bags/google cambridge campus tote</t>
+          <t>google redesign/bags/google incognito flap pack</t>
         </is>
       </c>
       <c r="B217" t="inlineStr"/>
@@ -3229,7 +3213,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>google redesign/bags/google flat front bag grey</t>
+          <t>google redesign/bags/google incognito laptop organizer v2</t>
         </is>
       </c>
       <c r="B218" t="inlineStr"/>
@@ -3237,7 +3221,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google campus bike carry pouch</t>
+          <t>google redesign/bags/google incognito messenger bag</t>
         </is>
       </c>
       <c r="B219" t="inlineStr"/>
@@ -3245,7 +3229,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google campus bike tote navy</t>
+          <t>google redesign/bags/google incognito techpack v2</t>
         </is>
       </c>
       <c r="B220" t="inlineStr"/>
@@ -3253,7 +3237,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google confetti accessory pouch</t>
+          <t>google redesign/bags/google incognito zippack v2</t>
         </is>
       </c>
       <c r="B221" t="inlineStr"/>
@@ -3261,7 +3245,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google striped penny pouch</t>
+          <t>google redesign/bags/google large tote white</t>
         </is>
       </c>
       <c r="B222" t="inlineStr"/>
@@ -3269,7 +3253,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>google redesign/bags/google hemp tote</t>
+          <t>google redesign/bags/google mesh bag blue</t>
         </is>
       </c>
       <c r="B223" t="inlineStr"/>
@@ -3277,7 +3261,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito dopp kit v2</t>
+          <t>google redesign/bags/google mural tote</t>
         </is>
       </c>
       <c r="B224" t="inlineStr"/>
@@ -3285,7 +3269,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito flap pack</t>
+          <t>google redesign/bags/google packable bag black</t>
         </is>
       </c>
       <c r="B225" t="inlineStr"/>
@@ -3293,7 +3277,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito laptop organizer v2</t>
+          <t>google redesign/bags/google seaport tote</t>
         </is>
       </c>
       <c r="B226" t="inlineStr"/>
@@ -3301,7 +3285,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito messenger bag</t>
+          <t>google redesign/bags/google totepak</t>
         </is>
       </c>
       <c r="B227" t="inlineStr"/>
@@ -3309,7 +3293,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito techpack v2</t>
+          <t>google redesign/bags/google utility backpack</t>
         </is>
       </c>
       <c r="B228" t="inlineStr"/>
@@ -3317,7 +3301,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito zippack v2</t>
+          <t>google redesign/bags/google utility bag grey</t>
         </is>
       </c>
       <c r="B229" t="inlineStr"/>
@@ -3325,7 +3309,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>google redesign/bags/google large tote white</t>
+          <t>google redesign/bags/more bags</t>
         </is>
       </c>
       <c r="B230" t="inlineStr"/>
@@ -3333,7 +3317,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mesh bag blue</t>
+          <t>google redesign/bags/shopping and totes</t>
         </is>
       </c>
       <c r="B231" t="inlineStr"/>
@@ -3341,7 +3325,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mesh bag red</t>
+          <t>google redesign/bags/supernatural paper backpack</t>
         </is>
       </c>
       <c r="B232" t="inlineStr"/>
@@ -3349,7 +3333,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mural tote</t>
+          <t>google redesign/bags/supernatural paper lunch sack</t>
         </is>
       </c>
       <c r="B233" t="inlineStr"/>
@@ -3357,7 +3341,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>google redesign/bags/google packable bag black</t>
+          <t>google redesign/bags/supernatural paper tote</t>
         </is>
       </c>
       <c r="B234" t="inlineStr"/>
@@ -3365,7 +3349,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>google redesign/bags/google seaport tote</t>
+          <t>google redesign/blm unisex pullover hoodie</t>
         </is>
       </c>
       <c r="B235" t="inlineStr"/>
@@ -3373,7 +3357,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>google redesign/bags/google sf campus tote</t>
+          <t>google redesign/campus collection</t>
         </is>
       </c>
       <c r="B236" t="inlineStr"/>
@@ -3381,7 +3365,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>google redesign/bags/google totepak</t>
+          <t>google redesign/campus collection/google mountain view campus ladies tee</t>
         </is>
       </c>
       <c r="B237" t="inlineStr"/>
@@ -3389,7 +3373,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility backpack</t>
+          <t>google redesign/campus collection/google mountain view campus mug</t>
         </is>
       </c>
       <c r="B238" t="inlineStr"/>
@@ -3397,7 +3381,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility bag grey</t>
+          <t>google redesign/campus collection/google mountain view campus sticker</t>
         </is>
       </c>
       <c r="B239" t="inlineStr"/>
@@ -3405,7 +3389,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>google redesign/bags/iamremarkable tote</t>
+          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
         </is>
       </c>
       <c r="B240" t="inlineStr"/>
@@ -3413,7 +3397,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>google redesign/bags/more bags</t>
+          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
         </is>
       </c>
       <c r="B241" t="inlineStr"/>
@@ -3421,7 +3405,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>google redesign/bags/shopping and totes</t>
+          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
         </is>
       </c>
       <c r="B242" t="inlineStr"/>
@@ -3429,7 +3413,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper backpack</t>
+          <t>google redesign/campus collection/google sunnyvale campus ladies tee</t>
         </is>
       </c>
       <c r="B243" t="inlineStr"/>
@@ -3437,7 +3421,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper lunch sack</t>
+          <t>google redesign/campus collection/google sunnyvale campus mug</t>
         </is>
       </c>
       <c r="B244" t="inlineStr"/>
@@ -3445,7 +3429,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper tote</t>
+          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
         </is>
       </c>
       <c r="B245" t="inlineStr"/>
@@ -3453,7 +3437,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
+          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
         </is>
       </c>
       <c r="B246" t="inlineStr"/>
@@ -3461,7 +3445,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
+          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
         </is>
       </c>
       <c r="B247" t="inlineStr"/>
@@ -3469,7 +3453,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus mug</t>
+          <t>google redesign/clearance</t>
         </is>
       </c>
       <c r="B248" t="inlineStr"/>
@@ -3477,7 +3461,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus sticker</t>
+          <t>google redesign/drinkware/android buoy bottle</t>
         </is>
       </c>
       <c r="B249" t="inlineStr"/>
@@ -3485,7 +3469,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
+          <t>google redesign/drinkware/android iconic glass bottle green</t>
         </is>
       </c>
       <c r="B250" t="inlineStr"/>
@@ -3493,7 +3477,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
+          <t>google redesign/drinkware/android iconic mug gray</t>
         </is>
       </c>
       <c r="B251" t="inlineStr"/>
@@ -3501,7 +3485,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
+          <t>google redesign/drinkware/campus corkbase mug blue</t>
         </is>
       </c>
       <c r="B252" t="inlineStr"/>
@@ -3509,7 +3493,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus ladies tee</t>
+          <t>google redesign/drinkware/google 16oz tumbler blue</t>
         </is>
       </c>
       <c r="B253" t="inlineStr"/>
@@ -3517,7 +3501,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus mug</t>
+          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
         </is>
       </c>
       <c r="B254" t="inlineStr"/>
@@ -3525,7 +3509,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
+          <t>google redesign/drinkware/google 24oz ring bottle red</t>
         </is>
       </c>
       <c r="B255" t="inlineStr"/>
@@ -3533,7 +3517,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
+          <t>google redesign/drinkware/google austin campus mug</t>
         </is>
       </c>
       <c r="B256" t="inlineStr"/>
@@ -3541,7 +3525,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
+          <t>google redesign/drinkware/google bike bottle</t>
         </is>
       </c>
       <c r="B257" t="inlineStr"/>
@@ -3549,7 +3533,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
+          <t>google redesign/drinkware/google cambridge campus bottle</t>
         </is>
       </c>
       <c r="B258" t="inlineStr"/>
@@ -3557,7 +3541,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android buoy bottle</t>
+          <t>google redesign/drinkware/google cambridge campus mug</t>
         </is>
       </c>
       <c r="B259" t="inlineStr"/>
@@ -3565,7 +3549,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic glass bottle green</t>
+          <t>google redesign/drinkware/google camp mug ivory</t>
         </is>
       </c>
       <c r="B260" t="inlineStr"/>
@@ -3573,7 +3557,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic mug gray</t>
+          <t>google redesign/drinkware/google canteen bottle black</t>
         </is>
       </c>
       <c r="B261" t="inlineStr"/>
@@ -3581,7 +3565,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/campus corkbase mug blue</t>
+          <t>google redesign/drinkware/google chicago campus mug</t>
         </is>
       </c>
       <c r="B262" t="inlineStr"/>
@@ -3589,7 +3573,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 16oz tumbler blue</t>
+          <t>google redesign/drinkware/google cork base tumbler</t>
         </is>
       </c>
       <c r="B263" t="inlineStr"/>
@@ -3597,7 +3581,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
+          <t>google redesign/drinkware/google cup cap tumbler grey</t>
         </is>
       </c>
       <c r="B264" t="inlineStr"/>
@@ -3605,7 +3589,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle red</t>
+          <t>google redesign/drinkware/google glass bottle</t>
         </is>
       </c>
       <c r="B265" t="inlineStr"/>
@@ -3613,7 +3597,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google austin campus bottle</t>
+          <t>google redesign/drinkware/google keepcup</t>
         </is>
       </c>
       <c r="B266" t="inlineStr"/>
@@ -3621,7 +3605,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google austin campus mug</t>
+          <t>google redesign/drinkware/google kirkland campus mug</t>
         </is>
       </c>
       <c r="B267" t="inlineStr"/>
@@ -3629,7 +3613,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google bike bottle</t>
+          <t>google redesign/drinkware/google la campus mug</t>
         </is>
       </c>
       <c r="B268" t="inlineStr"/>
@@ -3637,7 +3621,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google boulder campus mug</t>
+          <t>google redesign/drinkware/google mural bottle</t>
         </is>
       </c>
       <c r="B269" t="inlineStr"/>
@@ -3645,7 +3629,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus bottle</t>
+          <t>google redesign/drinkware/google mural mug</t>
         </is>
       </c>
       <c r="B270" t="inlineStr"/>
@@ -3653,7 +3637,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus mug</t>
+          <t>google redesign/drinkware/google nyc campus bottle</t>
         </is>
       </c>
       <c r="B271" t="inlineStr"/>
@@ -3661,7 +3645,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google camp mug ivory</t>
+          <t>google redesign/drinkware/google nyc campus mug</t>
         </is>
       </c>
       <c r="B272" t="inlineStr"/>
@@ -3669,7 +3653,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google canteen bottle black</t>
+          <t>google redesign/drinkware/google perk thermal cup</t>
         </is>
       </c>
       <c r="B273" t="inlineStr"/>
@@ -3677,7 +3661,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google chicago campus mug</t>
+          <t>google redesign/drinkware/google pnw campus bottle</t>
         </is>
       </c>
       <c r="B274" t="inlineStr"/>
@@ -3685,7 +3669,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cork base tumbler</t>
+          <t>google redesign/drinkware/google sf campus bottle</t>
         </is>
       </c>
       <c r="B275" t="inlineStr"/>
@@ -3693,7 +3677,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cup cap tumbler grey</t>
+          <t>google redesign/drinkware/google sf campus mug</t>
         </is>
       </c>
       <c r="B276" t="inlineStr"/>
@@ -3701,7 +3685,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google glass bottle</t>
+          <t>google redesign/drinkware/google super g tumbler blue lid</t>
         </is>
       </c>
       <c r="B277" t="inlineStr"/>
@@ -3709,7 +3693,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google keepcup</t>
+          <t>google redesign/drinkware/google super g tumbler red lid</t>
         </is>
       </c>
       <c r="B278" t="inlineStr"/>
@@ -3717,7 +3701,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google kirkland campus mug</t>
+          <t>google redesign/drinkware/google thermal tumbler navy</t>
         </is>
       </c>
       <c r="B279" t="inlineStr"/>
@@ -3725,7 +3709,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google la campus bottle</t>
+          <t>google redesign/drinkware/google woodtop bottle black</t>
         </is>
       </c>
       <c r="B280" t="inlineStr"/>
@@ -3733,7 +3717,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google la campus mug</t>
+          <t>google redesign/drinkware/iamremarkable water bottle</t>
         </is>
       </c>
       <c r="B281" t="inlineStr"/>
@@ -3741,7 +3725,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural bottle</t>
+          <t>google redesign/drinkware/mugs tumblers</t>
         </is>
       </c>
       <c r="B282" t="inlineStr"/>
@@ -3749,7 +3733,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural mug</t>
+          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
         </is>
       </c>
       <c r="B283" t="inlineStr"/>
@@ -3757,7 +3741,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus bottle</t>
+          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
         </is>
       </c>
       <c r="B284" t="inlineStr"/>
@@ -3765,7 +3749,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus mug</t>
+          <t>google redesign/drinkware/water bottles</t>
         </is>
       </c>
       <c r="B285" t="inlineStr"/>
@@ -3773,7 +3757,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google perk thermal cup</t>
+          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
         </is>
       </c>
       <c r="B286" t="inlineStr"/>
@@ -3781,7 +3765,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google pnw campus bottle</t>
+          <t>google redesign/drinkware/youtube play mug</t>
         </is>
       </c>
       <c r="B287" t="inlineStr"/>
@@ -3789,7 +3773,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google pnw campus mug</t>
+          <t>google redesign/eco friendly</t>
         </is>
       </c>
       <c r="B288" t="inlineStr"/>
@@ -3797,7 +3781,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google seattle campus mug</t>
+          <t>google redesign/electronics</t>
         </is>
       </c>
       <c r="B289" t="inlineStr"/>
@@ -3805,7 +3789,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus bottle</t>
+          <t>google redesign/electronics/accessories</t>
         </is>
       </c>
       <c r="B290" t="inlineStr"/>
@@ -3813,7 +3797,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus mug</t>
+          <t>google redesign/electronics/audio</t>
         </is>
       </c>
       <c r="B291" t="inlineStr"/>
@@ -3821,7 +3805,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler blue lid</t>
+          <t>google redesign/gift cards</t>
         </is>
       </c>
       <c r="B292" t="inlineStr"/>
@@ -3829,7 +3813,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler red lid</t>
+          <t>google redesign/google blue stojo cup</t>
         </is>
       </c>
       <c r="B293" t="inlineStr"/>
@@ -3837,7 +3821,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google thermal tumbler navy</t>
+          <t>google redesign/google chrome dino light up water bottle</t>
         </is>
       </c>
       <c r="B294" t="inlineStr"/>
@@ -3845,7 +3829,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google woodtop bottle black</t>
+          <t>google redesign/google crew sweater navy</t>
         </is>
       </c>
       <c r="B295" t="inlineStr"/>
@@ -3853,7 +3837,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/iamremarkable water bottle</t>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
         </is>
       </c>
       <c r="B296" t="inlineStr"/>
@@ -3861,7 +3845,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/mugs tumblers</t>
+          <t>google redesign/google land and sea french terry sweatshirt ls</t>
         </is>
       </c>
       <c r="B297" t="inlineStr"/>
@@ -3869,7 +3853,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B298" t="inlineStr"/>
@@ -3877,7 +3861,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B299" t="inlineStr"/>
@@ -3885,7 +3869,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/water bottles</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B300" t="inlineStr"/>
@@ -3893,7 +3877,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
+          <t>google redesign/lifestyle/bags</t>
         </is>
       </c>
       <c r="B301" t="inlineStr"/>
@@ -3901,7 +3885,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube play mug</t>
+          <t>google redesign/lifestyle/drinkware</t>
         </is>
       </c>
       <c r="B302" t="inlineStr"/>
@@ -3909,7 +3893,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
+          <t>google redesign/lifestyle/fun</t>
         </is>
       </c>
       <c r="B303" t="inlineStr"/>
@@ -3917,7 +3901,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
+          <t>google redesign/lifestyle/google aluminum bottle red</t>
         </is>
       </c>
       <c r="B304" t="inlineStr"/>
@@ -3925,7 +3909,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>google redesign/electronics/accessories</t>
+          <t>google redesign/lifestyle/google bear baby blanket beige</t>
         </is>
       </c>
       <c r="B305" t="inlineStr"/>
@@ -3933,7 +3917,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>google redesign/electronics/audio</t>
+          <t>google redesign/lifestyle/google camp mug gray</t>
         </is>
       </c>
       <c r="B306" t="inlineStr"/>
@@ -3941,7 +3925,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
+          <t>google redesign/lifestyle/google knit blanket</t>
         </is>
       </c>
       <c r="B307" t="inlineStr"/>
@@ -3949,7 +3933,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
+          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
         </is>
       </c>
       <c r="B308" t="inlineStr"/>
@@ -3957,7 +3941,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
+          <t>google redesign/lifestyle/google land and sea tote bag</t>
         </is>
       </c>
       <c r="B309" t="inlineStr"/>
@@ -3965,7 +3949,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
+          <t>google redesign/lifestyle/google-frisbee</t>
         </is>
       </c>
       <c r="B310" t="inlineStr"/>
@@ -3973,7 +3957,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
+          <t>google redesign/lifestyle/small goods</t>
         </is>
       </c>
       <c r="B311" t="inlineStr"/>
@@ -3981,7 +3965,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt ls</t>
+          <t>google redesign/lifestyle/white google shoreline bottle</t>
         </is>
       </c>
       <c r="B312" t="inlineStr"/>
@@ -3989,7 +3973,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B313" t="inlineStr"/>
@@ -3997,7 +3981,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/notebooks journals/google large standard journal grey</t>
         </is>
       </c>
       <c r="B314" t="inlineStr"/>
@@ -4005,7 +3989,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B315" t="inlineStr"/>
@@ -4013,7 +3997,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/office/android iconic notebook</t>
         </is>
       </c>
       <c r="B316" t="inlineStr"/>
@@ -4021,7 +4005,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/bags</t>
+          <t>google redesign/office/android iconic pen</t>
         </is>
       </c>
       <c r="B317" t="inlineStr"/>
@@ -4029,7 +4013,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/drinkware</t>
+          <t>google redesign/office/android large trace journal black</t>
         </is>
       </c>
       <c r="B318" t="inlineStr"/>
@@ -4037,7 +4021,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/fun</t>
+          <t>google redesign/office/android small trace journal bl</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
@@ -4045,7 +4029,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google aluminum bottle red</t>
+          <t>google redesign/office/google appeel journal red</t>
         </is>
       </c>
       <c r="B320" t="inlineStr"/>
@@ -4053,7 +4037,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google bear baby blanket beige</t>
+          <t>google redesign/office/google black cork journal</t>
         </is>
       </c>
       <c r="B321" t="inlineStr"/>
@@ -4061,7 +4045,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google camp mug gray</t>
+          <t>google redesign/office/google clear pen 4pack</t>
         </is>
       </c>
       <c r="B322" t="inlineStr"/>
@@ -4069,7 +4053,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google knit blanket</t>
+          <t>google redesign/office/google cork journal</t>
         </is>
       </c>
       <c r="B323" t="inlineStr"/>
@@ -4077,7 +4061,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
+          <t>google redesign/office/google cork pencil pouch</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
@@ -4085,7 +4069,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea tote bag</t>
+          <t>google redesign/office/google felt refillable journal</t>
         </is>
       </c>
       <c r="B325" t="inlineStr"/>
@@ -4093,7 +4077,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google-frisbee</t>
+          <t>google redesign/office/google google campus bike grid task pad</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
@@ -4101,7 +4085,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/small goods</t>
+          <t>google redesign/office/google google color block notebook</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
@@ -4109,7 +4093,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/white google shoreline bottle</t>
+          <t>google redesign/office/google google confetti pen white</t>
         </is>
       </c>
       <c r="B328" t="inlineStr"/>
@@ -4117,7 +4101,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/office/google google confetti slim task pad</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
@@ -4125,7 +4109,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals/google large standard journal grey</t>
+          <t>google redesign/office/google google confetti task pad</t>
         </is>
       </c>
       <c r="B330" t="inlineStr"/>
@@ -4133,7 +4117,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/office/google light up pen blue</t>
         </is>
       </c>
       <c r="B331" t="inlineStr"/>
@@ -4141,7 +4125,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>google redesign/office/android iconic notebook</t>
+          <t>google redesign/office/google light up pen green</t>
         </is>
       </c>
       <c r="B332" t="inlineStr"/>
@@ -4149,7 +4133,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>google redesign/office/android iconic pen</t>
+          <t>google redesign/office/google light up pen red</t>
         </is>
       </c>
       <c r="B333" t="inlineStr"/>
@@ -4157,7 +4141,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>google redesign/office/android large trace journal black</t>
+          <t>google redesign/office/google mural notebook</t>
         </is>
       </c>
       <c r="B334" t="inlineStr"/>
@@ -4165,7 +4149,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>google redesign/office/android small trace journal bl</t>
+          <t>google redesign/office/google mural sticky note pad</t>
         </is>
       </c>
       <c r="B335" t="inlineStr"/>
@@ -4173,7 +4157,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>google redesign/office/google appeel journal red</t>
+          <t>google redesign/office/google pen grey</t>
         </is>
       </c>
       <c r="B336" t="inlineStr"/>
@@ -4181,7 +4165,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>google redesign/office/google black cork journal</t>
+          <t>google redesign/office/google pen neon coral</t>
         </is>
       </c>
       <c r="B337" t="inlineStr"/>
@@ -4189,7 +4173,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>google redesign/office/google clear pen 4pack</t>
+          <t>google redesign/office/google pen white</t>
         </is>
       </c>
       <c r="B338" t="inlineStr"/>
@@ -4197,7 +4181,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork journal</t>
+          <t>google redesign/office/google phone stand bamboo</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
@@ -4205,7 +4189,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork pencil pouch</t>
+          <t>google redesign/office/google recycled notebook set natural</t>
         </is>
       </c>
       <c r="B340" t="inlineStr"/>
@@ -4213,7 +4197,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>google redesign/office/google felt refillable journal</t>
+          <t>google redesign/office/google recycled pen black</t>
         </is>
       </c>
       <c r="B341" t="inlineStr"/>
@@ -4221,7 +4205,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>google redesign/office/google google campus bike grid task pad</t>
+          <t>google redesign/office/google recycled pen green</t>
         </is>
       </c>
       <c r="B342" t="inlineStr"/>
@@ -4229,7 +4213,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>google redesign/office/google google color block notebook</t>
+          <t>google redesign/office/google recycled writing set</t>
         </is>
       </c>
       <c r="B343" t="inlineStr"/>
@@ -4237,7 +4221,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti pen white</t>
+          <t>google redesign/office/google small standard journal navy</t>
         </is>
       </c>
       <c r="B344" t="inlineStr"/>
@@ -4245,7 +4229,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti slim task pad</t>
+          <t>google redesign/office/google soft modal scarf</t>
         </is>
       </c>
       <c r="B345" t="inlineStr"/>
@@ -4253,7 +4237,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti task pad</t>
+          <t>google redesign/office/google sustainable pencil pouch</t>
         </is>
       </c>
       <c r="B346" t="inlineStr"/>
@@ -4261,7 +4245,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen blue</t>
+          <t>google redesign/office/iamremarkable journal</t>
         </is>
       </c>
       <c r="B347" t="inlineStr"/>
@@ -4269,7 +4253,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen green</t>
+          <t>google redesign/office/iamremarkable pen</t>
         </is>
       </c>
       <c r="B348" t="inlineStr"/>
@@ -4277,7 +4261,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen red</t>
+          <t>google redesign/office/notebooks journals</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
@@ -4285,7 +4269,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural notebook</t>
+          <t>google redesign/office/stickers</t>
         </is>
       </c>
       <c r="B350" t="inlineStr"/>
@@ -4293,7 +4277,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural sticky note pad</t>
+          <t>google redesign/office/writing</t>
         </is>
       </c>
       <c r="B351" t="inlineStr"/>
@@ -4301,7 +4285,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen bright blue</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B352" t="inlineStr"/>
@@ -4309,7 +4293,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen citron</t>
+          <t>google redesign/shop by brand/android</t>
         </is>
       </c>
       <c r="B353" t="inlineStr"/>
@@ -4317,7 +4301,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grass green</t>
+          <t>google redesign/shop by brand/google</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
@@ -4325,7 +4309,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grey</t>
+          <t>google redesign/shop by brand/google cloud</t>
         </is>
       </c>
       <c r="B355" t="inlineStr"/>
@@ -4333,7 +4317,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen lilac</t>
+          <t>google redesign/shop by brand/i am remarkable</t>
         </is>
       </c>
       <c r="B356" t="inlineStr"/>
@@ -4341,7 +4325,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen neon coral</t>
+          <t>google redesign/shop by brand/youtube</t>
         </is>
       </c>
       <c r="B357" t="inlineStr"/>
@@ -4349,7 +4333,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen red</t>
+          <t>google redesign/small goods/daddy works at google book</t>
         </is>
       </c>
       <c r="B358" t="inlineStr"/>
@@ -4357,7 +4341,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen white</t>
+          <t>google redesign/small goods/mommy works at google book</t>
         </is>
       </c>
       <c r="B359" t="inlineStr"/>
@@ -4365,7 +4349,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>google redesign/office/google phone stand bamboo</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B360" t="inlineStr"/>
@@ -4373,7 +4357,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled notebook set natural</t>
+          <t>google redesign/stationery/google 4in decal</t>
         </is>
       </c>
       <c r="B361" t="inlineStr"/>
@@ -4381,7 +4365,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen black</t>
+          <t>google redesign/stationery/google cloud pen</t>
         </is>
       </c>
       <c r="B362" t="inlineStr"/>
@@ -4389,7 +4373,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen green</t>
+          <t>google redesign/stationery/google jotter task pad</t>
         </is>
       </c>
       <c r="B363" t="inlineStr"/>
@@ -4397,7 +4381,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled writing set</t>
+          <t>google redesign/stationery/google land and sea journal set</t>
         </is>
       </c>
       <c r="B364" t="inlineStr"/>
@@ -4405,7 +4389,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>google redesign/office/google small standard journal navy</t>
+          <t>google redesign/stationery/notebooks</t>
         </is>
       </c>
       <c r="B365" t="inlineStr"/>
@@ -4413,7 +4397,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>google redesign/office/google soft modal scarf</t>
+          <t>google redesign/stationery/stickers</t>
         </is>
       </c>
       <c r="B366" t="inlineStr"/>
@@ -4421,7 +4405,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>google redesign/office/google sustainable pencil pouch</t>
+          <t>google redesign/stationery/writing</t>
         </is>
       </c>
       <c r="B367" t="inlineStr"/>
@@ -4429,7 +4413,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable journal</t>
+          <t>google redesign/stationery/youtube jotter task pad</t>
         </is>
       </c>
       <c r="B368" t="inlineStr"/>
@@ -4437,7 +4421,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable pen</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B369" t="inlineStr"/>
@@ -4445,7 +4429,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>google redesign/office/notebooks journals</t>
+          <t>google redesign/wearables/men s t-shirts</t>
         </is>
       </c>
       <c r="B370" t="inlineStr"/>
@@ -4453,7 +4437,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>google redesign/office/stickers</t>
+          <t>google rmg redesign/lifestyle/mural food container</t>
         </is>
       </c>
       <c r="B371" t="inlineStr"/>
@@ -4461,7 +4445,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>google redesign/office/writing</t>
+          <t>google yellowesign/apparel/google tee yellow</t>
         </is>
       </c>
       <c r="B372" t="inlineStr"/>
@@ -4469,7 +4453,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B373" t="inlineStr"/>
@@ -4477,7 +4461,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/android</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B374" t="inlineStr"/>
@@ -4485,7 +4469,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B375" t="inlineStr"/>
@@ -4493,7 +4477,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google cloud</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B376" t="inlineStr"/>
@@ -4501,7 +4485,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/i am remarkable</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B377" t="inlineStr"/>
@@ -4509,7 +4493,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/youtube</t>
+          <t>store-policies/privacy-policy</t>
         </is>
       </c>
       <c r="B378" t="inlineStr"/>
@@ -4517,7 +4501,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>google redesign/small goods/daddy works at google book</t>
+          <t>store-policies/return-policy</t>
         </is>
       </c>
       <c r="B379" t="inlineStr"/>
@@ -4525,7 +4509,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>google redesign/small goods/mommy works at google book</t>
+          <t>store-policies/shipping-information</t>
         </is>
       </c>
       <c r="B380" t="inlineStr"/>
@@ -4533,7 +4517,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>store-policies/terms-of-use</t>
         </is>
       </c>
       <c r="B381" t="inlineStr"/>
@@ -4541,7 +4525,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>google redesign/stationery/android jotter task pad</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B382" t="inlineStr"/>
@@ -4549,7 +4533,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google 4in decal</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B383" t="inlineStr"/>
@@ -4557,7 +4541,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google cloud pen</t>
+          <t>the google merchandise store - register</t>
         </is>
       </c>
       <c r="B384" t="inlineStr"/>
@@ -4565,186 +4549,10 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google jotter task pad</t>
+          <t>your wishlist</t>
         </is>
       </c>
       <c r="B385" t="inlineStr"/>
-    </row>
-    <row r="386">
-      <c r="A386" t="inlineStr">
-        <is>
-          <t>google redesign/stationery/google land and sea journal set</t>
-        </is>
-      </c>
-      <c r="B386" t="inlineStr"/>
-    </row>
-    <row r="387">
-      <c r="A387" t="inlineStr">
-        <is>
-          <t>google redesign/stationery/notebooks</t>
-        </is>
-      </c>
-      <c r="B387" t="inlineStr"/>
-    </row>
-    <row r="388">
-      <c r="A388" t="inlineStr">
-        <is>
-          <t>google redesign/stationery/stickers</t>
-        </is>
-      </c>
-      <c r="B388" t="inlineStr"/>
-    </row>
-    <row r="389">
-      <c r="A389" t="inlineStr">
-        <is>
-          <t>google redesign/stationery/writing</t>
-        </is>
-      </c>
-      <c r="B389" t="inlineStr"/>
-    </row>
-    <row r="390">
-      <c r="A390" t="inlineStr">
-        <is>
-          <t>google redesign/stationery/youtube jotter task pad</t>
-        </is>
-      </c>
-      <c r="B390" t="inlineStr"/>
-    </row>
-    <row r="391">
-      <c r="A391" t="inlineStr">
-        <is>
-          <t>google redesign/super g unisex joggers</t>
-        </is>
-      </c>
-      <c r="B391" t="inlineStr"/>
-    </row>
-    <row r="392">
-      <c r="A392" t="inlineStr">
-        <is>
-          <t>google redesign/wearables/men s t-shirts</t>
-        </is>
-      </c>
-      <c r="B392" t="inlineStr"/>
-    </row>
-    <row r="393">
-      <c r="A393" t="inlineStr">
-        <is>
-          <t>google rmg redesign/lifestyle/mural food container</t>
-        </is>
-      </c>
-      <c r="B393" t="inlineStr"/>
-    </row>
-    <row r="394">
-      <c r="A394" t="inlineStr">
-        <is>
-          <t>google yellowesign/apparel/google tee yellow</t>
-        </is>
-      </c>
-      <c r="B394" t="inlineStr"/>
-    </row>
-    <row r="395">
-      <c r="A395" t="inlineStr">
-        <is>
-          <t>home</t>
-        </is>
-      </c>
-      <c r="B395" t="inlineStr"/>
-    </row>
-    <row r="396">
-      <c r="A396" t="inlineStr">
-        <is>
-          <t>payment method</t>
-        </is>
-      </c>
-      <c r="B396" t="inlineStr"/>
-    </row>
-    <row r="397">
-      <c r="A397" t="inlineStr">
-        <is>
-          <t>shopping cart</t>
-        </is>
-      </c>
-      <c r="B397" t="inlineStr"/>
-    </row>
-    <row r="398">
-      <c r="A398" t="inlineStr">
-        <is>
-          <t>store search results</t>
-        </is>
-      </c>
-      <c r="B398" t="inlineStr"/>
-    </row>
-    <row r="399">
-      <c r="A399" t="inlineStr">
-        <is>
-          <t>store-policies/frequently-asked-questions</t>
-        </is>
-      </c>
-      <c r="B399" t="inlineStr"/>
-    </row>
-    <row r="400">
-      <c r="A400" t="inlineStr">
-        <is>
-          <t>store-policies/privacy-policy</t>
-        </is>
-      </c>
-      <c r="B400" t="inlineStr"/>
-    </row>
-    <row r="401">
-      <c r="A401" t="inlineStr">
-        <is>
-          <t>store-policies/return-policy</t>
-        </is>
-      </c>
-      <c r="B401" t="inlineStr"/>
-    </row>
-    <row r="402">
-      <c r="A402" t="inlineStr">
-        <is>
-          <t>store-policies/shipping-information</t>
-        </is>
-      </c>
-      <c r="B402" t="inlineStr"/>
-    </row>
-    <row r="403">
-      <c r="A403" t="inlineStr">
-        <is>
-          <t>store-policies/terms-of-use</t>
-        </is>
-      </c>
-      <c r="B403" t="inlineStr"/>
-    </row>
-    <row r="404">
-      <c r="A404" t="inlineStr">
-        <is>
-          <t>the google merchandise store - log in</t>
-        </is>
-      </c>
-      <c r="B404" t="inlineStr"/>
-    </row>
-    <row r="405">
-      <c r="A405" t="inlineStr">
-        <is>
-          <t>the google merchandise store - my account</t>
-        </is>
-      </c>
-      <c r="B405" t="inlineStr"/>
-    </row>
-    <row r="406">
-      <c r="A406" t="inlineStr">
-        <is>
-          <t>the google merchandise store - register</t>
-        </is>
-      </c>
-      <c r="B406" t="inlineStr"/>
-    </row>
-    <row r="407">
-      <c r="A407" t="inlineStr">
-        <is>
-          <t>your wishlist</t>
-        </is>
-      </c>
-      <c r="B407" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5998,7 +5806,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6181,18 +5989,10 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Smartphone - Edge</t>
+          <t>Xiaomi - Mi 11</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Xiaomi - Mi 11</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
updated balancing, data prep rules
</commit_message>
<xml_diff>
--- a/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
+++ b/notebooks/google_merch_store/data/df_merch_values_pre_encoding.xlsx
@@ -855,7 +855,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
+          <t>black lives matter | google merchandise store</t>
         </is>
       </c>
       <c r="B3" t="inlineStr"/>
@@ -863,7 +863,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout review</t>
+          <t>checkout confirmation</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -871,7 +871,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout your information</t>
+          <t>checkout review</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -879,7 +879,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>clearance</t>
+          <t>checkout your information</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -1023,7 +1023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B54"/>
+  <dimension ref="A1:B52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1062,7 +1062,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
+          <t>black lives matter | google merchandise store</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -1070,7 +1070,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout review</t>
+          <t>checkout confirmation</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -1078,7 +1078,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout your information</t>
+          <t>checkout review</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -1086,7 +1086,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>clearance/clearance-accessories</t>
+          <t>checkout your information</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -1126,7 +1126,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/5k run</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1134,7 +1134,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1142,7 +1142,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1150,7 +1150,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+          <t>google redesign/bags</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1158,7 +1158,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>google redesign/bags</t>
+          <t>google redesign/blm unisex pullover hoodie</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1166,7 +1166,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
+          <t>google redesign/campus collection</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1174,7 +1174,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
+          <t>google redesign/clearance</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1182,7 +1182,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
+          <t>google redesign/drinkware</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1190,7 +1190,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>google redesign/drinkware</t>
+          <t>google redesign/eco friendly</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1198,7 +1198,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
+          <t>google redesign/electronics</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -1206,7 +1206,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
+          <t>google redesign/gift cards</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1214,7 +1214,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
+          <t>google redesign/google blue stojo cup</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1222,7 +1222,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
+          <t>google redesign/google chrome dino light up water bottle</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1230,7 +1230,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
+          <t>google redesign/google crew sweater navy</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1238,7 +1238,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1246,7 +1246,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1254,7 +1254,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1262,7 +1262,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1270,7 +1270,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1278,7 +1278,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/notebooks journals</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1286,7 +1286,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1294,7 +1294,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1302,7 +1302,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/small goods</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1310,7 +1310,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1318,7 +1318,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/small goods</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1326,7 +1326,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/wearables</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1334,7 +1334,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>google rmg redesign/lifestyle</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1342,7 +1342,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/wearables</t>
+          <t>google yellowesign/apparel</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1350,7 +1350,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1358,7 +1358,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1366,7 +1366,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1374,7 +1374,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1382,7 +1382,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1390,7 +1390,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>store-policies/privacy-policy</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1398,7 +1398,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>store-policies/return-policy</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1406,7 +1406,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
+          <t>store-policies/shipping-information</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1414,7 +1414,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
+          <t>store-policies/terms-of-use</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1422,7 +1422,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
+          <t>the google merchandise store - log in</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1430,7 +1430,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
+          <t>the google merchandise store - my account</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1438,7 +1438,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>the google merchandise store - register</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1446,26 +1446,10 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>your wishlist</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>the google merchandise store - register</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr"/>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>your wishlist</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1478,7 +1462,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B383"/>
+  <dimension ref="A1:B390"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1517,7 +1501,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>checkout confirmation</t>
+          <t>black lives matter | google merchandise store</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
@@ -1525,7 +1509,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>checkout review</t>
+          <t>checkout confirmation</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
@@ -1533,7 +1517,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>checkout your information</t>
+          <t>checkout review</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -1541,7 +1525,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>clearance/clearance-accessories</t>
+          <t>checkout your information</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -1581,7 +1565,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>google redesign/5k run/google 5k run 2020 womens tee</t>
+          <t>google redesign/accessories</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -1589,7 +1573,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>google redesign/accessories</t>
+          <t>google redesign/accessories/android iconic 4in decal</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
@@ -1597,7 +1581,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android large removable sticker sheet</t>
+          <t>google redesign/accessories/android iconic pin</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
@@ -1605,7 +1589,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android lumberjack pin</t>
+          <t>google redesign/accessories/android large removable sticker sheet</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
@@ -1613,7 +1597,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android puzzlebot v2</t>
+          <t>google redesign/accessories/android lumberjack pin</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
@@ -1621,7 +1605,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android sm sticker sheet</t>
+          <t>google redesign/accessories/android puzzlebot v2</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
@@ -1629,7 +1613,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android super hero 3d framed art</t>
+          <t>google redesign/accessories/android sm sticker sheet</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
@@ -1637,7 +1621,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>google redesign/accessories/android techie 3d framed art</t>
+          <t>google redesign/accessories/android super hero 3d framed art</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
@@ -1645,7 +1629,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>google redesign/accessories/fun</t>
+          <t>google redesign/accessories/android techie 3d framed art</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -1653,7 +1637,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google blue yoyo</t>
+          <t>google redesign/accessories/fun</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -1661,7 +1645,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google bot</t>
+          <t>google redesign/accessories/google blue yoyo</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -1669,7 +1653,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google bot multicolored</t>
+          <t>google redesign/accessories/google bot</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -1677,7 +1661,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google campus bike</t>
+          <t>google redesign/accessories/google bot multicolored</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -1685,7 +1669,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google chrome dinosaur collectible</t>
+          <t>google redesign/accessories/google campus bike</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -1693,7 +1677,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed blue shades</t>
+          <t>google redesign/accessories/google chrome dinosaur collectible</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -1701,7 +1685,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed gray shades</t>
+          <t>google redesign/accessories/google clear framed blue shades</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -1709,7 +1693,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google clear framed yellow shades</t>
+          <t>google redesign/accessories/google clear framed gray shades</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -1717,7 +1701,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cloth pouch black</t>
+          <t>google redesign/accessories/google clear framed yellow shades</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -1725,7 +1709,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork card holder</t>
+          <t>google redesign/accessories/google cloth pouch black</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -1733,7 +1717,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork passport holder</t>
+          <t>google redesign/accessories/google cork card holder</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -1741,7 +1725,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google cork tablet case</t>
+          <t>google redesign/accessories/google cork key ring</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -1749,7 +1733,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji magnet set</t>
+          <t>google redesign/accessories/google cork passport holder</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -1757,7 +1741,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
+          <t>google redesign/accessories/google cork tablet case</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -1765,7 +1749,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt luggage tag</t>
+          <t>google redesign/accessories/google emoji magnet set</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -1773,7 +1757,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google felt strap keyring</t>
+          <t>google redesign/accessories/google emoji sticker pack 2 sheet</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -1781,7 +1765,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google inverted umbrella</t>
+          <t>google redesign/accessories/google felt luggage tag</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -1789,7 +1773,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google keychain 19</t>
+          <t>google redesign/accessories/google felt strap keyring</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -1797,7 +1781,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lapel pin</t>
+          <t>google redesign/accessories/google inverted umbrella</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -1805,7 +1789,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google laptop sleeve charcoal</t>
+          <t>google redesign/accessories/google keychain 19</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -1813,7 +1797,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google lovehandle black</t>
+          <t>google redesign/accessories/google lapel pin</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -1821,7 +1805,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google magnet</t>
+          <t>google redesign/accessories/google laptop sleeve charcoal</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -1829,7 +1813,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google maps pin</t>
+          <t>google redesign/accessories/google large pet collar blue green</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -1837,7 +1821,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google medium pet collar blue green</t>
+          <t>google redesign/accessories/google lovehandle black</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -1845,7 +1829,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google medium pet leash blue green</t>
+          <t>google redesign/accessories/google magnet</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -1853,7 +1837,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mouse pad navy</t>
+          <t>google redesign/accessories/google maps pin</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -1861,7 +1845,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google mural sticker sheet</t>
+          <t>google redesign/accessories/google medium pet collar blue green</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1869,7 +1853,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google nyc campus lapel pin</t>
+          <t>google redesign/accessories/google medium pet leash blue green</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -1877,7 +1861,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google pride sticker</t>
+          <t>google redesign/accessories/google mouse pad navy</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -1885,7 +1869,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google see no hear no set</t>
+          <t>google redesign/accessories/google mural sticker sheet</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -1893,7 +1877,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google small cable organizer blue</t>
+          <t>google redesign/accessories/google nyc campus lapel pin</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -1901,7 +1885,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google tech taco</t>
+          <t>google redesign/accessories/google nyc campus sticker</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -1909,7 +1893,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google utensil set</t>
+          <t>google redesign/accessories/google pride sticker</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -1917,7 +1901,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>google redesign/accessories/google yellow yoyo</t>
+          <t>google redesign/accessories/google see no hear no set</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -1925,7 +1909,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>google redesign/accessories/iamremarkable lapel pin</t>
+          <t>google redesign/accessories/google small cable organizer blue</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -1933,7 +1917,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>google redesign/accessories/noogler android figure 2019</t>
+          <t>google redesign/accessories/google tech taco</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -1941,7 +1925,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
+          <t>google redesign/accessories/google utensil set</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -1949,7 +1933,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube iconic play pin</t>
+          <t>google redesign/accessories/iamremarkable lapel pin</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -1957,7 +1941,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>google redesign/accessories/youtube small sticker sheet</t>
+          <t>google redesign/accessories/noogler android figure 2019</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -1965,7 +1949,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>google redesign/apparel</t>
+          <t>google redesign/accessories/snowflake android cardboard sculpture</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -1973,7 +1957,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android garden tee orange</t>
+          <t>google redesign/accessories/youtube iconic play pin</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -1981,7 +1965,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic beanie</t>
+          <t>google redesign/accessories/youtube small sticker sheet</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
@@ -1989,7 +1973,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic crew</t>
+          <t>google redesign/apparel</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
@@ -1997,7 +1981,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat green</t>
+          <t>google redesign/apparel/android garden tee orange</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
@@ -2005,7 +1989,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat v2 black</t>
+          <t>google redesign/apparel/android iconic beanie</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -2013,7 +1997,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic hat white</t>
+          <t>google redesign/apparel/android iconic crew</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -2021,7 +2005,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android iconic sock</t>
+          <t>google redesign/apparel/android iconic hat green</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -2029,7 +2013,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie navy</t>
+          <t>google redesign/apparel/android iconic hat v2 black</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -2037,7 +2021,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket onesie white</t>
+          <t>google redesign/apparel/android iconic hat white</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -2045,7 +2029,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee green</t>
+          <t>google redesign/apparel/android iconic sock</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -2053,7 +2037,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket tee navy</t>
+          <t>google redesign/apparel/android pocket onesie navy</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
@@ -2061,7 +2045,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee navy</t>
+          <t>google redesign/apparel/android pocket onesie white</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
@@ -2069,7 +2053,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket toddler tee white</t>
+          <t>google redesign/apparel/android pocket tee green</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
@@ -2077,7 +2061,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee green</t>
+          <t>google redesign/apparel/android pocket tee navy</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
@@ -2085,7 +2069,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>google redesign/apparel/android pocket youth tee navy</t>
+          <t>google redesign/apparel/android pocket toddler tee navy</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
@@ -2093,7 +2077,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>google redesign/apparel/flamingo and friends tee blue</t>
+          <t>google redesign/apparel/android pocket toddler tee white</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
@@ -2101,7 +2085,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus unisex tee</t>
+          <t>google redesign/apparel/android pocket youth tee green</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
@@ -2109,7 +2093,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google austin campus zip hoodie</t>
+          <t>google redesign/apparel/android pocket youth tee navy</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
@@ -2117,7 +2101,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google badge heavyweight pullover black</t>
+          <t>google redesign/apparel/flamingo and friends tee blue</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -2125,7 +2109,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black cloud zip hoodie</t>
+          <t>google redesign/apparel/google austin campus unisex tee</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
@@ -2133,7 +2117,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google black tee</t>
+          <t>google redesign/apparel/google austin campus zip hoodie</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
@@ -2141,7 +2125,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google boulder campus unisex tee</t>
+          <t>google redesign/apparel/google badge heavyweight pullover black</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
@@ -2149,7 +2133,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google boulder campus zip hoodie</t>
+          <t>google redesign/apparel/google black cloud zip hoodie</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
@@ -2157,7 +2141,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus unisex tee</t>
+          <t>google redesign/apparel/google black tee</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -2165,7 +2149,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
+          <t>google redesign/apparel/google boulder campus unisex tee</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -2173,7 +2157,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google campus bike eco tee navy</t>
+          <t>google redesign/apparel/google cambridge campus zip hoodie</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -2181,7 +2165,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus unisex tee</t>
+          <t>google redesign/apparel/google campus bike eco tee navy</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -2189,7 +2173,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google chicago campus zip hoodie</t>
+          <t>google redesign/apparel/google chicago campus ladies tee</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
@@ -2197,7 +2181,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google cotopaxi shell</t>
+          <t>google redesign/apparel/google chicago campus unisex tee</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
@@ -2205,7 +2189,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew grey</t>
+          <t>google redesign/apparel/google chicago campus zip hoodie</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
@@ -2213,7 +2197,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crew socks</t>
+          <t>google redesign/apparel/google cotopaxi shell</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
@@ -2221,7 +2205,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google crewneck sweatshirt green</t>
+          <t>google redesign/apparel/google crew grey</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -2229,7 +2213,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google dino game tee</t>
+          <t>google redesign/apparel/google crew socks</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -2237,7 +2221,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve ash</t>
+          <t>google redesign/apparel/google crewneck sweatshirt green</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
@@ -2245,7 +2229,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google dino game tee</t>
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
@@ -2253,7 +2237,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google blue kids sunglasses</t>
+          <t>google redesign/apparel/google fc longsleeve ash</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
@@ -2261,7 +2245,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew combed cotton sock</t>
+          <t>google redesign/apparel/google fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
@@ -2269,7 +2253,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google crew striped athletic sock</t>
+          <t>google redesign/apparel/google google blue kids sunglasses</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
@@ -2277,7 +2261,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google kids playful tee</t>
+          <t>google redesign/apparel/google google crew combed cotton sock</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -2285,7 +2269,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google premium sunglasses</t>
+          <t>google redesign/apparel/google google crew striped athletic sock</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
@@ -2293,7 +2277,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google google summer19 crew grey</t>
+          <t>google redesign/apparel/google google kids playful tee</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
@@ -2301,7 +2285,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google grey tee</t>
+          <t>google redesign/apparel/google google premium sunglasses</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
@@ -2309,7 +2293,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heather green speckled tee</t>
+          <t>google redesign/apparel/google google red kids sunglasses</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
@@ -2317,7 +2301,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google heathered pom beanie</t>
+          <t>google redesign/apparel/google google summer19 crew grey</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -2325,7 +2309,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant charcoal onesie</t>
+          <t>google redesign/apparel/google grey tee</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -2333,7 +2317,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero onesie grey</t>
+          <t>google redesign/apparel/google heather green speckled tee</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -2341,7 +2325,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google infant hero tee olive</t>
+          <t>google redesign/apparel/google heathered pom beanie</t>
         </is>
       </c>
       <c r="B107" t="inlineStr"/>
@@ -2349,7 +2333,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus unisex tee</t>
+          <t>google redesign/apparel/google infant charcoal onesie</t>
         </is>
       </c>
       <c r="B108" t="inlineStr"/>
@@ -2357,7 +2341,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google la campus zip hoodie</t>
+          <t>google redesign/apparel/google infant hero onesie grey</t>
         </is>
       </c>
       <c r="B109" t="inlineStr"/>
@@ -2365,7 +2349,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea cotton cap ls</t>
+          <t>google redesign/apparel/google infant hero tee olive</t>
         </is>
       </c>
       <c r="B110" t="inlineStr"/>
@@ -2373,7 +2357,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea unisex tee</t>
+          <t>google redesign/apparel/google kirkland campus unisex tee</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -2381,7 +2365,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google land and sea womens eco tee</t>
+          <t>google redesign/apparel/google la campus unisex tee</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -2389,7 +2373,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat black</t>
+          <t>google redesign/apparel/google la campus zip hoodie</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -2397,7 +2381,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google leather strap hat blue</t>
+          <t>google redesign/apparel/google land and sea cotton cap ls</t>
         </is>
       </c>
       <c r="B114" t="inlineStr"/>
@@ -2405,7 +2389,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens discovery lt rain shell</t>
+          <t>google redesign/apparel/google land and sea unisex tee</t>
         </is>
       </c>
       <c r="B115" t="inlineStr"/>
@@ -2413,7 +2397,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens microfleece jacket black</t>
+          <t>google redesign/apparel/google land and sea womens eco tee</t>
         </is>
       </c>
       <c r="B116" t="inlineStr"/>
@@ -2421,7 +2405,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens puff jacket black</t>
+          <t>google redesign/apparel/google leather strap hat black</t>
         </is>
       </c>
       <c r="B117" t="inlineStr"/>
@@ -2429,7 +2413,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens softshell moss</t>
+          <t>google redesign/apparel/google leather strap hat blue</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -2437,7 +2421,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece grey</t>
+          <t>google redesign/apparel/google mens discovery lt rain shell</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -2445,7 +2429,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google mens microfleece jacket black</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -2453,7 +2437,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee blue</t>
+          <t>google redesign/apparel/google mens puff jacket black</t>
         </is>
       </c>
       <c r="B121" t="inlineStr"/>
@@ -2461,7 +2445,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mountain view tee red</t>
+          <t>google redesign/apparel/google mens softshell moss</t>
         </is>
       </c>
       <c r="B122" t="inlineStr"/>
@@ -2469,7 +2453,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google mural socks</t>
+          <t>google redesign/apparel/google mens tech fleece grey</t>
         </is>
       </c>
       <c r="B123" t="inlineStr"/>
@@ -2477,7 +2461,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google navy speckled tee</t>
+          <t>google redesign/apparel/google mens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B124" t="inlineStr"/>
@@ -2485,7 +2469,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus ladies tee</t>
+          <t>google redesign/apparel/google mountain view tee blue</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -2493,7 +2477,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus unisex tee</t>
+          <t>google redesign/apparel/google mountain view tee red</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -2501,7 +2485,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google nyc campus zip hoodie</t>
+          <t>google redesign/apparel/google mural socks</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -2509,7 +2493,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus unisex tee</t>
+          <t>google redesign/apparel/google navy speckled tee</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -2517,7 +2501,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google pnw campus zip hoodie</t>
+          <t>google redesign/apparel/google nyc campus ladies tee</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -2525,7 +2509,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google raincoat navy</t>
+          <t>google redesign/apparel/google nyc campus unisex tee</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -2533,7 +2517,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google red speckled tee</t>
+          <t>google redesign/apparel/google nyc campus zip hoodie</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -2541,7 +2525,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google seattle campus unisex tee</t>
+          <t>google redesign/apparel/google pnw campus zip hoodie</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
@@ -2549,7 +2533,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus ladies tee</t>
+          <t>google redesign/apparel/google raincoat navy</t>
         </is>
       </c>
       <c r="B133" t="inlineStr"/>
@@ -2557,7 +2541,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus unisex tee</t>
+          <t>google redesign/apparel/google red speckled tee</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -2565,7 +2549,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sf campus zip hoodie</t>
+          <t>google redesign/apparel/google sf campus ladies tee</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
@@ -2573,7 +2557,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa vest black</t>
+          <t>google redesign/apparel/google sf campus unisex tee</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -2581,7 +2565,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
+          <t>google redesign/apparel/google sf campus zip hoodie</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -2589,7 +2573,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
+          <t>google redesign/apparel/google sherpa vest black</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -2597,7 +2581,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie grey</t>
+          <t>google redesign/apparel/google sherpa zip hoodie charcoal</t>
         </is>
       </c>
       <c r="B139" t="inlineStr"/>
@@ -2605,7 +2589,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google speckled beanie navy</t>
+          <t>google redesign/apparel/google sherpa zip hoodie navy</t>
         </is>
       </c>
       <c r="B140" t="inlineStr"/>
@@ -2613,7 +2597,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google split seam tee olive</t>
+          <t>google redesign/apparel/google speckled beanie grey</t>
         </is>
       </c>
       <c r="B141" t="inlineStr"/>
@@ -2621,7 +2605,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee blue</t>
+          <t>google redesign/apparel/google speckled beanie navy</t>
         </is>
       </c>
       <c r="B142" t="inlineStr"/>
@@ -2629,7 +2613,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee dark blue</t>
+          <t>google redesign/apparel/google split seam tee olive</t>
         </is>
       </c>
       <c r="B143" t="inlineStr"/>
@@ -2637,7 +2621,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee fc black</t>
+          <t>google redesign/apparel/google tee blue</t>
         </is>
       </c>
       <c r="B144" t="inlineStr"/>
@@ -2645,7 +2629,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee mint green</t>
+          <t>google redesign/apparel/google tee dark blue</t>
         </is>
       </c>
       <c r="B145" t="inlineStr"/>
@@ -2653,7 +2637,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tee red</t>
+          <t>google redesign/apparel/google tee fc black</t>
         </is>
       </c>
       <c r="B146" t="inlineStr"/>
@@ -2661,7 +2645,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc tee charcoal</t>
+          <t>google redesign/apparel/google tee mint green</t>
         </is>
       </c>
       <c r="B147" t="inlineStr"/>
@@ -2669,7 +2653,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler fc zip hoodie</t>
+          <t>google redesign/apparel/google tee red</t>
         </is>
       </c>
       <c r="B148" t="inlineStr"/>
@@ -2677,7 +2661,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee black</t>
+          <t>google redesign/apparel/google toddler fc tee charcoal</t>
         </is>
       </c>
       <c r="B149" t="inlineStr"/>
@@ -2685,7 +2669,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler hero tee olive</t>
+          <t>google redesign/apparel/google toddler fc zip hoodie</t>
         </is>
       </c>
       <c r="B150" t="inlineStr"/>
@@ -2693,7 +2677,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google toddler tee white</t>
+          <t>google redesign/apparel/google toddler hero tee black</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -2701,7 +2685,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee coral</t>
+          <t>google redesign/apparel/google toddler hero tee olive</t>
         </is>
       </c>
       <c r="B152" t="inlineStr"/>
@@ -2709,7 +2693,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tonal tee spearmint</t>
+          <t>google redesign/apparel/google toddler tee white</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
@@ -2717,7 +2701,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tracking hat</t>
+          <t>google redesign/apparel/google tonal tee coral</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -2725,7 +2709,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google tudes recycled tee</t>
+          <t>google redesign/apparel/google tonal tee spearmint</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
@@ -2733,7 +2717,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google twill cap charcoal</t>
+          <t>google redesign/apparel/google tracking hat</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -2741,7 +2725,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex eco tee black</t>
+          <t>google redesign/apparel/google tudes recycled tee</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
@@ -2749,7 +2733,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
+          <t>google redesign/apparel/google twill cap charcoal</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
@@ -2757,7 +2741,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex google pocket tee grey</t>
+          <t>google redesign/apparel/google unisex eco tee black</t>
         </is>
       </c>
       <c r="B159" t="inlineStr"/>
@@ -2765,7 +2749,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google unisex pride eco-tee black</t>
+          <t>google redesign/apparel/google unisex google jumbo print tee white</t>
         </is>
       </c>
       <c r="B160" t="inlineStr"/>
@@ -2773,7 +2757,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens black tee</t>
+          <t>google redesign/apparel/google unisex google pocket tee grey</t>
         </is>
       </c>
       <c r="B161" t="inlineStr"/>
@@ -2781,7 +2765,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens discovery</t>
+          <t>google redesign/apparel/google unisex pride eco-tee black</t>
         </is>
       </c>
       <c r="B162" t="inlineStr"/>
@@ -2789,7 +2773,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens eco tee black</t>
+          <t>google redesign/apparel/google womens black tee</t>
         </is>
       </c>
       <c r="B163" t="inlineStr"/>
@@ -2797,7 +2781,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens google striped ls</t>
+          <t>google redesign/apparel/google womens discovery</t>
         </is>
       </c>
       <c r="B164" t="inlineStr"/>
@@ -2805,7 +2789,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens grid zip up</t>
+          <t>google redesign/apparel/google womens eco tee black</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -2813,7 +2797,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens kirkland pullover</t>
+          <t>google redesign/apparel/google womens google striped ls</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
@@ -2821,7 +2805,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens microfleece jacket black</t>
+          <t>google redesign/apparel/google womens grid zip up</t>
         </is>
       </c>
       <c r="B167" t="inlineStr"/>
@@ -2829,7 +2813,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens pride eco-tee black</t>
+          <t>google redesign/apparel/google womens kirkland pullover</t>
         </is>
       </c>
       <c r="B168" t="inlineStr"/>
@@ -2837,7 +2821,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens puff jacket black</t>
+          <t>google redesign/apparel/google womens microfleece jacket black</t>
         </is>
       </c>
       <c r="B169" t="inlineStr"/>
@@ -2845,7 +2829,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens softshell moss</t>
+          <t>google redesign/apparel/google womens pride eco-tee black</t>
         </is>
       </c>
       <c r="B170" t="inlineStr"/>
@@ -2853,7 +2837,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece grey</t>
+          <t>google redesign/apparel/google womens puff jacket black</t>
         </is>
       </c>
       <c r="B171" t="inlineStr"/>
@@ -2861,7 +2845,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
+          <t>google redesign/apparel/google womens softshell moss</t>
         </is>
       </c>
       <c r="B172" t="inlineStr"/>
@@ -2869,7 +2853,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee navy</t>
+          <t>google redesign/apparel/google womens tech fleece grey</t>
         </is>
       </c>
       <c r="B173" t="inlineStr"/>
@@ -2877,7 +2861,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth badge tee olive</t>
+          <t>google redesign/apparel/google womens tech fleece vest charcoal</t>
         </is>
       </c>
       <c r="B174" t="inlineStr"/>
@@ -2885,7 +2869,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
+          <t>google redesign/apparel/google youth badge tee navy</t>
         </is>
       </c>
       <c r="B175" t="inlineStr"/>
@@ -2893,7 +2877,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc pullover hoodie</t>
+          <t>google redesign/apparel/google youth badge tee olive</t>
         </is>
       </c>
       <c r="B176" t="inlineStr"/>
@@ -2901,7 +2885,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc tee charcoal</t>
+          <t>google redesign/apparel/google youth fc longsleeve charcoal</t>
         </is>
       </c>
       <c r="B177" t="inlineStr"/>
@@ -2909,7 +2893,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth fc zip hoodie</t>
+          <t>google redesign/apparel/google youth fc pullover hoodie</t>
         </is>
       </c>
       <c r="B178" t="inlineStr"/>
@@ -2917,7 +2901,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee grey</t>
+          <t>google redesign/apparel/google youth fc tee charcoal</t>
         </is>
       </c>
       <c r="B179" t="inlineStr"/>
@@ -2925,7 +2909,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth hero tee maroon</t>
+          <t>google redesign/apparel/google youth fc zip hoodie</t>
         </is>
       </c>
       <c r="B180" t="inlineStr"/>
@@ -2933,7 +2917,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google youth jumbo print tee white</t>
+          <t>google redesign/apparel/google youth hero tee grey</t>
         </is>
       </c>
       <c r="B181" t="inlineStr"/>
@@ -2941,7 +2925,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>google redesign/apparel/google zip hoodie fc</t>
+          <t>google redesign/apparel/google youth hero tee maroon</t>
         </is>
       </c>
       <c r="B182" t="inlineStr"/>
@@ -2949,7 +2933,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>google redesign/apparel/hats</t>
+          <t>google redesign/apparel/google youth jumbo print tee white</t>
         </is>
       </c>
       <c r="B183" t="inlineStr"/>
@@ -2957,7 +2941,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable hoodie</t>
+          <t>google redesign/apparel/google zip hoodie fc</t>
         </is>
       </c>
       <c r="B184" t="inlineStr"/>
@@ -2965,7 +2949,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
+          <t>google redesign/apparel/hats</t>
         </is>
       </c>
       <c r="B185" t="inlineStr"/>
@@ -2973,7 +2957,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
+          <t>google redesign/apparel/iamremarkable hoodie</t>
         </is>
       </c>
       <c r="B186" t="inlineStr"/>
@@ -2981,7 +2965,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>google redesign/apparel/kids</t>
+          <t>google redesign/apparel/iamremarkable ladies t-shirt</t>
         </is>
       </c>
       <c r="B187" t="inlineStr"/>
@@ -2989,7 +2973,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>google redesign/apparel/mens</t>
+          <t>google redesign/apparel/iamremarkable unisex t-shirt</t>
         </is>
       </c>
       <c r="B188" t="inlineStr"/>
@@ -2997,7 +2981,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>google redesign/apparel/socks</t>
+          <t>google redesign/apparel/kids</t>
         </is>
       </c>
       <c r="B189" t="inlineStr"/>
@@ -3005,7 +2989,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>google redesign/apparel/stan and friends tee green</t>
+          <t>google redesign/apparel/mens</t>
         </is>
       </c>
       <c r="B190" t="inlineStr"/>
@@ -3013,7 +2997,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>google redesign/apparel/womens</t>
+          <t>google redesign/apparel/socks</t>
         </is>
       </c>
       <c r="B191" t="inlineStr"/>
@@ -3021,7 +3005,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube crew socks</t>
+          <t>google redesign/apparel/stan and friends onesie green</t>
         </is>
       </c>
       <c r="B192" t="inlineStr"/>
@@ -3029,7 +3013,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube favorite tee white</t>
+          <t>google redesign/apparel/stan and friends tee green</t>
         </is>
       </c>
       <c r="B193" t="inlineStr"/>
@@ -3037,7 +3021,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon hoodie black</t>
+          <t>google redesign/apparel/stan and friends youth tee green</t>
         </is>
       </c>
       <c r="B194" t="inlineStr"/>
@@ -3045,7 +3029,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee charcoal</t>
+          <t>google redesign/apparel/womens</t>
         </is>
       </c>
       <c r="B195" t="inlineStr"/>
@@ -3053,7 +3037,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube icon tee grey</t>
+          <t>google redesign/apparel/youtube crew socks</t>
         </is>
       </c>
       <c r="B196" t="inlineStr"/>
@@ -3061,7 +3045,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube leather strap hat black</t>
+          <t>google redesign/apparel/youtube favorite tee white</t>
         </is>
       </c>
       <c r="B197" t="inlineStr"/>
@@ -3069,7 +3053,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube standards zip hoodie black</t>
+          <t>google redesign/apparel/youtube icon hoodie black</t>
         </is>
       </c>
       <c r="B198" t="inlineStr"/>
@@ -3077,7 +3061,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube transmission journal red</t>
+          <t>google redesign/apparel/youtube icon tee charcoal</t>
         </is>
       </c>
       <c r="B199" t="inlineStr"/>
@@ -3085,7 +3069,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>google redesign/apparel/youtube twill cap sandwich black</t>
+          <t>google redesign/apparel/youtube icon tee grey</t>
         </is>
       </c>
       <c r="B200" t="inlineStr"/>
@@ -3093,7 +3077,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>google redesign/apparelgoogle beekeepers tee mint</t>
+          <t>google redesign/apparel/youtube leather strap hat black</t>
         </is>
       </c>
       <c r="B201" t="inlineStr"/>
@@ -3101,7 +3085,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>google redesign/bags/android iconic backpack</t>
+          <t>google redesign/apparel/youtube standards zip hoodie black</t>
         </is>
       </c>
       <c r="B202" t="inlineStr"/>
@@ -3109,7 +3093,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>google redesign/bags/backpacks</t>
+          <t>google redesign/apparel/youtube transmission journal red</t>
         </is>
       </c>
       <c r="B203" t="inlineStr"/>
@@ -3117,7 +3101,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>google redesign/bags/essential canvas tote</t>
+          <t>google redesign/apparel/youtube twill cap sandwich black</t>
         </is>
       </c>
       <c r="B204" t="inlineStr"/>
@@ -3125,7 +3109,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>google redesign/bags/google bike mini backpack</t>
+          <t>google redesign/apparelgoogle beekeepers tee mint</t>
         </is>
       </c>
       <c r="B205" t="inlineStr"/>
@@ -3133,7 +3117,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>google redesign/bags/google flat front bag grey</t>
+          <t>google redesign/bags/android iconic backpack</t>
         </is>
       </c>
       <c r="B206" t="inlineStr"/>
@@ -3141,7 +3125,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google campus bike carry pouch</t>
+          <t>google redesign/bags/backpacks</t>
         </is>
       </c>
       <c r="B207" t="inlineStr"/>
@@ -3149,7 +3133,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google campus bike tote navy</t>
+          <t>google redesign/bags/essential canvas tote</t>
         </is>
       </c>
       <c r="B208" t="inlineStr"/>
@@ -3157,7 +3141,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google confetti accessory pouch</t>
+          <t>google redesign/bags/google bike mini backpack</t>
         </is>
       </c>
       <c r="B209" t="inlineStr"/>
@@ -3165,7 +3149,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>google redesign/bags/google google striped penny pouch</t>
+          <t>google redesign/bags/google flat front bag grey</t>
         </is>
       </c>
       <c r="B210" t="inlineStr"/>
@@ -3173,7 +3157,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>google redesign/bags/google hemp tote</t>
+          <t>google redesign/bags/google google campus bike carry pouch</t>
         </is>
       </c>
       <c r="B211" t="inlineStr"/>
@@ -3181,7 +3165,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito dopp kit v2</t>
+          <t>google redesign/bags/google google campus bike tote navy</t>
         </is>
       </c>
       <c r="B212" t="inlineStr"/>
@@ -3189,7 +3173,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito flap pack</t>
+          <t>google redesign/bags/google google confetti accessory pouch</t>
         </is>
       </c>
       <c r="B213" t="inlineStr"/>
@@ -3197,7 +3181,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito laptop organizer v2</t>
+          <t>google redesign/bags/google google striped penny pouch</t>
         </is>
       </c>
       <c r="B214" t="inlineStr"/>
@@ -3205,7 +3189,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito messenger bag</t>
+          <t>google redesign/bags/google hemp tote</t>
         </is>
       </c>
       <c r="B215" t="inlineStr"/>
@@ -3213,7 +3197,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito techpack v2</t>
+          <t>google redesign/bags/google incognito dopp kit v2</t>
         </is>
       </c>
       <c r="B216" t="inlineStr"/>
@@ -3221,7 +3205,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>google redesign/bags/google incognito zippack v2</t>
+          <t>google redesign/bags/google incognito flap pack</t>
         </is>
       </c>
       <c r="B217" t="inlineStr"/>
@@ -3229,7 +3213,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>google redesign/bags/google large tote white</t>
+          <t>google redesign/bags/google incognito laptop organizer v2</t>
         </is>
       </c>
       <c r="B218" t="inlineStr"/>
@@ -3237,7 +3221,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mesh bag blue</t>
+          <t>google redesign/bags/google incognito messenger bag</t>
         </is>
       </c>
       <c r="B219" t="inlineStr"/>
@@ -3245,7 +3229,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>google redesign/bags/google mural tote</t>
+          <t>google redesign/bags/google incognito techpack v2</t>
         </is>
       </c>
       <c r="B220" t="inlineStr"/>
@@ -3253,7 +3237,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>google redesign/bags/google packable bag black</t>
+          <t>google redesign/bags/google incognito zippack v2</t>
         </is>
       </c>
       <c r="B221" t="inlineStr"/>
@@ -3261,7 +3245,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>google redesign/bags/google seaport tote</t>
+          <t>google redesign/bags/google large tote white</t>
         </is>
       </c>
       <c r="B222" t="inlineStr"/>
@@ -3269,7 +3253,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>google redesign/bags/google sf campus tote</t>
+          <t>google redesign/bags/google large white gift bag 5pk</t>
         </is>
       </c>
       <c r="B223" t="inlineStr"/>
@@ -3277,7 +3261,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>google redesign/bags/google small white gift bag 5pk</t>
+          <t>google redesign/bags/google mesh bag blue</t>
         </is>
       </c>
       <c r="B224" t="inlineStr"/>
@@ -3285,7 +3269,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>google redesign/bags/google totepak</t>
+          <t>google redesign/bags/google mural tote</t>
         </is>
       </c>
       <c r="B225" t="inlineStr"/>
@@ -3293,7 +3277,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility backpack</t>
+          <t>google redesign/bags/google packable bag black</t>
         </is>
       </c>
       <c r="B226" t="inlineStr"/>
@@ -3301,7 +3285,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>google redesign/bags/google utility bag grey</t>
+          <t>google redesign/bags/google seaport tote</t>
         </is>
       </c>
       <c r="B227" t="inlineStr"/>
@@ -3309,7 +3293,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>google redesign/bags/more bags</t>
+          <t>google redesign/bags/google sf campus tote</t>
         </is>
       </c>
       <c r="B228" t="inlineStr"/>
@@ -3317,7 +3301,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>google redesign/bags/shopping and totes</t>
+          <t>google redesign/bags/google totepak</t>
         </is>
       </c>
       <c r="B229" t="inlineStr"/>
@@ -3325,7 +3309,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper backpack</t>
+          <t>google redesign/bags/google utility backpack</t>
         </is>
       </c>
       <c r="B230" t="inlineStr"/>
@@ -3333,7 +3317,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper lunch sack</t>
+          <t>google redesign/bags/google utility bag grey</t>
         </is>
       </c>
       <c r="B231" t="inlineStr"/>
@@ -3341,7 +3325,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>google redesign/bags/supernatural paper tote</t>
+          <t>google redesign/bags/iamremarkable tote</t>
         </is>
       </c>
       <c r="B232" t="inlineStr"/>
@@ -3349,7 +3333,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>google redesign/blm unisex pullover hoodie</t>
+          <t>google redesign/bags/more bags</t>
         </is>
       </c>
       <c r="B233" t="inlineStr"/>
@@ -3357,7 +3341,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>google redesign/campus collection</t>
+          <t>google redesign/bags/shopping and totes</t>
         </is>
       </c>
       <c r="B234" t="inlineStr"/>
@@ -3365,7 +3349,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus mug</t>
+          <t>google redesign/bags/supernatural paper backpack</t>
         </is>
       </c>
       <c r="B235" t="inlineStr"/>
@@ -3373,7 +3357,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus sticker</t>
+          <t>google redesign/bags/supernatural paper lunch sack</t>
         </is>
       </c>
       <c r="B236" t="inlineStr"/>
@@ -3381,7 +3365,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
+          <t>google redesign/bags/supernatural paper tote</t>
         </is>
       </c>
       <c r="B237" t="inlineStr"/>
@@ -3389,7 +3373,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
+          <t>google redesign/blm unisex pullover hoodie</t>
         </is>
       </c>
       <c r="B238" t="inlineStr"/>
@@ -3397,7 +3381,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
+          <t>google redesign/campus collection</t>
         </is>
       </c>
       <c r="B239" t="inlineStr"/>
@@ -3405,7 +3389,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus mug</t>
+          <t>google redesign/campus collection/google mountain view campus mug</t>
         </is>
       </c>
       <c r="B240" t="inlineStr"/>
@@ -3413,7 +3397,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
+          <t>google redesign/campus collection/google mountain view campus sticker</t>
         </is>
       </c>
       <c r="B241" t="inlineStr"/>
@@ -3421,7 +3405,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
+          <t>google redesign/campus collection/google mountain view campus unisex tee</t>
         </is>
       </c>
       <c r="B242" t="inlineStr"/>
@@ -3429,7 +3413,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
+          <t>google redesign/campus collection/google mountain view campus zip hoodie</t>
         </is>
       </c>
       <c r="B243" t="inlineStr"/>
@@ -3437,7 +3421,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>google redesign/clearance</t>
+          <t>google redesign/campus collection/google sunnyvale campus bottle</t>
         </is>
       </c>
       <c r="B244" t="inlineStr"/>
@@ -3445,7 +3429,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android buoy bottle</t>
+          <t>google redesign/campus collection/google sunnyvale campus mug</t>
         </is>
       </c>
       <c r="B245" t="inlineStr"/>
@@ -3453,7 +3437,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic glass bottle green</t>
+          <t>google redesign/campus collection/google sunnyvale campus sticker</t>
         </is>
       </c>
       <c r="B246" t="inlineStr"/>
@@ -3461,7 +3445,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/android iconic mug gray</t>
+          <t>google redesign/campus collection/google sunnyvale campus unisex tee</t>
         </is>
       </c>
       <c r="B247" t="inlineStr"/>
@@ -3469,7 +3453,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/campus corkbase mug blue</t>
+          <t>google redesign/campus collection/google sunnyvale campus zip hoodie</t>
         </is>
       </c>
       <c r="B248" t="inlineStr"/>
@@ -3477,7 +3461,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 16oz tumbler blue</t>
+          <t>google redesign/clearance</t>
         </is>
       </c>
       <c r="B249" t="inlineStr"/>
@@ -3485,7 +3469,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
+          <t>google redesign/drinkware/android buoy bottle</t>
         </is>
       </c>
       <c r="B250" t="inlineStr"/>
@@ -3493,7 +3477,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google 24oz ring bottle red</t>
+          <t>google redesign/drinkware/android iconic glass bottle green</t>
         </is>
       </c>
       <c r="B251" t="inlineStr"/>
@@ -3501,7 +3485,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google austin campus mug</t>
+          <t>google redesign/drinkware/android iconic mug gray</t>
         </is>
       </c>
       <c r="B252" t="inlineStr"/>
@@ -3509,7 +3493,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google bike bottle</t>
+          <t>google redesign/drinkware/campus corkbase mug blue</t>
         </is>
       </c>
       <c r="B253" t="inlineStr"/>
@@ -3517,7 +3501,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus bottle</t>
+          <t>google redesign/drinkware/google 16oz tumbler blue</t>
         </is>
       </c>
       <c r="B254" t="inlineStr"/>
@@ -3525,7 +3509,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cambridge campus mug</t>
+          <t>google redesign/drinkware/google 24oz ring bottle blue</t>
         </is>
       </c>
       <c r="B255" t="inlineStr"/>
@@ -3533,7 +3517,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google camp mug ivory</t>
+          <t>google redesign/drinkware/google 24oz ring bottle red</t>
         </is>
       </c>
       <c r="B256" t="inlineStr"/>
@@ -3541,7 +3525,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google canteen bottle black</t>
+          <t>google redesign/drinkware/google austin campus mug</t>
         </is>
       </c>
       <c r="B257" t="inlineStr"/>
@@ -3549,7 +3533,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google chicago campus bottle</t>
+          <t>google redesign/drinkware/google bike bottle</t>
         </is>
       </c>
       <c r="B258" t="inlineStr"/>
@@ -3557,7 +3541,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google chicago campus mug</t>
+          <t>google redesign/drinkware/google boulder campus bottle</t>
         </is>
       </c>
       <c r="B259" t="inlineStr"/>
@@ -3565,7 +3549,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cork base tumbler</t>
+          <t>google redesign/drinkware/google boulder campus mug</t>
         </is>
       </c>
       <c r="B260" t="inlineStr"/>
@@ -3573,7 +3557,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google cup cap tumbler grey</t>
+          <t>google redesign/drinkware/google cambridge campus bottle</t>
         </is>
       </c>
       <c r="B261" t="inlineStr"/>
@@ -3581,7 +3565,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google glass bottle</t>
+          <t>google redesign/drinkware/google cambridge campus mug</t>
         </is>
       </c>
       <c r="B262" t="inlineStr"/>
@@ -3589,7 +3573,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google keepcup</t>
+          <t>google redesign/drinkware/google camp mug ivory</t>
         </is>
       </c>
       <c r="B263" t="inlineStr"/>
@@ -3597,7 +3581,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google la campus mug</t>
+          <t>google redesign/drinkware/google canteen bottle black</t>
         </is>
       </c>
       <c r="B264" t="inlineStr"/>
@@ -3605,7 +3589,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural bottle</t>
+          <t>google redesign/drinkware/google chicago campus mug</t>
         </is>
       </c>
       <c r="B265" t="inlineStr"/>
@@ -3613,7 +3597,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google mural mug</t>
+          <t>google redesign/drinkware/google cork base tumbler</t>
         </is>
       </c>
       <c r="B266" t="inlineStr"/>
@@ -3621,7 +3605,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus bottle</t>
+          <t>google redesign/drinkware/google cup cap tumbler grey</t>
         </is>
       </c>
       <c r="B267" t="inlineStr"/>
@@ -3629,7 +3613,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google nyc campus mug</t>
+          <t>google redesign/drinkware/google glass bottle</t>
         </is>
       </c>
       <c r="B268" t="inlineStr"/>
@@ -3637,7 +3621,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google perk thermal cup</t>
+          <t>google redesign/drinkware/google keepcup</t>
         </is>
       </c>
       <c r="B269" t="inlineStr"/>
@@ -3645,7 +3629,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google pnw campus bottle</t>
+          <t>google redesign/drinkware/google la campus mug</t>
         </is>
       </c>
       <c r="B270" t="inlineStr"/>
@@ -3653,7 +3637,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google pnw campus mug</t>
+          <t>google redesign/drinkware/google mural bottle</t>
         </is>
       </c>
       <c r="B271" t="inlineStr"/>
@@ -3661,7 +3645,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus bottle</t>
+          <t>google redesign/drinkware/google mural mug</t>
         </is>
       </c>
       <c r="B272" t="inlineStr"/>
@@ -3669,7 +3653,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google sf campus mug</t>
+          <t>google redesign/drinkware/google nyc campus bottle</t>
         </is>
       </c>
       <c r="B273" t="inlineStr"/>
@@ -3677,7 +3661,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler blue lid</t>
+          <t>google redesign/drinkware/google nyc campus mug</t>
         </is>
       </c>
       <c r="B274" t="inlineStr"/>
@@ -3685,7 +3669,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google super g tumbler red lid</t>
+          <t>google redesign/drinkware/google perk thermal cup</t>
         </is>
       </c>
       <c r="B275" t="inlineStr"/>
@@ -3693,7 +3677,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google thermal tumbler navy</t>
+          <t>google redesign/drinkware/google pnw campus bottle</t>
         </is>
       </c>
       <c r="B276" t="inlineStr"/>
@@ -3701,7 +3685,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/google woodtop bottle black</t>
+          <t>google redesign/drinkware/google pnw campus mug</t>
         </is>
       </c>
       <c r="B277" t="inlineStr"/>
@@ -3709,7 +3693,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/iamremarkable water bottle</t>
+          <t>google redesign/drinkware/google seattle campus mug</t>
         </is>
       </c>
       <c r="B278" t="inlineStr"/>
@@ -3717,7 +3701,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/mugs tumblers</t>
+          <t>google redesign/drinkware/google sf campus bottle</t>
         </is>
       </c>
       <c r="B279" t="inlineStr"/>
@@ -3725,7 +3709,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
+          <t>google redesign/drinkware/google super g tumbler blue lid</t>
         </is>
       </c>
       <c r="B280" t="inlineStr"/>
@@ -3733,7 +3717,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
+          <t>google redesign/drinkware/google super g tumbler red lid</t>
         </is>
       </c>
       <c r="B281" t="inlineStr"/>
@@ -3741,7 +3725,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/water bottles</t>
+          <t>google redesign/drinkware/google thermal tumbler navy</t>
         </is>
       </c>
       <c r="B282" t="inlineStr"/>
@@ -3749,7 +3733,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
+          <t>google redesign/drinkware/google woodtop bottle black</t>
         </is>
       </c>
       <c r="B283" t="inlineStr"/>
@@ -3757,7 +3741,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>google redesign/drinkware/youtube play mug</t>
+          <t>google redesign/drinkware/iamremarkable water bottle</t>
         </is>
       </c>
       <c r="B284" t="inlineStr"/>
@@ -3765,7 +3749,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>google redesign/eco friendly</t>
+          <t>google redesign/drinkware/mugs tumblers</t>
         </is>
       </c>
       <c r="B285" t="inlineStr"/>
@@ -3773,7 +3757,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>google redesign/electronics</t>
+          <t>google redesign/drinkware/stainless bent straw and cleaner</t>
         </is>
       </c>
       <c r="B286" t="inlineStr"/>
@@ -3781,7 +3765,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>google redesign/electronics/accessories</t>
+          <t>google redesign/drinkware/stainless straight straw and cleaner</t>
         </is>
       </c>
       <c r="B287" t="inlineStr"/>
@@ -3789,7 +3773,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>google redesign/electronics/audio</t>
+          <t>google redesign/drinkware/water bottles</t>
         </is>
       </c>
       <c r="B288" t="inlineStr"/>
@@ -3797,7 +3781,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>google redesign/gift cards</t>
+          <t>google redesign/drinkware/youtube 25oz gear cap bottle black</t>
         </is>
       </c>
       <c r="B289" t="inlineStr"/>
@@ -3805,7 +3789,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>google redesign/google blue stojo cup</t>
+          <t>google redesign/drinkware/youtube play mug</t>
         </is>
       </c>
       <c r="B290" t="inlineStr"/>
@@ -3813,7 +3797,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>google redesign/google chrome dino light up water bottle</t>
+          <t>google redesign/eco friendly</t>
         </is>
       </c>
       <c r="B291" t="inlineStr"/>
@@ -3821,7 +3805,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>google redesign/google crew sweater navy</t>
+          <t>google redesign/electronics</t>
         </is>
       </c>
       <c r="B292" t="inlineStr"/>
@@ -3829,7 +3813,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea french terry sweatshirt</t>
+          <t>google redesign/electronics/accessories</t>
         </is>
       </c>
       <c r="B293" t="inlineStr"/>
@@ -3837,7 +3821,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug</t>
+          <t>google redesign/gift cards</t>
         </is>
       </c>
       <c r="B294" t="inlineStr"/>
@@ -3845,7 +3829,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea mug ls</t>
+          <t>google redesign/google blue stojo cup</t>
         </is>
       </c>
       <c r="B295" t="inlineStr"/>
@@ -3853,7 +3837,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>google redesign/google land and sea tech taco</t>
+          <t>google redesign/google chrome dino light up water bottle</t>
         </is>
       </c>
       <c r="B296" t="inlineStr"/>
@@ -3861,7 +3845,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle</t>
+          <t>google redesign/google crew sweater navy</t>
         </is>
       </c>
       <c r="B297" t="inlineStr"/>
@@ -3869,7 +3853,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/bags</t>
+          <t>google redesign/google land and sea french terry sweatshirt</t>
         </is>
       </c>
       <c r="B298" t="inlineStr"/>
@@ -3877,7 +3861,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/drinkware</t>
+          <t>google redesign/google land and sea mug</t>
         </is>
       </c>
       <c r="B299" t="inlineStr"/>
@@ -3885,7 +3869,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/fun</t>
+          <t>google redesign/google land and sea tech taco</t>
         </is>
       </c>
       <c r="B300" t="inlineStr"/>
@@ -3893,7 +3877,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google aluminum bottle red</t>
+          <t>google redesign/lifestyle</t>
         </is>
       </c>
       <c r="B301" t="inlineStr"/>
@@ -3901,7 +3885,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google bear baby blanket beige</t>
+          <t>google redesign/lifestyle/bags</t>
         </is>
       </c>
       <c r="B302" t="inlineStr"/>
@@ -3909,7 +3893,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google camp mug gray</t>
+          <t>google redesign/lifestyle/drinkware</t>
         </is>
       </c>
       <c r="B303" t="inlineStr"/>
@@ -3917,7 +3901,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google knit blanket</t>
+          <t>google redesign/lifestyle/fun</t>
         </is>
       </c>
       <c r="B304" t="inlineStr"/>
@@ -3925,7 +3909,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
+          <t>google redesign/lifestyle/google aluminum bottle red</t>
         </is>
       </c>
       <c r="B305" t="inlineStr"/>
@@ -3933,7 +3917,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google land and sea tote bag</t>
+          <t>google redesign/lifestyle/google bear baby blanket beige</t>
         </is>
       </c>
       <c r="B306" t="inlineStr"/>
@@ -3941,7 +3925,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/google-frisbee</t>
+          <t>google redesign/lifestyle/google camp mug gray</t>
         </is>
       </c>
       <c r="B307" t="inlineStr"/>
@@ -3949,7 +3933,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/small goods</t>
+          <t>google redesign/lifestyle/google knit blanket</t>
         </is>
       </c>
       <c r="B308" t="inlineStr"/>
@@ -3957,7 +3941,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>google redesign/lifestyle/white google shoreline bottle</t>
+          <t>google redesign/lifestyle/google land and sea nalgene water bottle ls</t>
         </is>
       </c>
       <c r="B309" t="inlineStr"/>
@@ -3965,7 +3949,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>google redesign/new</t>
+          <t>google redesign/lifestyle/google land and sea tote bag</t>
         </is>
       </c>
       <c r="B310" t="inlineStr"/>
@@ -3973,7 +3957,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>google redesign/notebooks journals/google large standard journal grey</t>
+          <t>google redesign/lifestyle/small goods</t>
         </is>
       </c>
       <c r="B311" t="inlineStr"/>
@@ -3981,7 +3965,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>google redesign/office</t>
+          <t>google redesign/lifestyle/white google shoreline bottle</t>
         </is>
       </c>
       <c r="B312" t="inlineStr"/>
@@ -3989,7 +3973,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>google redesign/office/android iconic notebook</t>
+          <t>google redesign/new</t>
         </is>
       </c>
       <c r="B313" t="inlineStr"/>
@@ -3997,7 +3981,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>google redesign/office/android large trace journal black</t>
+          <t>google redesign/notebooks journals/google large standard journal grey</t>
         </is>
       </c>
       <c r="B314" t="inlineStr"/>
@@ -4005,7 +3989,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>google redesign/office/android small trace journal bl</t>
+          <t>google redesign/office</t>
         </is>
       </c>
       <c r="B315" t="inlineStr"/>
@@ -4013,7 +3997,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>google redesign/office/google appeel journal red</t>
+          <t>google redesign/office/android iconic notebook</t>
         </is>
       </c>
       <c r="B316" t="inlineStr"/>
@@ -4021,7 +4005,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>google redesign/office/google black cork journal</t>
+          <t>google redesign/office/android iconic pen</t>
         </is>
       </c>
       <c r="B317" t="inlineStr"/>
@@ -4029,7 +4013,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>google redesign/office/google clear pen 4pack</t>
+          <t>google redesign/office/android large trace journal black</t>
         </is>
       </c>
       <c r="B318" t="inlineStr"/>
@@ -4037,7 +4021,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork journal</t>
+          <t>google redesign/office/android small trace journal bl</t>
         </is>
       </c>
       <c r="B319" t="inlineStr"/>
@@ -4045,7 +4029,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>google redesign/office/google cork pencil pouch</t>
+          <t>google redesign/office/google appeel journal red</t>
         </is>
       </c>
       <c r="B320" t="inlineStr"/>
@@ -4053,7 +4037,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>google redesign/office/google felt refillable journal</t>
+          <t>google redesign/office/google black cork journal</t>
         </is>
       </c>
       <c r="B321" t="inlineStr"/>
@@ -4061,7 +4045,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>google redesign/office/google google campus bike grid task pad</t>
+          <t>google redesign/office/google clear pen 4pack</t>
         </is>
       </c>
       <c r="B322" t="inlineStr"/>
@@ -4069,7 +4053,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>google redesign/office/google google color block notebook</t>
+          <t>google redesign/office/google cork journal</t>
         </is>
       </c>
       <c r="B323" t="inlineStr"/>
@@ -4077,7 +4061,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti pen white</t>
+          <t>google redesign/office/google cork pencil pouch</t>
         </is>
       </c>
       <c r="B324" t="inlineStr"/>
@@ -4085,7 +4069,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti slim task pad</t>
+          <t>google redesign/office/google felt refillable journal</t>
         </is>
       </c>
       <c r="B325" t="inlineStr"/>
@@ -4093,7 +4077,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>google redesign/office/google google confetti task pad</t>
+          <t>google redesign/office/google google campus bike grid task pad</t>
         </is>
       </c>
       <c r="B326" t="inlineStr"/>
@@ -4101,7 +4085,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen blue</t>
+          <t>google redesign/office/google google color block notebook</t>
         </is>
       </c>
       <c r="B327" t="inlineStr"/>
@@ -4109,7 +4093,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>google redesign/office/google light up pen green</t>
+          <t>google redesign/office/google google confetti pen white</t>
         </is>
       </c>
       <c r="B328" t="inlineStr"/>
@@ -4117,7 +4101,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural notebook</t>
+          <t>google redesign/office/google google confetti slim task pad</t>
         </is>
       </c>
       <c r="B329" t="inlineStr"/>
@@ -4125,7 +4109,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>google redesign/office/google mural sticky note pad</t>
+          <t>google redesign/office/google google confetti task pad</t>
         </is>
       </c>
       <c r="B330" t="inlineStr"/>
@@ -4133,7 +4117,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen citron</t>
+          <t>google redesign/office/google light up pen blue</t>
         </is>
       </c>
       <c r="B331" t="inlineStr"/>
@@ -4141,7 +4125,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grass green</t>
+          <t>google redesign/office/google light up pen green</t>
         </is>
       </c>
       <c r="B332" t="inlineStr"/>
@@ -4149,7 +4133,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen grey</t>
+          <t>google redesign/office/google light up pen red</t>
         </is>
       </c>
       <c r="B333" t="inlineStr"/>
@@ -4157,7 +4141,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen red</t>
+          <t>google redesign/office/google mural notebook</t>
         </is>
       </c>
       <c r="B334" t="inlineStr"/>
@@ -4165,7 +4149,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>google redesign/office/google pen white</t>
+          <t>google redesign/office/google mural sticky note pad</t>
         </is>
       </c>
       <c r="B335" t="inlineStr"/>
@@ -4173,7 +4157,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>google redesign/office/google phone stand bamboo</t>
+          <t>google redesign/office/google pen bright blue</t>
         </is>
       </c>
       <c r="B336" t="inlineStr"/>
@@ -4181,7 +4165,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled notebook set natural</t>
+          <t>google redesign/office/google pen citron</t>
         </is>
       </c>
       <c r="B337" t="inlineStr"/>
@@ -4189,7 +4173,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen black</t>
+          <t>google redesign/office/google pen grass green</t>
         </is>
       </c>
       <c r="B338" t="inlineStr"/>
@@ -4197,7 +4181,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled pen green</t>
+          <t>google redesign/office/google pen grey</t>
         </is>
       </c>
       <c r="B339" t="inlineStr"/>
@@ -4205,7 +4189,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>google redesign/office/google recycled writing set</t>
+          <t>google redesign/office/google pen neon coral</t>
         </is>
       </c>
       <c r="B340" t="inlineStr"/>
@@ -4213,7 +4197,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>google redesign/office/google small standard journal navy</t>
+          <t>google redesign/office/google pen red</t>
         </is>
       </c>
       <c r="B341" t="inlineStr"/>
@@ -4221,7 +4205,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>google redesign/office/google soft modal scarf</t>
+          <t>google redesign/office/google pen white</t>
         </is>
       </c>
       <c r="B342" t="inlineStr"/>
@@ -4229,7 +4213,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>google redesign/office/google sustainable pencil pouch</t>
+          <t>google redesign/office/google phone stand bamboo</t>
         </is>
       </c>
       <c r="B343" t="inlineStr"/>
@@ -4237,7 +4221,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable journal</t>
+          <t>google redesign/office/google recycled notebook set natural</t>
         </is>
       </c>
       <c r="B344" t="inlineStr"/>
@@ -4245,7 +4229,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>google redesign/office/iamremarkable pen</t>
+          <t>google redesign/office/google recycled pen black</t>
         </is>
       </c>
       <c r="B345" t="inlineStr"/>
@@ -4253,7 +4237,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>google redesign/office/notebooks journals</t>
+          <t>google redesign/office/google recycled pen green</t>
         </is>
       </c>
       <c r="B346" t="inlineStr"/>
@@ -4261,7 +4245,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>google redesign/office/stickers</t>
+          <t>google redesign/office/google recycled writing set</t>
         </is>
       </c>
       <c r="B347" t="inlineStr"/>
@@ -4269,7 +4253,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>google redesign/office/writing</t>
+          <t>google redesign/office/google small standard journal navy</t>
         </is>
       </c>
       <c r="B348" t="inlineStr"/>
@@ -4277,7 +4261,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand</t>
+          <t>google redesign/office/google soft modal scarf</t>
         </is>
       </c>
       <c r="B349" t="inlineStr"/>
@@ -4285,7 +4269,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/android</t>
+          <t>google redesign/office/google sustainable pencil pouch</t>
         </is>
       </c>
       <c r="B350" t="inlineStr"/>
@@ -4293,7 +4277,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google</t>
+          <t>google redesign/office/iamremarkable journal</t>
         </is>
       </c>
       <c r="B351" t="inlineStr"/>
@@ -4301,7 +4285,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/google cloud</t>
+          <t>google redesign/office/iamremarkable pen</t>
         </is>
       </c>
       <c r="B352" t="inlineStr"/>
@@ -4309,7 +4293,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/i am remarkable</t>
+          <t>google redesign/office/notebooks journals</t>
         </is>
       </c>
       <c r="B353" t="inlineStr"/>
@@ -4317,7 +4301,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>google redesign/shop by brand/youtube</t>
+          <t>google redesign/office/stickers</t>
         </is>
       </c>
       <c r="B354" t="inlineStr"/>
@@ -4325,7 +4309,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>google redesign/small goods/daddy works at google book</t>
+          <t>google redesign/office/writing</t>
         </is>
       </c>
       <c r="B355" t="inlineStr"/>
@@ -4333,7 +4317,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>google redesign/small goods/mommy works at google book</t>
+          <t>google redesign/shop by brand</t>
         </is>
       </c>
       <c r="B356" t="inlineStr"/>
@@ -4341,7 +4325,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>google redesign/stationery</t>
+          <t>google redesign/shop by brand/android</t>
         </is>
       </c>
       <c r="B357" t="inlineStr"/>
@@ -4349,7 +4333,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>google redesign/stationery/android jotter task pad</t>
+          <t>google redesign/shop by brand/google</t>
         </is>
       </c>
       <c r="B358" t="inlineStr"/>
@@ -4357,7 +4341,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google 4in decal</t>
+          <t>google redesign/shop by brand/google cloud</t>
         </is>
       </c>
       <c r="B359" t="inlineStr"/>
@@ -4365,7 +4349,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google cloud pen</t>
+          <t>google redesign/shop by brand/i am remarkable</t>
         </is>
       </c>
       <c r="B360" t="inlineStr"/>
@@ -4373,7 +4357,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google jotter task pad</t>
+          <t>google redesign/shop by brand/youtube</t>
         </is>
       </c>
       <c r="B361" t="inlineStr"/>
@@ -4381,7 +4365,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>google redesign/stationery/google land and sea journal set</t>
+          <t>google redesign/small goods/daddy works at google book</t>
         </is>
       </c>
       <c r="B362" t="inlineStr"/>
@@ -4389,7 +4373,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>google redesign/stationery/notebooks</t>
+          <t>google redesign/small goods/mommy works at google book</t>
         </is>
       </c>
       <c r="B363" t="inlineStr"/>
@@ -4397,7 +4381,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>google redesign/stationery/stickers</t>
+          <t>google redesign/stationery</t>
         </is>
       </c>
       <c r="B364" t="inlineStr"/>
@@ -4405,7 +4389,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>google redesign/stationery/writing</t>
+          <t>google redesign/stationery/android jotter task pad</t>
         </is>
       </c>
       <c r="B365" t="inlineStr"/>
@@ -4413,7 +4397,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>google redesign/stationery/youtube jotter task pad</t>
+          <t>google redesign/stationery/google 4in decal</t>
         </is>
       </c>
       <c r="B366" t="inlineStr"/>
@@ -4421,7 +4405,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>google redesign/super g unisex joggers</t>
+          <t>google redesign/stationery/google cloud pen</t>
         </is>
       </c>
       <c r="B367" t="inlineStr"/>
@@ -4429,7 +4413,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>google redesign/wearables/men s t-shirts</t>
+          <t>google redesign/stationery/google jotter task pad</t>
         </is>
       </c>
       <c r="B368" t="inlineStr"/>
@@ -4437,7 +4421,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>google rmg redesign/lifestyle/mural food container</t>
+          <t>google redesign/stationery/google land and sea journal set</t>
         </is>
       </c>
       <c r="B369" t="inlineStr"/>
@@ -4445,7 +4429,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>google yellowesign/apparel/google tee yellow</t>
+          <t>google redesign/stationery/notebooks</t>
         </is>
       </c>
       <c r="B370" t="inlineStr"/>
@@ -4453,7 +4437,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>home</t>
+          <t>google redesign/stationery/stickers</t>
         </is>
       </c>
       <c r="B371" t="inlineStr"/>
@@ -4461,7 +4445,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>payment method</t>
+          <t>google redesign/stationery/writing</t>
         </is>
       </c>
       <c r="B372" t="inlineStr"/>
@@ -4469,7 +4453,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>shopping cart</t>
+          <t>google redesign/stationery/youtube jotter task pad</t>
         </is>
       </c>
       <c r="B373" t="inlineStr"/>
@@ -4477,7 +4461,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>store search results</t>
+          <t>google redesign/super g unisex joggers</t>
         </is>
       </c>
       <c r="B374" t="inlineStr"/>
@@ -4485,7 +4469,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>store-policies/frequently-asked-questions</t>
+          <t>google redesign/wearables/men s t-shirts</t>
         </is>
       </c>
       <c r="B375" t="inlineStr"/>
@@ -4493,7 +4477,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>store-policies/privacy-policy</t>
+          <t>google rmg redesign/lifestyle/mural food container</t>
         </is>
       </c>
       <c r="B376" t="inlineStr"/>
@@ -4501,7 +4485,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>store-policies/return-policy</t>
+          <t>google yellowesign/apparel/google tee yellow</t>
         </is>
       </c>
       <c r="B377" t="inlineStr"/>
@@ -4509,7 +4493,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>store-policies/shipping-information</t>
+          <t>home</t>
         </is>
       </c>
       <c r="B378" t="inlineStr"/>
@@ -4517,7 +4501,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>store-policies/terms-of-use</t>
+          <t>payment method</t>
         </is>
       </c>
       <c r="B379" t="inlineStr"/>
@@ -4525,7 +4509,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>the google merchandise store - log in</t>
+          <t>shopping cart</t>
         </is>
       </c>
       <c r="B380" t="inlineStr"/>
@@ -4533,7 +4517,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>the google merchandise store - my account</t>
+          <t>store search results</t>
         </is>
       </c>
       <c r="B381" t="inlineStr"/>
@@ -4541,7 +4525,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>the google merchandise store - register</t>
+          <t>store-policies/frequently-asked-questions</t>
         </is>
       </c>
       <c r="B382" t="inlineStr"/>
@@ -4549,10 +4533,66 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
+          <t>store-policies/privacy-policy</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr"/>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>store-policies/return-policy</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr"/>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>store-policies/shipping-information</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr"/>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>store-policies/terms-of-use</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr"/>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>the google merchandise store - log in</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr"/>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>the google merchandise store - my account</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>the google merchandise store - register</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr"/>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
           <t>your wishlist</t>
         </is>
       </c>
-      <c r="B383" t="inlineStr"/>
+      <c r="B390" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5806,7 +5846,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5989,18 +6029,10 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Smartphone - Edge</t>
+          <t>Xiaomi - Mi 11</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Xiaomi - Mi 11</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>